<commit_message>
fix submit data to sheet db and translation
</commit_message>
<xml_diff>
--- a/translation.xlsx
+++ b/translation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dunguyenchiem/Project/ActiveAgeing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFADED91-3431-DD41-929B-97E49C04C694}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826F56CE-281C-B844-BD3C-971D9D9626D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={653CA507-9AB3-964F-B18A-38EB8AA570F0}</author>
+  </authors>
+  <commentList>
+    <comment ref="A63" authorId="0" shapeId="0" xr:uid="{653CA507-9AB3-964F-B18A-38EB8AA570F0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dịch lại nhé a</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="216">
   <si>
     <t>English</t>
   </si>
@@ -76,12 +94,6 @@
   </si>
   <si>
     <t>Liên hệ</t>
-  </si>
-  <si>
-    <t>For a prosperous, healthy and happy old age</t>
-  </si>
-  <si>
-    <t>Vì một tuổi"xế chiều" thịnh vượng, khỏe mạnh, an vui.</t>
   </si>
   <si>
     <t>raw data</t>
@@ -277,13 +289,7 @@
     <t>Annual retirement savings (%)</t>
   </si>
   <si>
-    <t>Khoản tiết kiệm về hưu hằng năm (%)</t>
-  </si>
-  <si>
     <t>Expected annual income increase (%)</t>
-  </si>
-  <si>
-    <t>Tăng trưởng thu nhập ước tính hàng năm (%)</t>
   </si>
   <si>
     <t>Years of retirement income</t>
@@ -546,13 +552,160 @@
   </si>
   <si>
     <t>% thu nhập năm cuối cùng</t>
+  </si>
+  <si>
+    <t>Nơi ở</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Tăng trưởng thu nhập ước tính hằng năm (%)</t>
+  </si>
+  <si>
+    <t>Khoản tiết kiệm về hưu hàng năm (Theo phần trăm thu nhập)</t>
+  </si>
+  <si>
+    <t>Để &lt;span&gt;chúng tôi&lt;/span&gt; tính toán kế hoạch về hưu giúp bạn.</t>
+  </si>
+  <si>
+    <t>Let's &lt;span&gt;us&lt;/span&gt; calculate retirement planing for you.</t>
+  </si>
+  <si>
+    <t>BẮT ĐẦU NGAY</t>
+  </si>
+  <si>
+    <t>START NOW</t>
+  </si>
+  <si>
+    <t>Contributing to resonating efforts to cope with the challenges that the whole society has been facing, the project conducts “a Package of solutions for the elderly to manage their finance and access to health care in preparation for old age”. We believe that improving financial and health proactiveness is not only suitable for an individual but also positively impact the community, contributing to socio-economic development towards a more sustainable future</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Góp phần cộng hưởng những nỗ lực để đối phó với các thách thức mà cả xã hội đang gặp phải, dự án tiến hành thực hiện “Gói các giải pháp hỗ trợ người cao tuổi quản lý tài chính và tiếp cận dịch vụ chăm sóc sức khỏe chuẩn bị cho tuổi già”. Chúng tôi tin rằng việc nâng cao sự chủ động trong tài chính và sức khoẻ không chỉ ích cho riêng một cá nhân mà còn tạo ra những ảnh hưởng tích cực cho cộng đồng, góp phần vào việc phát triển kinh tế-xã hội, hướng đến một tương lai bền vững hơn.
+</t>
+  </si>
+  <si>
+    <t>Our project aims to</t>
+  </si>
+  <si>
+    <t>Dự án chúng tôi hướng đến</t>
+  </si>
+  <si>
+    <t>Promote personal savings by providing easy-to-use spending and savings management tools</t>
+  </si>
+  <si>
+    <t>Thúc đẩy tiết kiệm cá nhân qua việc cung cấp các công cụ quản lý chi tiêu, quản lý tiết kiệm dễ sử dụng</t>
+  </si>
+  <si>
+    <t>Help users set up financial management plans to prepare for the post-retirement period and provide networking opportunities with financial professionals through personal consultation packages (1-1)</t>
+  </si>
+  <si>
+    <t>Giúp người dùng thiết lập kế hoạch quản lý tài chính chuẩn bị cho giai đoạn sau về hưu và cung cấp cơ hội kết nối với các chuyên gia tài chính qua các gói tư vấn cá nhân 1-1</t>
+  </si>
+  <si>
+    <t>Provide information about health care, health insurance, travel, entertainment, and other activities.</t>
+  </si>
+  <si>
+    <t>Cung cấp thông tin về dịch vụ chăm sóc sức khỏe, bảo hiểm y tế, du lịch, giải trí và các hoạt động khác.</t>
+  </si>
+  <si>
+    <t>Problem details</t>
+  </si>
+  <si>
+    <t>Chi tiết vấn đề</t>
+  </si>
+  <si>
+    <t>According to the United Nations Department on Economic and Social Issues, the rate of population aging in Southeast Asian countries is now speedy. According to a report by the National Committee on The Elderly of Vietnam in 2019, about 1 in 5 Vietnamese will be 60 years of age or older by 2035, making Vietnam one of only three ASEAN countries with an elderly rate of over 20%.</t>
+  </si>
+  <si>
+    <t>Theo Vụ Liên Hiệp Quốc về vấn đề Kinh tế và Xã hội, tốc độ già hoá dân số tại các quốc gia Đông Nam Á hiện nay rất nhanh. Theo báo cáo năm 2019 của Ủy ban Quốc gia về Người cao tuổi Việt Nam, khoảng 1/5 người Việt Nam sẽ từ 60 tuổi trở lên vào năm 2035, đưa Việt Nam trở thành một trong ba nước ASEAN duy nhất có tỷ lệ người cao tuổi trên 20%.</t>
+  </si>
+  <si>
+    <t>In that situation, the preparation for the ageing of the population is exceptionally urgent. If people do not grasp the golden period right now, in the next 15 years, Vietnam will fall into the middle-income trap, and people will be increasingly at risk of "getting old before getting rich".</t>
+  </si>
+  <si>
+    <t>Trước thực tế đó, sự chuẩn bị cho giai đoạn già hoá dân số là vô cùng cấp thiết. Nếu không nắm bắt được giai đoạn vàng lúc này, 15 năm tới, Việt Nam sẽ rơi vào bẫy thu nhập trung bình và người dân sẽ ngày càng có nguy cơ “già trước khi giàu”.</t>
+  </si>
+  <si>
+    <t>"Getting old before getting rich" - macro concept, personal impact.</t>
+  </si>
+  <si>
+    <t>“Getting old before getting rich” - khái niệm vĩ mô, tác động cá nhân.</t>
+  </si>
+  <si>
+    <t>The report "Vietnam as an Ageing Society" recently explained that up to 16% of Vietnamese aged over 60 fall into poverty. Meanwhile, only 23.5% of people over 60 are entitled to receive a monthly pension or social insurance benefit. The income of the elderly after retirement depends heavily on their family. The traditional family model of many generations living under the same roof is gradually shifting to the nuclear family model. At that time, the elderly had to live alone, away from their children. In addition, the health care system is limited in Vietnam, along with the increasing health care cost has negatively affected the living standard after the retirement of the elderly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Báo cáo “Vietnam as an Ageing Society” mới đây đã chỉ ra rằng có đến 16% người Việt Nam trên 60 tuổi rơi vào nhóm nghèo. Trong khi đó, chỉ có 23,5% người trên 60 tuổi được hưởng lương hưu hoặc trợ cấp bảo hiểm xã hội hàng tháng. Thu nhập của người cao tuổi sau về hưu phụ thuộc lớn vào trợ cấp từ con cái. Mô hình gia đình truyền thống nhiều thế hệ cùng chung sống dưới một mái nhà đang chuyển dần sang mô hình gia đình hạt nhân. Khi đó, người cao tuổi phải sống xa con cái và có khả năng sống một mình. Ngoài ra, hệ thống chăm sóc sức khỏe còn hạn chế ở Việt Nam, cùng với chi phí khám chữa bệnh ngày càng tăng đã ảnh hưởng tiêu cực đến sự hưởng thụ sau khi về hưu của người cao tuổi. 
+</t>
+  </si>
+  <si>
+    <t>People aged over 60 by 2035</t>
+  </si>
+  <si>
+    <t>Người trên 60 tuổi vào năm 2035</t>
+  </si>
+  <si>
+    <t>People aged over 60 as the poor</t>
+  </si>
+  <si>
+    <t>Người trên 60 tuổi vào nhóm nghèo</t>
+  </si>
+  <si>
+    <t>People aged over 60 with pensions</t>
+  </si>
+  <si>
+    <t>Người trên 60 tuổi có lương hưu</t>
+  </si>
+  <si>
+    <t>Without a positive attitude of preparing for the over-60s, the elderly will face serious consequences such as financial restrictions and limited access to health care services.</t>
+  </si>
+  <si>
+    <t>Nếu không có thái độ tích cực chuẩn bị cho độ tuổi trên 60, người cao tuổi sẽ phải đối mặt với những hậu quả nghiêm trọng như hạn chế tài chính và hạn chế tiếp cận các dịch vụ chăm sóc sức khỏe.</t>
+  </si>
+  <si>
+    <t>"These problems will be exacerbated when the number of elderly people will increase in the next 15 years"</t>
+  </si>
+  <si>
+    <t>"Những vấn đề trên sẽ trở nên càng trầm trọng hơn khi 15 năm tới đây, số người cao tuổi sẽ tăng"</t>
+  </si>
+  <si>
+    <t>Seeing these problems will be exacerbated when in the next 15 years, the number of older people will increase and account for more than a fifth of the population. Active Ageing Vietnam wishes to resonate with existing changes to help each person be better prepared for old age sooner. Along with the Government's policy changes, Active Ageing is an optimal solution in doing so.</t>
+  </si>
+  <si>
+    <t>Nhìn thấy những vấn đề trên sẽ trở nên càng trầm trọng hơn khi 15 năm tới đây, số người cao tuổi sẽ tăng và chiếm hơn ⅕ dân số, Active Ageing Vietnam mong muốn có thể cộng hưởng đến những thay đổi hiện có để giúp mỗi người có sự chuẩn bị cho tuổi già tốt hơn, sớm hơn. Cùng với những thay đổi chính sách của Chính phủ, Active Ageing là một giải pháp tối ưu trong việc.</t>
+  </si>
+  <si>
+    <t>"Promoting positive thinking towards financial safety preparation and access to healthcare is essential"</t>
+  </si>
+  <si>
+    <t>"Thúc đẩy tư duy tích cực hướng tới chuẩn bị an toàn tài chính và tiếp cận chăm sóc sức khỏe là vô cùng cần thiết"</t>
+  </si>
+  <si>
+    <t>Prepare for Vietnam as a country that will be an aging nation by 2035.</t>
+  </si>
+  <si>
+    <t>chuẩn bị cho một Việt Nam sẽ là một quốc gia có già hóa dân số vào năm 2035.</t>
+  </si>
+  <si>
+    <t>In the early stages, our target audience is middle-income workers at least 15 years before retirement.</t>
+  </si>
+  <si>
+    <t>Trong giai đoạn đầu, đối tượng mục tiêu của chúng tôi là những người lao động có thu nhập trung bình ít nhất 15 năm trước khi nghỉ hưu.</t>
+  </si>
+  <si>
+    <t>Vì một tuổi &lt;span&gt;"xế chiều"&lt;/span&gt; thịnh vượng, khỏe mạnh, an vui.</t>
+  </si>
+  <si>
+    <t>For a &lt;span&gt;"aprosperous"&lt;/span&gt;, healthy and happy old age</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -619,6 +772,29 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -679,7 +855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -733,6 +909,13 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,6 +931,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Нгуен Чием Зы -" id="{B3183222-7D21-154A-933C-CC3B5F2A23AF}" userId="S::m1911836@edu.misis.ru::510efaf2-522d-45db-b2dd-e8a553adf0cb" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -946,13 +1135,21 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A63" dT="2021-06-19T05:32:53.39" personId="{B3183222-7D21-154A-933C-CC3B5F2A23AF}" id="{653CA507-9AB3-964F-B18A-38EB8AA570F0}">
+    <text>Dịch lại nhé a</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C981"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C984"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B83" sqref="B83"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -996,7 +1193,7 @@
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="5"/>
@@ -1036,151 +1233,151 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:3" ht="32">
+      <c r="A9" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16">
       <c r="A10" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="34">
       <c r="A11" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="32">
       <c r="A12" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16">
       <c r="A13" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="64">
       <c r="A14" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="112">
       <c r="A15" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16">
       <c r="A16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16">
       <c r="A17" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16">
       <c r="A18" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16">
       <c r="A19" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16">
       <c r="A20" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16">
       <c r="A21" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16">
       <c r="A22" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16">
       <c r="A23" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16">
       <c r="A24" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="119">
       <c r="A25" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="16">
       <c r="A26" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>16</v>
@@ -1188,562 +1385,670 @@
     </row>
     <row r="27" spans="1:2" ht="16">
       <c r="A27" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="16">
       <c r="A28" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="16">
       <c r="A29" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="16">
       <c r="A30" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="16">
       <c r="A31" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="16">
       <c r="A32" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="16">
       <c r="A33" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="96">
       <c r="A34" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="192">
       <c r="A35" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="160">
+      <c r="A36" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="16">
+      <c r="A37" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="16">
+      <c r="A38" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38" s="30" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="16">
+      <c r="A39" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="16">
+      <c r="A40" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="16">
+      <c r="A41" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="16">
+      <c r="A42" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="B42" s="30" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="16">
+      <c r="A43" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="B43" s="30" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="16">
+      <c r="A44" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="B44" s="30" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="192">
+      <c r="A45" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="16">
+      <c r="A46" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="16">
+      <c r="A47" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="16">
+      <c r="A48" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="16">
+      <c r="A49" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="16">
+      <c r="A50" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="16">
+      <c r="A51" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="B51" s="30" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="16">
+      <c r="A52" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="B52" s="30" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="16">
+      <c r="A53" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="B53" s="30" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="16">
+      <c r="A54" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="B54" s="30" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="17">
+      <c r="A55" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="17">
+      <c r="A56" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="16">
+      <c r="A57" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B57" s="26" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="16">
-      <c r="A36" s="12" t="s">
+    <row r="58" spans="1:2" ht="16">
+      <c r="A58" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="B58" s="26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B59" s="14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="14" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B60" s="14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="14" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B61" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="14" t="s">
+    <row r="62" spans="1:2">
+      <c r="A62" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B62" s="14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="14" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B63" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="14" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="14" t="s">
+      <c r="B64" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B65" s="14" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="14" t="s">
+    <row r="66" spans="1:2">
+      <c r="A66" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B66" s="14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="14" t="s">
+    <row r="67" spans="1:2">
+      <c r="A67" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B67" s="14" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="14" t="s">
+    <row r="68" spans="1:2">
+      <c r="A68" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B68" s="14" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="14" t="s">
+    <row r="69" spans="1:2">
+      <c r="A69" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B69" s="14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="14" t="s">
+    <row r="70" spans="1:2">
+      <c r="A70" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B70" s="14" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="14" t="s">
+    <row r="71" spans="1:2" ht="14">
+      <c r="A71" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B71" s="15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="14" t="s">
+    <row r="72" spans="1:2">
+      <c r="A72" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B72" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="14">
-      <c r="A49" s="15" t="s">
+    <row r="73" spans="1:2" ht="16">
+      <c r="A73" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B73" s="18" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="16" t="s">
+    <row r="74" spans="1:2" ht="96">
+      <c r="A74" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B74" s="18" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="16">
-      <c r="A51" s="17" t="s">
+    <row r="75" spans="1:2" ht="16">
+      <c r="A75" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="18" t="s">
+      <c r="B75" s="18" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="96">
-      <c r="A52" s="17" t="s">
+    <row r="76" spans="1:2" ht="80">
+      <c r="A76" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="18" t="s">
+      <c r="B76" s="18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="16">
-      <c r="A53" s="17" t="s">
+    <row r="77" spans="1:2" ht="32">
+      <c r="A77" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B53" s="18" t="s">
+      <c r="B77" s="18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="80">
-      <c r="A54" s="17" t="s">
+    <row r="78" spans="1:2" ht="30">
+      <c r="A78" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="18" t="s">
+      <c r="B78" s="19" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="32">
-      <c r="A55" s="17" t="s">
+    <row r="79" spans="1:2" ht="90">
+      <c r="A79" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="B55" s="18" t="s">
+      <c r="B79" s="19" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="30">
-      <c r="A56" s="17" t="s">
+    <row r="80" spans="1:2" ht="32">
+      <c r="A80" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="B56" s="19" t="s">
+      <c r="B80" s="18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="90">
-      <c r="A57" s="17" t="s">
+    <row r="81" spans="1:2" ht="32">
+      <c r="A81" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B57" s="19" t="s">
+      <c r="B81" s="18" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="32">
-      <c r="A58" s="17" t="s">
+    <row r="82" spans="1:2" ht="16">
+      <c r="A82" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="B58" s="18" t="s">
+      <c r="B82" s="18" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="32">
-      <c r="A59" s="17" t="s">
+    <row r="83" spans="1:2" ht="32">
+      <c r="A83" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="B59" s="18" t="s">
+      <c r="B83" s="18" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="16">
-      <c r="A60" s="17" t="s">
+    <row r="84" spans="1:2" ht="16">
+      <c r="A84" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="B60" s="18" t="s">
+      <c r="B84" s="18" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="32">
-      <c r="A61" s="17" t="s">
+    <row r="85" spans="1:2" ht="16">
+      <c r="A85" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B61" s="18" t="s">
+      <c r="B85" s="18" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="16">
-      <c r="A62" s="17" t="s">
+    <row r="86" spans="1:2" ht="32">
+      <c r="A86" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="B62" s="18" t="s">
+      <c r="B86" s="18" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="16">
-      <c r="A63" s="17" t="s">
+    <row r="87" spans="1:2" ht="16">
+      <c r="A87" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="B63" s="18" t="s">
+      <c r="B87" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A88" s="17" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" ht="32">
-      <c r="A64" s="17" t="s">
+      <c r="B88" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="B64" s="18" t="s">
+    </row>
+    <row r="89" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A89" s="17" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" ht="16">
-      <c r="A65" s="17" t="s">
+      <c r="B89" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="B65" s="18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="48">
-      <c r="A66" s="17" t="s">
+    </row>
+    <row r="90" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A90" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B66" s="18" t="s">
+      <c r="B90" s="18" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="16">
-      <c r="A67" s="17" t="s">
+    <row r="91" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A91" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B67" s="18" t="s">
+      <c r="B91" s="20" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="48">
-      <c r="A68" s="17" t="s">
+    <row r="92" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A92" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="B68" s="18" t="s">
+      <c r="B92" s="20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A93" s="21" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" ht="16">
-      <c r="A69" s="17" t="s">
+      <c r="B93" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="B69" s="20" t="s">
+    </row>
+    <row r="94" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A94" s="21" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="21" t="s">
+      <c r="B94" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="B70" s="20" t="s">
+    </row>
+    <row r="95" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A95" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B95" s="22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A96" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B96" s="22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A97" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="B97" s="22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A98" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B98" s="19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A99" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="B99" s="19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A100" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B100" s="26" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A101" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B101" s="26" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A102" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B102" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A103" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B103" s="26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A104" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="B104" s="13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A105" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="B105" s="13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A106" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="B106" s="13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A107" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B107" s="26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A108" s="11" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" ht="14">
-      <c r="A71" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="B71" s="22" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="14">
-      <c r="A72" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="B72" s="22" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="14">
-      <c r="A73" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="B73" s="22" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="14">
-      <c r="A74" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="B74" s="22" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="14">
-      <c r="A75" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="B75" s="22" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="17">
-      <c r="A76" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="B76" s="19" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="17">
-      <c r="A77" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="B77" s="19" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="16">
-      <c r="A78" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="B78" s="26" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="16">
-      <c r="A79" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="B79" s="26" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="16">
-      <c r="A80" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B80" s="26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="16">
-      <c r="A81" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B81" s="26" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="16">
-      <c r="A82" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="B82" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="16">
-      <c r="A83" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="B83" s="13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="16">
-      <c r="A84" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="B84" s="13" t="s">
+      <c r="B108" s="26" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A85" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="B85" s="26" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A86" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="B86" s="26" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A87" s="11"/>
-      <c r="B87" s="26"/>
-    </row>
-    <row r="88" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A88" s="11"/>
-      <c r="B88" s="26"/>
-    </row>
-    <row r="89" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A89" s="11"/>
-    </row>
-    <row r="90" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A90" s="11"/>
-    </row>
-    <row r="91" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A91" s="11"/>
-    </row>
-    <row r="92" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A92" s="11"/>
-    </row>
-    <row r="93" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A93" s="11"/>
-    </row>
-    <row r="94" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A94" s="11"/>
-    </row>
-    <row r="95" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A95" s="11"/>
-    </row>
-    <row r="96" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A96" s="11"/>
-    </row>
-    <row r="97" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A97" s="11"/>
-    </row>
-    <row r="98" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A98" s="11"/>
-    </row>
-    <row r="99" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A99" s="11"/>
-    </row>
-    <row r="100" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A100" s="11"/>
-    </row>
-    <row r="101" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A101" s="11"/>
-    </row>
-    <row r="102" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A102" s="11"/>
-    </row>
-    <row r="103" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A103" s="11"/>
-    </row>
-    <row r="104" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A104" s="11"/>
-    </row>
-    <row r="105" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A105" s="11"/>
-    </row>
-    <row r="106" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A106" s="11"/>
-    </row>
-    <row r="107" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A107" s="11"/>
-    </row>
-    <row r="108" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A108" s="11"/>
-    </row>
-    <row r="109" spans="1:1" ht="15.75" customHeight="1">
+    <row r="109" spans="1:2" ht="15.75" customHeight="1">
       <c r="A109" s="11"/>
     </row>
-    <row r="110" spans="1:1" ht="15.75" customHeight="1">
+    <row r="110" spans="1:2" ht="15.75" customHeight="1">
       <c r="A110" s="11"/>
     </row>
-    <row r="111" spans="1:1" ht="15.75" customHeight="1">
+    <row r="111" spans="1:2" ht="15.75" customHeight="1">
       <c r="A111" s="11"/>
     </row>
-    <row r="112" spans="1:1" ht="15.75" customHeight="1">
+    <row r="112" spans="1:2" ht="15.75" customHeight="1">
       <c r="A112" s="11"/>
     </row>
     <row r="113" spans="1:1" ht="15.75" customHeight="1">
@@ -4352,9 +4657,19 @@
     </row>
     <row r="981" spans="1:1" ht="15.75" customHeight="1">
       <c r="A981" s="11"/>
+    </row>
+    <row r="982" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A982" s="11"/>
+    </row>
+    <row r="983" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A983" s="11"/>
+    </row>
+    <row r="984" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A984" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add submit to server for sign up function
</commit_message>
<xml_diff>
--- a/translation.xlsx
+++ b/translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dunguyenchiem/Project/ActiveAgeing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E2BE02-2797-DF48-AB72-D55B84441D8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384B61F7-9C36-374E-B9DD-AABD728CF0E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,9 +511,6 @@
     <t>Để &lt;span&gt;chúng tôi&lt;/span&gt; tính toán kế hoạch về hưu giúp bạn.</t>
   </si>
   <si>
-    <t>Let's &lt;span&gt;us&lt;/span&gt; calculate retirement planing for you.</t>
-  </si>
-  <si>
     <t>BẮT ĐẦU NGAY</t>
   </si>
   <si>
@@ -696,13 +693,16 @@
   </si>
   <si>
     <t>Your retirement savings plan is on track. Use the Manage Savings function to easily track and manage your progress!</t>
+  </si>
+  <si>
+    <t>Let &lt;span&gt;us &lt;/span&gt; help you to make a retirement plan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -794,6 +794,11 @@
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="&quot;Open Sans&quot;"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -860,7 +865,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -917,6 +922,10 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1149,8 +1158,8 @@
   <dimension ref="A1:Z985"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A95" sqref="A95"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -1192,7 +1201,7 @@
     </row>
     <row r="4" spans="1:3" ht="16">
       <c r="A4" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>7</v>
@@ -1201,7 +1210,7 @@
     </row>
     <row r="5" spans="1:3" ht="16">
       <c r="A5" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
@@ -1236,10 +1245,10 @@
     </row>
     <row r="9" spans="1:3" ht="32">
       <c r="A9" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>15</v>
@@ -1255,7 +1264,7 @@
     </row>
     <row r="11" spans="1:3" ht="32">
       <c r="A11" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>18</v>
@@ -1279,7 +1288,7 @@
     </row>
     <row r="14" spans="1:3" ht="64">
       <c r="A14" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>23</v>
@@ -1287,7 +1296,7 @@
     </row>
     <row r="15" spans="1:3" ht="112">
       <c r="A15" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>24</v>
@@ -1295,7 +1304,7 @@
     </row>
     <row r="16" spans="1:3" ht="16">
       <c r="A16" s="25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>25</v>
@@ -1354,7 +1363,7 @@
     </row>
     <row r="23" spans="1:2" ht="16">
       <c r="A23" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>39</v>
@@ -1362,7 +1371,7 @@
     </row>
     <row r="24" spans="1:2" ht="16">
       <c r="A24" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>40</v>
@@ -1370,7 +1379,7 @@
     </row>
     <row r="25" spans="1:2" ht="112">
       <c r="A25" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>41</v>
@@ -1386,7 +1395,7 @@
     </row>
     <row r="27" spans="1:2" ht="16">
       <c r="A27" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>42</v>
@@ -1442,71 +1451,71 @@
     </row>
     <row r="34" spans="1:26" ht="64">
       <c r="A34" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:26" ht="160">
       <c r="A35" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="128">
       <c r="A36" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="16">
       <c r="A37" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="B37" s="28" t="s">
         <v>159</v>
-      </c>
-      <c r="B37" s="28" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:26" ht="16">
       <c r="A38" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="B38" s="28" t="s">
         <v>161</v>
-      </c>
-      <c r="B38" s="28" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="16">
       <c r="A39" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="B39" s="28" t="s">
         <v>163</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="16">
       <c r="A40" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="B40" s="28" t="s">
         <v>165</v>
-      </c>
-      <c r="B40" s="28" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:26" ht="16">
       <c r="A41" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="B41" s="28" t="s">
         <v>167</v>
-      </c>
-      <c r="B41" s="28" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="16">
       <c r="A42" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B42" s="24" t="s">
         <v>7</v>
@@ -1538,111 +1547,111 @@
     </row>
     <row r="43" spans="1:26" ht="16">
       <c r="A43" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="B43" s="28" t="s">
         <v>169</v>
-      </c>
-      <c r="B43" s="28" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:26" ht="16">
       <c r="A44" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" s="28" t="s">
         <v>171</v>
-      </c>
-      <c r="B44" s="28" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:26" ht="16">
       <c r="A45" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="B45" s="28" t="s">
         <v>173</v>
-      </c>
-      <c r="B45" s="28" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="46" spans="1:26" ht="192">
       <c r="A46" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="B46" s="26" t="s">
         <v>175</v>
-      </c>
-      <c r="B46" s="26" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:26" ht="16">
       <c r="A47" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B47" s="28" t="s">
         <v>177</v>
-      </c>
-      <c r="B47" s="28" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="48" spans="1:26" ht="16">
       <c r="A48" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B48" s="28" t="s">
         <v>179</v>
-      </c>
-      <c r="B48" s="28" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="16">
       <c r="A49" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="B49" s="28" t="s">
         <v>181</v>
-      </c>
-      <c r="B49" s="28" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="16">
       <c r="A50" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="B50" s="28" t="s">
         <v>183</v>
-      </c>
-      <c r="B50" s="28" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="16">
       <c r="A51" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="B51" s="28" t="s">
         <v>185</v>
-      </c>
-      <c r="B51" s="28" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="16">
       <c r="A52" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="B52" s="28" t="s">
         <v>187</v>
-      </c>
-      <c r="B52" s="28" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="16">
       <c r="A53" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="B53" s="28" t="s">
         <v>189</v>
-      </c>
-      <c r="B53" s="28" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="16">
       <c r="A54" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="B54" s="28" t="s">
         <v>191</v>
-      </c>
-      <c r="B54" s="28" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="16">
       <c r="A55" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="B55" s="28" t="s">
         <v>193</v>
-      </c>
-      <c r="B55" s="28" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="17">
       <c r="A56" s="8" t="s">
-        <v>155</v>
+        <v>216</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>154</v>
@@ -1650,10 +1659,10 @@
     </row>
     <row r="57" spans="1:2" ht="17">
       <c r="A57" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="16">
@@ -1705,7 +1714,7 @@
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="12" t="s">
+      <c r="A64" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B64" s="12" t="s">
@@ -1914,10 +1923,10 @@
     </row>
     <row r="90" spans="1:2" ht="15.75" customHeight="1">
       <c r="A90" s="29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15.75" customHeight="1">
@@ -1986,7 +1995,7 @@
     </row>
     <row r="99" spans="1:2" ht="15.75" customHeight="1">
       <c r="A99" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B99" s="17" t="s">
         <v>129</v>
@@ -2026,7 +2035,7 @@
     </row>
     <row r="104" spans="1:2" ht="15.75" customHeight="1">
       <c r="A104" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B104" s="24" t="s">
         <v>149</v>
@@ -2073,11 +2082,11 @@
       </c>
     </row>
     <row r="110" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A110" s="9" t="s">
-        <v>197</v>
+      <c r="A110" s="31" t="s">
+        <v>196</v>
       </c>
       <c r="B110" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
fix retirement plan formula
</commit_message>
<xml_diff>
--- a/translation.xlsx
+++ b/translation.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mirZOfLVqb5pL9yRehA+mMekFEs8A=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mieT1fQgQV0KJd06R3oRBw/7UF+Fw=="/>
     </ext>
   </extLst>
 </workbook>
@@ -21,16 +21,15 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A68">
+    <comment authorId="0" ref="B69">
       <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Dịch lại nhé a
-======</t>
+        <t xml:space="preserve">======
+ID#AAAAM3c6OYc
+Dự Nguyễn Chiếm    (2021-06-20 13:01:38)
+chỗ này vừa sửa content lại ạ, cần bổ sung bản dịchmới</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A79">
+    <comment authorId="0" ref="A80">
       <text>
         <t xml:space="preserve">======
 ID#AAAAMi8LqaU
@@ -41,14 +40,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mi4u9hw6WEVv4cdYzwqhmP3CG8YMw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhYiDt+YYOvQXjhafipvSmTV67sqw=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="274">
   <si>
     <t>English</t>
   </si>
@@ -471,6 +470,9 @@
     <t>Số dư khoản tiết kiệm về hưu hiện tại</t>
   </si>
   <si>
+    <t>Tỷ lệ chi tiêu khi về hưu so với thu nhập năm cuối trước khi nghỉ hưu. (%)</t>
+  </si>
+  <si>
     <t>Annual retirement savings (As a percentage of income)</t>
   </si>
   <si>
@@ -912,6 +914,12 @@
   </si>
   <si>
     <t>Xây dựng kế hoạch về hưu hợp lý cùng Active Ageing ngay hôm nay!</t>
+  </si>
+  <si>
+    <t>Million</t>
+  </si>
+  <si>
+    <t>Triệu</t>
   </si>
 </sst>
 </file>
@@ -947,11 +955,11 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
     </font>
+    <font/>
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -1007,14 +1015,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF00FF"/>
-        <bgColor rgb="FFFF00FF"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor rgb="FFFF00FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -1042,7 +1050,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1086,25 +1094,34 @@
     <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -1125,25 +1142,25 @@
     <xf borderId="0" fillId="10" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="10" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="10" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="10" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2014,1154 +2031,1163 @@
       <c r="C67" s="7"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="14" t="s">
+      <c r="A68" s="14"/>
+      <c r="B68" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B68" s="13" t="s">
+      <c r="C68" s="7"/>
+    </row>
+    <row r="69" ht="15.75" customHeight="1">
+      <c r="A69" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="C68" s="7"/>
-    </row>
-    <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="15" t="s">
+      <c r="B69" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B69" s="13" t="s">
+      <c r="C69" s="7"/>
+    </row>
+    <row r="70" ht="15.75" customHeight="1">
+      <c r="A70" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="C69" s="7"/>
-    </row>
-    <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="15" t="s">
+      <c r="B70" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B70" s="13" t="s">
+      <c r="C70" s="7"/>
+    </row>
+    <row r="71" ht="15.75" customHeight="1">
+      <c r="A71" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C70" s="7"/>
-    </row>
-    <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="5" t="s">
+      <c r="B71" s="13" t="s">
         <v>138</v>
-      </c>
-      <c r="B71" s="13" t="s">
-        <v>139</v>
       </c>
       <c r="C71" s="7"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B72" s="13" t="s">
         <v>140</v>
-      </c>
-      <c r="B72" s="13" t="s">
-        <v>141</v>
       </c>
       <c r="C72" s="7"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B73" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="B73" s="13" t="s">
-        <v>143</v>
       </c>
       <c r="C73" s="7"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B74" s="13" t="s">
         <v>144</v>
-      </c>
-      <c r="B74" s="13" t="s">
-        <v>145</v>
       </c>
       <c r="C74" s="7"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B75" s="13" t="s">
         <v>146</v>
-      </c>
-      <c r="B75" s="13" t="s">
-        <v>147</v>
       </c>
       <c r="C75" s="7"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B76" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="C76" s="7"/>
+    </row>
+    <row r="77" ht="15.75" customHeight="1">
+      <c r="A77" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C76" s="7"/>
-    </row>
-    <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="16" t="s">
+      <c r="B77" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B77" s="16" t="s">
+      <c r="C77" s="7"/>
+    </row>
+    <row r="78" ht="15.75" customHeight="1">
+      <c r="A78" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="C77" s="17" t="s">
+      <c r="B78" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="D77" s="18" t="s">
+      <c r="C78" s="20" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="11" t="s">
+      <c r="D78" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="B78" s="5" t="s">
+    </row>
+    <row r="79" ht="15.75" customHeight="1">
+      <c r="A79" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C78" s="7"/>
-    </row>
-    <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="19" t="s">
+      <c r="B79" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="C79" s="7"/>
+    </row>
+    <row r="80" ht="15.75" customHeight="1">
+      <c r="A80" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="C79" s="7"/>
-    </row>
-    <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="11" t="s">
+      <c r="B80" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>159</v>
       </c>
       <c r="C80" s="7"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="C81" s="7"/>
+    </row>
+    <row r="82" ht="15.75" customHeight="1">
+      <c r="A82" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="C81" s="7"/>
-    </row>
-    <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="12" t="s">
+      <c r="B82" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="C82" s="7"/>
+    </row>
+    <row r="83" ht="15.75" customHeight="1">
+      <c r="A83" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="C82" s="7"/>
-    </row>
-    <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="11" t="s">
+      <c r="B83" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="C83" s="7"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B84" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>167</v>
       </c>
       <c r="C84" s="7"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B85" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="C85" s="7"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="B86" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>171</v>
       </c>
       <c r="C86" s="7"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B87" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>173</v>
       </c>
       <c r="C87" s="7"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="C88" s="7"/>
+    </row>
+    <row r="89" ht="15.75" customHeight="1">
+      <c r="A89" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="C88" s="7"/>
-    </row>
-    <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="20" t="s">
+      <c r="B89" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="C89" s="7"/>
+    </row>
+    <row r="90" ht="15.75" customHeight="1">
+      <c r="A90" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="C89" s="7"/>
-    </row>
-    <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="11" t="s">
+      <c r="B90" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="C90" s="7"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B91" s="5" t="s">
         <v>180</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>181</v>
       </c>
       <c r="C91" s="7"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B92" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="C92" s="7"/>
+    </row>
+    <row r="93" ht="15.75" customHeight="1">
+      <c r="A93" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="C92" s="7"/>
-    </row>
-    <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="12" t="s">
+      <c r="B93" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="C93" s="7"/>
+    </row>
+    <row r="94" ht="15.75" customHeight="1">
+      <c r="A94" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="C93" s="7"/>
-    </row>
-    <row r="94" ht="67.5" customHeight="1">
-      <c r="A94" s="21" t="s">
+      <c r="B94" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B94" s="9" t="s">
+      <c r="C94" s="7"/>
+    </row>
+    <row r="95" ht="67.5" customHeight="1">
+      <c r="A95" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="C94" s="7"/>
-    </row>
-    <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="11" t="s">
+      <c r="B95" s="9" t="s">
         <v>188</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>189</v>
       </c>
       <c r="C95" s="7"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="B96" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>191</v>
       </c>
       <c r="C96" s="7"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B97" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="C97" s="7"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B98" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="B98" s="22" t="s">
-        <v>195</v>
       </c>
       <c r="C98" s="7"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="B99" s="25" t="s">
         <v>196</v>
-      </c>
-      <c r="B99" s="22" t="s">
-        <v>197</v>
       </c>
       <c r="C99" s="7"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B100" s="25" t="s">
         <v>198</v>
-      </c>
-      <c r="B100" s="22" t="s">
-        <v>199</v>
       </c>
       <c r="C100" s="7"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="B101" s="25" t="s">
         <v>200</v>
-      </c>
-      <c r="B101" s="22" t="s">
-        <v>201</v>
       </c>
       <c r="C101" s="7"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="B102" s="25" t="s">
         <v>202</v>
-      </c>
-      <c r="B102" s="22" t="s">
-        <v>203</v>
       </c>
       <c r="C102" s="7"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B103" s="25" t="s">
         <v>204</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>205</v>
       </c>
       <c r="C103" s="7"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B104" s="5" t="s">
         <v>206</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>207</v>
       </c>
       <c r="C104" s="7"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B105" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>209</v>
       </c>
       <c r="C105" s="7"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B106" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="B106" s="23" t="s">
-        <v>211</v>
       </c>
       <c r="C106" s="7"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B107" s="26" t="s">
         <v>212</v>
-      </c>
-      <c r="B107" s="5" t="s">
-        <v>213</v>
       </c>
       <c r="C107" s="7"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="B108" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="C108" s="7"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="B109" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>217</v>
       </c>
       <c r="C109" s="7"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B110" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="B110" s="5" t="s">
-        <v>219</v>
       </c>
       <c r="C110" s="7"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B111" s="5" t="s">
         <v>220</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>221</v>
       </c>
       <c r="C111" s="7"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B112" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>223</v>
       </c>
       <c r="C112" s="7"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
       <c r="A113" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="B113" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="B113" s="5" t="s">
+      <c r="C113" s="7"/>
+    </row>
+    <row r="114" ht="15.75" customHeight="1">
+      <c r="A114" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="C113" s="7"/>
-    </row>
-    <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="24" t="s">
+      <c r="B114" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="B114" s="5" t="s">
+      <c r="C114" s="7"/>
+    </row>
+    <row r="115" ht="15.75" customHeight="1">
+      <c r="A115" s="27" t="s">
         <v>227</v>
       </c>
-      <c r="C114" s="7"/>
-    </row>
-    <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="25" t="s">
+      <c r="B115" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B115" s="9" t="s">
+      <c r="C115" s="7"/>
+    </row>
+    <row r="116" ht="15.75" customHeight="1">
+      <c r="A116" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="B116" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C115" s="7"/>
-    </row>
-    <row r="116" ht="90.0" customHeight="1">
-      <c r="A116" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="B116" s="11" t="s">
+      <c r="C116" s="7"/>
+    </row>
+    <row r="117" ht="90.0" customHeight="1">
+      <c r="A117" s="29" t="s">
         <v>230</v>
       </c>
-      <c r="C116" s="7"/>
-    </row>
-    <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="25" t="s">
+      <c r="B117" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="B117" s="11" t="s">
+      <c r="C117" s="7"/>
+    </row>
+    <row r="118" ht="15.75" customHeight="1">
+      <c r="A118" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="C117" s="7"/>
-    </row>
-    <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="25" t="s">
+      <c r="B118" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="B118" s="11" t="s">
+      <c r="C118" s="7"/>
+    </row>
+    <row r="119" ht="15.75" customHeight="1">
+      <c r="A119" s="28" t="s">
         <v>234</v>
       </c>
-      <c r="C118" s="7"/>
-    </row>
-    <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="25" t="s">
+      <c r="B119" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="B119" s="11" t="s">
+      <c r="C119" s="7"/>
+    </row>
+    <row r="120" ht="15.75" customHeight="1">
+      <c r="A120" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="C119" s="7"/>
-    </row>
-    <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="25" t="s">
+      <c r="B120" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="B120" s="11" t="s">
+      <c r="C120" s="7"/>
+    </row>
+    <row r="121" ht="15.75" customHeight="1">
+      <c r="A121" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="C120" s="7"/>
-    </row>
-    <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="25" t="s">
+      <c r="B121" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="B121" s="11" t="s">
+      <c r="C121" s="7"/>
+    </row>
+    <row r="122" ht="15.75" customHeight="1">
+      <c r="A122" s="28" t="s">
         <v>240</v>
       </c>
-      <c r="C121" s="7"/>
-    </row>
-    <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="26" t="s">
+      <c r="B122" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="B122" s="11" t="s">
+      <c r="C122" s="7"/>
+    </row>
+    <row r="123" ht="15.75" customHeight="1">
+      <c r="A123" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="C122" s="7"/>
-    </row>
-    <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="27" t="s">
+      <c r="B123" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="B123" s="11" t="s">
+      <c r="C123" s="7"/>
+    </row>
+    <row r="124" ht="15.75" customHeight="1">
+      <c r="A124" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="C123" s="7"/>
-    </row>
-    <row r="124" ht="82.5" customHeight="1">
-      <c r="A124" s="27" t="s">
+      <c r="B124" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="B124" s="11" t="s">
+      <c r="C124" s="7"/>
+    </row>
+    <row r="125" ht="82.5" customHeight="1">
+      <c r="A125" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="C124" s="7"/>
-    </row>
-    <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="27" t="s">
+      <c r="B125" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="B125" s="11" t="s">
+      <c r="C125" s="7"/>
+    </row>
+    <row r="126" ht="15.75" customHeight="1">
+      <c r="A126" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="C125" s="7"/>
-    </row>
-    <row r="126" ht="17.25" customHeight="1">
-      <c r="A126" s="28" t="s">
+      <c r="B126" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="B126" s="29" t="s">
+      <c r="C126" s="7"/>
+    </row>
+    <row r="127" ht="17.25" customHeight="1">
+      <c r="A127" s="31" t="s">
         <v>250</v>
       </c>
-      <c r="C126" s="7"/>
-    </row>
-    <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="30" t="s">
+      <c r="B127" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="B127" s="31" t="s">
+      <c r="C127" s="7"/>
+    </row>
+    <row r="128" ht="15.75" customHeight="1">
+      <c r="A128" s="33" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="32" t="s">
+      <c r="B128" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="B128" s="31" t="s">
+    </row>
+    <row r="129" ht="15.75" customHeight="1">
+      <c r="A129" s="35" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="30" t="s">
+      <c r="B129" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="B129" s="31" t="s">
+    </row>
+    <row r="130" ht="15.75" customHeight="1">
+      <c r="A130" s="33" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="130" ht="16.5" customHeight="1">
-      <c r="A130" s="30" t="s">
+      <c r="B130" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="B130" s="31" t="s">
+    </row>
+    <row r="131" ht="16.5" customHeight="1">
+      <c r="A131" s="33" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="30" t="s">
+      <c r="B131" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="B131" s="31" t="s">
+    </row>
+    <row r="132" ht="15.75" customHeight="1">
+      <c r="A132" s="33" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="30" t="s">
+      <c r="B132" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="B132" s="33" t="s">
+    </row>
+    <row r="133" ht="15.75" customHeight="1">
+      <c r="A133" s="33" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="34" t="s">
+      <c r="B133" s="36" t="s">
         <v>263</v>
       </c>
-      <c r="B133" s="35" t="s">
+    </row>
+    <row r="134" ht="15.75" customHeight="1">
+      <c r="A134" s="37" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="34" t="s">
+      <c r="B134" s="38" t="s">
         <v>265</v>
       </c>
-      <c r="B134" s="35" t="s">
+    </row>
+    <row r="135" ht="15.75" customHeight="1">
+      <c r="A135" s="37" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="36" t="s">
+      <c r="B135" s="38" t="s">
         <v>267</v>
       </c>
-      <c r="B135" s="33" t="s">
+    </row>
+    <row r="136" ht="15.75" customHeight="1">
+      <c r="A136" s="39" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="36" t="s">
+      <c r="B136" s="36" t="s">
         <v>269</v>
       </c>
-      <c r="B136" s="35" t="s">
+    </row>
+    <row r="137" ht="15.75" customHeight="1">
+      <c r="A137" s="39" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="37"/>
+      <c r="B137" s="38" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="37"/>
+      <c r="A138" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="B138" s="38" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="37"/>
+      <c r="A139" s="40"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="37"/>
+      <c r="A140" s="40"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="37"/>
+      <c r="A141" s="40"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="37"/>
+      <c r="A142" s="40"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="37"/>
+      <c r="A143" s="40"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="A144" s="37"/>
+      <c r="A144" s="40"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="37"/>
+      <c r="A145" s="40"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="37"/>
+      <c r="A146" s="40"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="37"/>
+      <c r="A147" s="40"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="A148" s="37"/>
+      <c r="A148" s="40"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="A149" s="37"/>
+      <c r="A149" s="40"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="A150" s="37"/>
+      <c r="A150" s="40"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="A151" s="37"/>
+      <c r="A151" s="40"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="A152" s="37"/>
+      <c r="A152" s="40"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="A153" s="37"/>
+      <c r="A153" s="40"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="A154" s="37"/>
+      <c r="A154" s="40"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="37"/>
+      <c r="A155" s="40"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="A156" s="37"/>
+      <c r="A156" s="40"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="A157" s="37"/>
+      <c r="A157" s="40"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="A158" s="37"/>
+      <c r="A158" s="40"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="A159" s="37"/>
+      <c r="A159" s="40"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="37"/>
+      <c r="A160" s="40"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="A161" s="37"/>
+      <c r="A161" s="40"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="A162" s="37"/>
+      <c r="A162" s="40"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="A163" s="37"/>
+      <c r="A163" s="40"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="A164" s="37"/>
+      <c r="A164" s="40"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="37"/>
+      <c r="A165" s="40"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="A166" s="37"/>
+      <c r="A166" s="40"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="A167" s="37"/>
+      <c r="A167" s="40"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="A168" s="37"/>
+      <c r="A168" s="40"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="A169" s="37"/>
+      <c r="A169" s="40"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="A170" s="37"/>
+      <c r="A170" s="40"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="A171" s="37"/>
+      <c r="A171" s="40"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="37"/>
+      <c r="A172" s="40"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="A173" s="37"/>
+      <c r="A173" s="40"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="A174" s="37"/>
+      <c r="A174" s="40"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="A175" s="37"/>
+      <c r="A175" s="40"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="A176" s="37"/>
+      <c r="A176" s="40"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="A177" s="37"/>
+      <c r="A177" s="40"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="A178" s="37"/>
+      <c r="A178" s="40"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="A179" s="37"/>
+      <c r="A179" s="40"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="A180" s="37"/>
+      <c r="A180" s="40"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="A181" s="37"/>
+      <c r="A181" s="40"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="A182" s="37"/>
+      <c r="A182" s="40"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="A183" s="37"/>
+      <c r="A183" s="40"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="A184" s="37"/>
+      <c r="A184" s="40"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="A185" s="37"/>
+      <c r="A185" s="40"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="A186" s="37"/>
+      <c r="A186" s="40"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="A187" s="37"/>
+      <c r="A187" s="40"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="A188" s="37"/>
+      <c r="A188" s="40"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="A189" s="37"/>
+      <c r="A189" s="40"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="A190" s="37"/>
+      <c r="A190" s="40"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="A191" s="37"/>
+      <c r="A191" s="40"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="A192" s="37"/>
+      <c r="A192" s="40"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="A193" s="37"/>
+      <c r="A193" s="40"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="A194" s="37"/>
+      <c r="A194" s="40"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="A195" s="37"/>
+      <c r="A195" s="40"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="A196" s="37"/>
+      <c r="A196" s="40"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="A197" s="37"/>
+      <c r="A197" s="40"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="A198" s="37"/>
+      <c r="A198" s="40"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="A199" s="37"/>
+      <c r="A199" s="40"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="A200" s="37"/>
+      <c r="A200" s="40"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="A201" s="37"/>
+      <c r="A201" s="40"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="A202" s="37"/>
+      <c r="A202" s="40"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="A203" s="37"/>
+      <c r="A203" s="40"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="A204" s="37"/>
+      <c r="A204" s="40"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="A205" s="37"/>
+      <c r="A205" s="40"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="A206" s="37"/>
+      <c r="A206" s="40"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="A207" s="37"/>
+      <c r="A207" s="40"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="A208" s="37"/>
+      <c r="A208" s="40"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="A209" s="37"/>
+      <c r="A209" s="40"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="A210" s="37"/>
+      <c r="A210" s="40"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="A211" s="37"/>
+      <c r="A211" s="40"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="A212" s="37"/>
+      <c r="A212" s="40"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="A213" s="37"/>
+      <c r="A213" s="40"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="A214" s="37"/>
+      <c r="A214" s="40"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="A215" s="37"/>
+      <c r="A215" s="40"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="A216" s="37"/>
+      <c r="A216" s="40"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="A217" s="37"/>
+      <c r="A217" s="40"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="A218" s="37"/>
+      <c r="A218" s="40"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="A219" s="37"/>
+      <c r="A219" s="40"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="A220" s="37"/>
+      <c r="A220" s="40"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="A221" s="37"/>
+      <c r="A221" s="40"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="A222" s="37"/>
+      <c r="A222" s="40"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="A223" s="37"/>
+      <c r="A223" s="40"/>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="A224" s="37"/>
+      <c r="A224" s="40"/>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="A225" s="37"/>
+      <c r="A225" s="40"/>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="A226" s="37"/>
+      <c r="A226" s="40"/>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="A227" s="37"/>
+      <c r="A227" s="40"/>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="A228" s="37"/>
+      <c r="A228" s="40"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="A229" s="37"/>
+      <c r="A229" s="40"/>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="A230" s="37"/>
+      <c r="A230" s="40"/>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="A231" s="37"/>
+      <c r="A231" s="40"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="A232" s="37"/>
+      <c r="A232" s="40"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
-      <c r="A233" s="37"/>
+      <c r="A233" s="40"/>
     </row>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="A234" s="37"/>
+      <c r="A234" s="40"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="A235" s="37"/>
+      <c r="A235" s="40"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="A236" s="37"/>
+      <c r="A236" s="40"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="A237" s="37"/>
+      <c r="A237" s="40"/>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="A238" s="37"/>
+      <c r="A238" s="40"/>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="A239" s="37"/>
+      <c r="A239" s="40"/>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="A240" s="37"/>
+      <c r="A240" s="40"/>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="A241" s="37"/>
+      <c r="A241" s="40"/>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="A242" s="37"/>
+      <c r="A242" s="40"/>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="A243" s="37"/>
+      <c r="A243" s="40"/>
     </row>
     <row r="244" ht="15.75" customHeight="1">
-      <c r="A244" s="37"/>
+      <c r="A244" s="40"/>
     </row>
     <row r="245" ht="15.75" customHeight="1">
-      <c r="A245" s="37"/>
+      <c r="A245" s="40"/>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="A246" s="37"/>
+      <c r="A246" s="40"/>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="A247" s="37"/>
+      <c r="A247" s="40"/>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="A248" s="37"/>
+      <c r="A248" s="40"/>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="A249" s="37"/>
+      <c r="A249" s="40"/>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="A250" s="37"/>
+      <c r="A250" s="40"/>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="A251" s="37"/>
+      <c r="A251" s="40"/>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="A252" s="37"/>
+      <c r="A252" s="40"/>
     </row>
     <row r="253" ht="15.75" customHeight="1">
-      <c r="A253" s="37"/>
+      <c r="A253" s="40"/>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="A254" s="37"/>
+      <c r="A254" s="40"/>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="A255" s="37"/>
+      <c r="A255" s="40"/>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="A256" s="37"/>
+      <c r="A256" s="40"/>
     </row>
     <row r="257" ht="15.75" customHeight="1">
-      <c r="A257" s="37"/>
+      <c r="A257" s="40"/>
     </row>
     <row r="258" ht="15.75" customHeight="1">
-      <c r="A258" s="37"/>
+      <c r="A258" s="40"/>
     </row>
     <row r="259" ht="15.75" customHeight="1">
-      <c r="A259" s="37"/>
+      <c r="A259" s="40"/>
     </row>
     <row r="260" ht="15.75" customHeight="1">
-      <c r="A260" s="37"/>
+      <c r="A260" s="40"/>
     </row>
     <row r="261" ht="15.75" customHeight="1">
-      <c r="A261" s="37"/>
+      <c r="A261" s="40"/>
     </row>
     <row r="262" ht="15.75" customHeight="1">
-      <c r="A262" s="37"/>
+      <c r="A262" s="40"/>
     </row>
     <row r="263" ht="15.75" customHeight="1">
-      <c r="A263" s="37"/>
+      <c r="A263" s="40"/>
     </row>
     <row r="264" ht="15.75" customHeight="1">
-      <c r="A264" s="37"/>
+      <c r="A264" s="40"/>
     </row>
     <row r="265" ht="15.75" customHeight="1">
-      <c r="A265" s="37"/>
+      <c r="A265" s="40"/>
     </row>
     <row r="266" ht="15.75" customHeight="1">
-      <c r="A266" s="37"/>
+      <c r="A266" s="40"/>
     </row>
     <row r="267" ht="15.75" customHeight="1">
-      <c r="A267" s="37"/>
+      <c r="A267" s="40"/>
     </row>
     <row r="268" ht="15.75" customHeight="1">
-      <c r="A268" s="37"/>
+      <c r="A268" s="40"/>
     </row>
     <row r="269" ht="15.75" customHeight="1">
-      <c r="A269" s="37"/>
+      <c r="A269" s="40"/>
     </row>
     <row r="270" ht="15.75" customHeight="1">
-      <c r="A270" s="37"/>
+      <c r="A270" s="40"/>
     </row>
     <row r="271" ht="15.75" customHeight="1">
-      <c r="A271" s="37"/>
+      <c r="A271" s="40"/>
     </row>
     <row r="272" ht="15.75" customHeight="1">
-      <c r="A272" s="37"/>
+      <c r="A272" s="40"/>
     </row>
     <row r="273" ht="15.75" customHeight="1">
-      <c r="A273" s="37"/>
+      <c r="A273" s="40"/>
     </row>
     <row r="274" ht="15.75" customHeight="1">
-      <c r="A274" s="37"/>
+      <c r="A274" s="40"/>
     </row>
     <row r="275" ht="15.75" customHeight="1">
-      <c r="A275" s="37"/>
+      <c r="A275" s="40"/>
     </row>
     <row r="276" ht="15.75" customHeight="1">
-      <c r="A276" s="37"/>
+      <c r="A276" s="40"/>
     </row>
     <row r="277" ht="15.75" customHeight="1">
-      <c r="A277" s="37"/>
+      <c r="A277" s="40"/>
     </row>
     <row r="278" ht="15.75" customHeight="1">
-      <c r="A278" s="37"/>
+      <c r="A278" s="40"/>
     </row>
     <row r="279" ht="15.75" customHeight="1">
-      <c r="A279" s="37"/>
+      <c r="A279" s="40"/>
     </row>
     <row r="280" ht="15.75" customHeight="1">
-      <c r="A280" s="37"/>
+      <c r="A280" s="40"/>
     </row>
     <row r="281" ht="15.75" customHeight="1">
-      <c r="A281" s="37"/>
+      <c r="A281" s="40"/>
     </row>
     <row r="282" ht="15.75" customHeight="1">
-      <c r="A282" s="37"/>
+      <c r="A282" s="40"/>
     </row>
     <row r="283" ht="15.75" customHeight="1">
-      <c r="A283" s="37"/>
+      <c r="A283" s="40"/>
     </row>
     <row r="284" ht="15.75" customHeight="1">
-      <c r="A284" s="37"/>
+      <c r="A284" s="40"/>
     </row>
     <row r="285" ht="15.75" customHeight="1">
-      <c r="A285" s="37"/>
+      <c r="A285" s="40"/>
     </row>
     <row r="286" ht="15.75" customHeight="1">
-      <c r="A286" s="37"/>
+      <c r="A286" s="40"/>
     </row>
     <row r="287" ht="15.75" customHeight="1">
-      <c r="A287" s="37"/>
+      <c r="A287" s="40"/>
     </row>
     <row r="288" ht="15.75" customHeight="1">
-      <c r="A288" s="37"/>
+      <c r="A288" s="40"/>
     </row>
     <row r="289" ht="15.75" customHeight="1">
-      <c r="A289" s="37"/>
+      <c r="A289" s="40"/>
     </row>
     <row r="290" ht="15.75" customHeight="1">
-      <c r="A290" s="37"/>
+      <c r="A290" s="40"/>
     </row>
     <row r="291" ht="15.75" customHeight="1">
-      <c r="A291" s="37"/>
+      <c r="A291" s="40"/>
     </row>
     <row r="292" ht="15.75" customHeight="1">
-      <c r="A292" s="37"/>
+      <c r="A292" s="40"/>
     </row>
     <row r="293" ht="15.75" customHeight="1">
-      <c r="A293" s="37"/>
+      <c r="A293" s="40"/>
     </row>
     <row r="294" ht="15.75" customHeight="1">
-      <c r="A294" s="37"/>
+      <c r="A294" s="40"/>
     </row>
     <row r="295" ht="15.75" customHeight="1">
-      <c r="A295" s="37"/>
+      <c r="A295" s="40"/>
     </row>
     <row r="296" ht="15.75" customHeight="1">
-      <c r="A296" s="37"/>
+      <c r="A296" s="40"/>
     </row>
     <row r="297" ht="15.75" customHeight="1">
-      <c r="A297" s="37"/>
+      <c r="A297" s="40"/>
     </row>
     <row r="298" ht="15.75" customHeight="1">
-      <c r="A298" s="37"/>
+      <c r="A298" s="40"/>
     </row>
     <row r="299" ht="15.75" customHeight="1">
-      <c r="A299" s="37"/>
+      <c r="A299" s="40"/>
     </row>
     <row r="300" ht="15.75" customHeight="1">
-      <c r="A300" s="37"/>
+      <c r="A300" s="40"/>
     </row>
     <row r="301" ht="15.75" customHeight="1">
-      <c r="A301" s="37"/>
+      <c r="A301" s="40"/>
     </row>
     <row r="302" ht="15.75" customHeight="1">
-      <c r="A302" s="37"/>
+      <c r="A302" s="40"/>
     </row>
     <row r="303" ht="15.75" customHeight="1">
-      <c r="A303" s="37"/>
+      <c r="A303" s="40"/>
     </row>
     <row r="304" ht="15.75" customHeight="1">
-      <c r="A304" s="37"/>
+      <c r="A304" s="40"/>
     </row>
     <row r="305" ht="15.75" customHeight="1">
-      <c r="A305" s="37"/>
+      <c r="A305" s="40"/>
     </row>
     <row r="306" ht="15.75" customHeight="1">
-      <c r="A306" s="37"/>
+      <c r="A306" s="40"/>
     </row>
     <row r="307" ht="15.75" customHeight="1">
-      <c r="A307" s="37"/>
+      <c r="A307" s="40"/>
     </row>
     <row r="308" ht="15.75" customHeight="1">
-      <c r="A308" s="37"/>
+      <c r="A308" s="40"/>
     </row>
     <row r="309" ht="15.75" customHeight="1">
-      <c r="A309" s="37"/>
+      <c r="A309" s="40"/>
     </row>
     <row r="310" ht="15.75" customHeight="1">
-      <c r="A310" s="37"/>
+      <c r="A310" s="40"/>
     </row>
     <row r="311" ht="15.75" customHeight="1">
-      <c r="A311" s="37"/>
+      <c r="A311" s="40"/>
     </row>
     <row r="312" ht="15.75" customHeight="1">
-      <c r="A312" s="37"/>
+      <c r="A312" s="40"/>
     </row>
     <row r="313" ht="15.75" customHeight="1">
-      <c r="A313" s="37"/>
+      <c r="A313" s="40"/>
     </row>
     <row r="314" ht="15.75" customHeight="1">
-      <c r="A314" s="7"/>
+      <c r="A314" s="40"/>
     </row>
     <row r="315" ht="15.75" customHeight="1">
       <c r="A315" s="7"/>
@@ -5229,6 +5255,9 @@
     </row>
     <row r="1003" ht="15.75" customHeight="1">
       <c r="A1003" s="7"/>
+    </row>
+    <row r="1004" ht="15.75" customHeight="1">
+      <c r="A1004" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add log in function
</commit_message>
<xml_diff>
--- a/translation.xlsx
+++ b/translation.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="278">
   <si>
     <t>English</t>
   </si>
@@ -340,8 +340,7 @@
     <t>The report "Vietnam as an Ageing Society" recently explained that up to 16% of Vietnamese aged over 60 fall into poverty. Meanwhile, only 23.5% of people over 60 are entitled to receive a monthly pension or social insurance benefit. The income of the elderly after retirement depends heavily on their family. The traditional family model of many generations living under the same roof is gradually shifting to the nuclear family model. At that time, the elderly had to live alone, away from their children. In addition, the health care system is limited in Vietnam, along with the increasing health care cost has negatively affected the living standard after the retirement of the elderly</t>
   </si>
   <si>
-    <t xml:space="preserve">Báo cáo “Vietnam as an Ageing Society” mới đây đã chỉ ra rằng có đến 16% người Việt Nam trên 60 tuổi rơi vào nhóm nghèo. Trong khi đó, chỉ có 23,5% người trên 60 tuổi được hưởng lương hưu hoặc trợ cấp bảo hiểm xã hội hàng tháng. Thu nhập của người cao tuổi sau về hưu phụ thuộc lớn vào trợ cấp từ con cái. Mô hình gia đình truyền thống nhiều thế hệ cùng chung sống dưới một mái nhà đang chuyển dần sang mô hình gia đình hạt nhân. Khi đó, người cao tuổi phải sống xa con cái và có khả năng sống một mình. Ngoài ra, hệ thống chăm sóc sức khỏe còn hạn chế ở Việt Nam, cùng với chi phí khám chữa bệnh ngày càng tăng đã ảnh hưởng tiêu cực đến sự hưởng thụ sau khi về hưu của người cao tuổi. 
-</t>
+    <t>Báo cáo “Vietnam as an Ageing Society” mới đây đã chỉ ra rằng có đến 16% người Việt Nam trên 60 tuổi rơi vào nhóm nghèo. Trong khi đó, chỉ có 23,5% người trên 60 tuổi được hưởng lương hưu hoặc trợ cấp bảo hiểm xã hội hàng tháng. Thu nhập của người cao tuổi sau về hưu phụ thuộc lớn vào trợ cấp từ con cái. Mô hình gia đình truyền thống nhiều thế hệ cùng chung sống dưới một mái nhà đang chuyển dần sang mô hình gia đình hạt nhân. Khi đó, người cao tuổi phải sống xa con cái và có khả năng sống một mình. Ngoài ra, hệ thống chăm sóc sức khỏe còn hạn chế ở Việt Nam, cùng với chi phí khám chữa bệnh ngày càng tăng đã ảnh hưởng tiêu cực đến sự hưởng thụ sau khi về hưu của người cao tuổi.</t>
   </si>
   <si>
     <t>People aged over 60 by 2035</t>
@@ -920,6 +919,18 @@
   </si>
   <si>
     <t>Triệu</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Mật khẩu</t>
+  </si>
+  <si>
+    <t>Sign out</t>
+  </si>
+  <si>
+    <t>Đăng xuất</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1061,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1082,6 +1093,9 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1872,7 +1886,7 @@
       <c r="A50" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="11" t="s">
         <v>97</v>
       </c>
       <c r="C50" s="7"/>
@@ -1896,7 +1910,7 @@
       <c r="C52" s="7"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="12" t="s">
         <v>102</v>
       </c>
       <c r="B53" s="5" t="s">
@@ -1905,7 +1919,7 @@
       <c r="C53" s="7"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="11" t="s">
+      <c r="A54" s="12" t="s">
         <v>104</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -1914,7 +1928,7 @@
       <c r="C54" s="7"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="12" t="s">
         <v>106</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -1923,7 +1937,7 @@
       <c r="C55" s="7"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="12" t="s">
         <v>108</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -1932,7 +1946,7 @@
       <c r="C56" s="7"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="12" t="s">
+      <c r="A57" s="13" t="s">
         <v>110</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -1941,7 +1955,7 @@
       <c r="C57" s="7"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="12" t="s">
+      <c r="A58" s="13" t="s">
         <v>112</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -1950,7 +1964,7 @@
       <c r="C58" s="7"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="12" t="s">
         <v>114</v>
       </c>
       <c r="B59" s="5" t="s">
@@ -1959,7 +1973,7 @@
       <c r="C59" s="7"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="12" t="s">
         <v>116</v>
       </c>
       <c r="B60" s="5" t="s">
@@ -1968,7 +1982,7 @@
       <c r="C60" s="7"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="11" t="s">
+      <c r="A61" s="12" t="s">
         <v>118</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -1977,7 +1991,7 @@
       <c r="C61" s="7"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="11" t="s">
+      <c r="A62" s="12" t="s">
         <v>120</v>
       </c>
       <c r="B62" s="5" t="s">
@@ -1986,7 +2000,7 @@
       <c r="C62" s="7"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="12" t="s">
         <v>122</v>
       </c>
       <c r="B63" s="5" t="s">
@@ -1995,71 +2009,71 @@
       <c r="C63" s="7"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B64" s="13" t="s">
+      <c r="B64" s="14" t="s">
         <v>125</v>
       </c>
       <c r="C64" s="7"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="11" t="s">
+      <c r="A65" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B65" s="13" t="s">
+      <c r="B65" s="14" t="s">
         <v>127</v>
       </c>
       <c r="C65" s="7"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="11" t="s">
+      <c r="A66" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B66" s="13" t="s">
+      <c r="B66" s="14" t="s">
         <v>129</v>
       </c>
       <c r="C66" s="7"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="11" t="s">
+      <c r="A67" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="B67" s="13" t="s">
+      <c r="B67" s="14" t="s">
         <v>131</v>
       </c>
       <c r="C67" s="7"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="14"/>
-      <c r="B68" s="15" t="s">
+      <c r="A68" s="15"/>
+      <c r="B68" s="16" t="s">
         <v>132</v>
       </c>
       <c r="C68" s="7"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="B69" s="17" t="s">
+      <c r="B69" s="18" t="s">
         <v>134</v>
       </c>
       <c r="C69" s="7"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="18" t="s">
+      <c r="A70" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="B70" s="13" t="s">
+      <c r="B70" s="14" t="s">
         <v>136</v>
       </c>
       <c r="C70" s="7"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="18" t="s">
+      <c r="A71" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B71" s="13" t="s">
+      <c r="B71" s="14" t="s">
         <v>138</v>
       </c>
       <c r="C71" s="7"/>
@@ -2068,7 +2082,7 @@
       <c r="A72" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B72" s="13" t="s">
+      <c r="B72" s="14" t="s">
         <v>140</v>
       </c>
       <c r="C72" s="7"/>
@@ -2077,7 +2091,7 @@
       <c r="A73" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B73" s="13" t="s">
+      <c r="B73" s="14" t="s">
         <v>142</v>
       </c>
       <c r="C73" s="7"/>
@@ -2086,7 +2100,7 @@
       <c r="A74" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B74" s="13" t="s">
+      <c r="B74" s="14" t="s">
         <v>144</v>
       </c>
       <c r="C74" s="7"/>
@@ -2095,7 +2109,7 @@
       <c r="A75" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B75" s="13" t="s">
+      <c r="B75" s="14" t="s">
         <v>146</v>
       </c>
       <c r="C75" s="7"/>
@@ -2104,7 +2118,7 @@
       <c r="A76" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="B76" s="13" t="s">
+      <c r="B76" s="14" t="s">
         <v>148</v>
       </c>
       <c r="C76" s="7"/>
@@ -2119,21 +2133,21 @@
       <c r="C77" s="7"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="19" t="s">
+      <c r="A78" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="B78" s="19" t="s">
+      <c r="B78" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="C78" s="20" t="s">
+      <c r="C78" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="D78" s="21" t="s">
+      <c r="D78" s="22" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="11" t="s">
+      <c r="A79" s="12" t="s">
         <v>155</v>
       </c>
       <c r="B79" s="5" t="s">
@@ -2142,7 +2156,7 @@
       <c r="C79" s="7"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="22" t="s">
+      <c r="A80" s="23" t="s">
         <v>157</v>
       </c>
       <c r="B80" s="5" t="s">
@@ -2151,7 +2165,7 @@
       <c r="C80" s="7"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="11" t="s">
+      <c r="A81" s="12" t="s">
         <v>159</v>
       </c>
       <c r="B81" s="5" t="s">
@@ -2160,7 +2174,7 @@
       <c r="C81" s="7"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="11" t="s">
+      <c r="A82" s="12" t="s">
         <v>161</v>
       </c>
       <c r="B82" s="5" t="s">
@@ -2169,7 +2183,7 @@
       <c r="C82" s="7"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="12" t="s">
+      <c r="A83" s="13" t="s">
         <v>163</v>
       </c>
       <c r="B83" s="5" t="s">
@@ -2178,7 +2192,7 @@
       <c r="C83" s="7"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="11" t="s">
+      <c r="A84" s="12" t="s">
         <v>165</v>
       </c>
       <c r="B84" s="5" t="s">
@@ -2187,7 +2201,7 @@
       <c r="C84" s="7"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="12" t="s">
         <v>167</v>
       </c>
       <c r="B85" s="5" t="s">
@@ -2196,7 +2210,7 @@
       <c r="C85" s="7"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="11" t="s">
+      <c r="A86" s="12" t="s">
         <v>169</v>
       </c>
       <c r="B86" s="5" t="s">
@@ -2205,7 +2219,7 @@
       <c r="C86" s="7"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="11" t="s">
+      <c r="A87" s="12" t="s">
         <v>171</v>
       </c>
       <c r="B87" s="5" t="s">
@@ -2214,7 +2228,7 @@
       <c r="C87" s="7"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="11" t="s">
+      <c r="A88" s="12" t="s">
         <v>173</v>
       </c>
       <c r="B88" s="5" t="s">
@@ -2223,7 +2237,7 @@
       <c r="C88" s="7"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="11" t="s">
+      <c r="A89" s="12" t="s">
         <v>175</v>
       </c>
       <c r="B89" s="5" t="s">
@@ -2232,7 +2246,7 @@
       <c r="C89" s="7"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="23" t="s">
+      <c r="A90" s="24" t="s">
         <v>177</v>
       </c>
       <c r="B90" s="5" t="s">
@@ -2241,7 +2255,7 @@
       <c r="C90" s="7"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="11" t="s">
+      <c r="A91" s="12" t="s">
         <v>179</v>
       </c>
       <c r="B91" s="5" t="s">
@@ -2250,7 +2264,7 @@
       <c r="C91" s="7"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="11" t="s">
+      <c r="A92" s="12" t="s">
         <v>181</v>
       </c>
       <c r="B92" s="5" t="s">
@@ -2259,7 +2273,7 @@
       <c r="C92" s="7"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="11" t="s">
+      <c r="A93" s="12" t="s">
         <v>183</v>
       </c>
       <c r="B93" s="5" t="s">
@@ -2268,7 +2282,7 @@
       <c r="C93" s="7"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="12" t="s">
+      <c r="A94" s="13" t="s">
         <v>185</v>
       </c>
       <c r="B94" s="5" t="s">
@@ -2277,7 +2291,7 @@
       <c r="C94" s="7"/>
     </row>
     <row r="95" ht="67.5" customHeight="1">
-      <c r="A95" s="24" t="s">
+      <c r="A95" s="25" t="s">
         <v>187</v>
       </c>
       <c r="B95" s="9" t="s">
@@ -2286,7 +2300,7 @@
       <c r="C95" s="7"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="11" t="s">
+      <c r="A96" s="12" t="s">
         <v>189</v>
       </c>
       <c r="B96" s="5" t="s">
@@ -2295,7 +2309,7 @@
       <c r="C96" s="7"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="11" t="s">
+      <c r="A97" s="12" t="s">
         <v>191</v>
       </c>
       <c r="B97" s="5" t="s">
@@ -2304,7 +2318,7 @@
       <c r="C97" s="7"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="11" t="s">
+      <c r="A98" s="12" t="s">
         <v>193</v>
       </c>
       <c r="B98" s="5" t="s">
@@ -2313,52 +2327,52 @@
       <c r="C98" s="7"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="11" t="s">
+      <c r="A99" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B99" s="25" t="s">
+      <c r="B99" s="26" t="s">
         <v>196</v>
       </c>
       <c r="C99" s="7"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="11" t="s">
+      <c r="A100" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="B100" s="25" t="s">
+      <c r="B100" s="26" t="s">
         <v>198</v>
       </c>
       <c r="C100" s="7"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="11" t="s">
+      <c r="A101" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="B101" s="25" t="s">
+      <c r="B101" s="26" t="s">
         <v>200</v>
       </c>
       <c r="C101" s="7"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="11" t="s">
+      <c r="A102" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="B102" s="25" t="s">
+      <c r="B102" s="26" t="s">
         <v>202</v>
       </c>
       <c r="C102" s="7"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="11" t="s">
+      <c r="A103" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="B103" s="25" t="s">
+      <c r="B103" s="26" t="s">
         <v>204</v>
       </c>
       <c r="C103" s="7"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="11" t="s">
+      <c r="A104" s="12" t="s">
         <v>205</v>
       </c>
       <c r="B104" s="5" t="s">
@@ -2367,7 +2381,7 @@
       <c r="C104" s="7"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="11" t="s">
+      <c r="A105" s="12" t="s">
         <v>207</v>
       </c>
       <c r="B105" s="5" t="s">
@@ -2376,7 +2390,7 @@
       <c r="C105" s="7"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="11" t="s">
+      <c r="A106" s="12" t="s">
         <v>209</v>
       </c>
       <c r="B106" s="5" t="s">
@@ -2385,16 +2399,16 @@
       <c r="C106" s="7"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="11" t="s">
+      <c r="A107" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="B107" s="26" t="s">
+      <c r="B107" s="27" t="s">
         <v>212</v>
       </c>
       <c r="C107" s="7"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="11" t="s">
+      <c r="A108" s="12" t="s">
         <v>213</v>
       </c>
       <c r="B108" s="5" t="s">
@@ -2403,7 +2417,7 @@
       <c r="C108" s="7"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="11" t="s">
+      <c r="A109" s="12" t="s">
         <v>215</v>
       </c>
       <c r="B109" s="5" t="s">
@@ -2412,7 +2426,7 @@
       <c r="C109" s="7"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="11" t="s">
+      <c r="A110" s="12" t="s">
         <v>217</v>
       </c>
       <c r="B110" s="5" t="s">
@@ -2421,7 +2435,7 @@
       <c r="C110" s="7"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="11" t="s">
+      <c r="A111" s="12" t="s">
         <v>219</v>
       </c>
       <c r="B111" s="5" t="s">
@@ -2430,7 +2444,7 @@
       <c r="C111" s="7"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="11" t="s">
+      <c r="A112" s="12" t="s">
         <v>221</v>
       </c>
       <c r="B112" s="5" t="s">
@@ -2439,7 +2453,7 @@
       <c r="C112" s="7"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="11" t="s">
+      <c r="A113" s="12" t="s">
         <v>223</v>
       </c>
       <c r="B113" s="5" t="s">
@@ -2448,7 +2462,7 @@
       <c r="C113" s="7"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="11" t="s">
+      <c r="A114" s="12" t="s">
         <v>225</v>
       </c>
       <c r="B114" s="5" t="s">
@@ -2457,7 +2471,7 @@
       <c r="C114" s="7"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="27" t="s">
+      <c r="A115" s="28" t="s">
         <v>227</v>
       </c>
       <c r="B115" s="5" t="s">
@@ -2466,7 +2480,7 @@
       <c r="C115" s="7"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="28" t="s">
+      <c r="A116" s="29" t="s">
         <v>229</v>
       </c>
       <c r="B116" s="9" t="s">
@@ -2475,719 +2489,729 @@
       <c r="C116" s="7"/>
     </row>
     <row r="117" ht="90.0" customHeight="1">
-      <c r="A117" s="29" t="s">
+      <c r="A117" s="30" t="s">
         <v>230</v>
       </c>
-      <c r="B117" s="11" t="s">
+      <c r="B117" s="12" t="s">
         <v>231</v>
       </c>
       <c r="C117" s="7"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="28" t="s">
+      <c r="A118" s="29" t="s">
         <v>232</v>
       </c>
-      <c r="B118" s="11" t="s">
+      <c r="B118" s="12" t="s">
         <v>233</v>
       </c>
       <c r="C118" s="7"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="28" t="s">
+      <c r="A119" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="B119" s="11" t="s">
+      <c r="B119" s="12" t="s">
         <v>235</v>
       </c>
       <c r="C119" s="7"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="28" t="s">
+      <c r="A120" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="B120" s="11" t="s">
+      <c r="B120" s="12" t="s">
         <v>237</v>
       </c>
       <c r="C120" s="7"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="28" t="s">
+      <c r="A121" s="29" t="s">
         <v>238</v>
       </c>
-      <c r="B121" s="11" t="s">
+      <c r="B121" s="12" t="s">
         <v>239</v>
       </c>
       <c r="C121" s="7"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="28" t="s">
+      <c r="A122" s="29" t="s">
         <v>240</v>
       </c>
-      <c r="B122" s="11" t="s">
+      <c r="B122" s="12" t="s">
         <v>241</v>
       </c>
       <c r="C122" s="7"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="29" t="s">
+      <c r="A123" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="B123" s="11" t="s">
+      <c r="B123" s="12" t="s">
         <v>243</v>
       </c>
       <c r="C123" s="7"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="30" t="s">
+      <c r="A124" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="B124" s="11" t="s">
+      <c r="B124" s="12" t="s">
         <v>245</v>
       </c>
       <c r="C124" s="7"/>
     </row>
     <row r="125" ht="82.5" customHeight="1">
-      <c r="A125" s="30" t="s">
+      <c r="A125" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="B125" s="11" t="s">
+      <c r="B125" s="12" t="s">
         <v>247</v>
       </c>
       <c r="C125" s="7"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="30" t="s">
+      <c r="A126" s="31" t="s">
         <v>248</v>
       </c>
-      <c r="B126" s="11" t="s">
+      <c r="B126" s="12" t="s">
         <v>249</v>
       </c>
       <c r="C126" s="7"/>
     </row>
     <row r="127" ht="17.25" customHeight="1">
-      <c r="A127" s="31" t="s">
+      <c r="A127" s="32" t="s">
         <v>250</v>
       </c>
-      <c r="B127" s="32" t="s">
+      <c r="B127" s="33" t="s">
         <v>251</v>
       </c>
       <c r="C127" s="7"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="33" t="s">
+      <c r="A128" s="34" t="s">
         <v>252</v>
       </c>
-      <c r="B128" s="34" t="s">
+      <c r="B128" s="35" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="35" t="s">
+      <c r="A129" s="36" t="s">
         <v>254</v>
       </c>
-      <c r="B129" s="34" t="s">
+      <c r="B129" s="35" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="33" t="s">
+      <c r="A130" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="B130" s="34" t="s">
+      <c r="B130" s="35" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="131" ht="16.5" customHeight="1">
-      <c r="A131" s="33" t="s">
+      <c r="A131" s="34" t="s">
         <v>258</v>
       </c>
-      <c r="B131" s="34" t="s">
+      <c r="B131" s="35" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="33" t="s">
+      <c r="A132" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="B132" s="34" t="s">
+      <c r="B132" s="35" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="33" t="s">
+      <c r="A133" s="34" t="s">
         <v>262</v>
       </c>
-      <c r="B133" s="36" t="s">
+      <c r="B133" s="37" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="37" t="s">
+      <c r="A134" s="38" t="s">
         <v>264</v>
       </c>
-      <c r="B134" s="38" t="s">
+      <c r="B134" s="39" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="37" t="s">
+      <c r="A135" s="38" t="s">
         <v>266</v>
       </c>
-      <c r="B135" s="38" t="s">
+      <c r="B135" s="39" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="39" t="s">
+      <c r="A136" s="40" t="s">
         <v>268</v>
       </c>
-      <c r="B136" s="36" t="s">
+      <c r="B136" s="37" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="39" t="s">
+      <c r="A137" s="40" t="s">
         <v>270</v>
       </c>
-      <c r="B137" s="38" t="s">
+      <c r="B137" s="39" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="39" t="s">
+      <c r="A138" s="40" t="s">
         <v>272</v>
       </c>
-      <c r="B138" s="38" t="s">
+      <c r="B138" s="39" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="40"/>
+      <c r="A139" s="40" t="s">
+        <v>274</v>
+      </c>
+      <c r="B139" s="39" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="40"/>
+      <c r="A140" s="40" t="s">
+        <v>276</v>
+      </c>
+      <c r="B140" s="37" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="40"/>
+      <c r="A141" s="41"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="40"/>
+      <c r="A142" s="41"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="40"/>
+      <c r="A143" s="41"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="A144" s="40"/>
+      <c r="A144" s="41"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="40"/>
+      <c r="A145" s="41"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="40"/>
+      <c r="A146" s="41"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="40"/>
+      <c r="A147" s="41"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="A148" s="40"/>
+      <c r="A148" s="41"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="A149" s="40"/>
+      <c r="A149" s="41"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="A150" s="40"/>
+      <c r="A150" s="41"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="A151" s="40"/>
+      <c r="A151" s="41"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="A152" s="40"/>
+      <c r="A152" s="41"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="A153" s="40"/>
+      <c r="A153" s="41"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="A154" s="40"/>
+      <c r="A154" s="41"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="40"/>
+      <c r="A155" s="41"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="A156" s="40"/>
+      <c r="A156" s="41"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="A157" s="40"/>
+      <c r="A157" s="41"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="A158" s="40"/>
+      <c r="A158" s="41"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="A159" s="40"/>
+      <c r="A159" s="41"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="40"/>
+      <c r="A160" s="41"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="A161" s="40"/>
+      <c r="A161" s="41"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="A162" s="40"/>
+      <c r="A162" s="41"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="A163" s="40"/>
+      <c r="A163" s="41"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="A164" s="40"/>
+      <c r="A164" s="41"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="40"/>
+      <c r="A165" s="41"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="A166" s="40"/>
+      <c r="A166" s="41"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="A167" s="40"/>
+      <c r="A167" s="41"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="A168" s="40"/>
+      <c r="A168" s="41"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="A169" s="40"/>
+      <c r="A169" s="41"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="A170" s="40"/>
+      <c r="A170" s="41"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="A171" s="40"/>
+      <c r="A171" s="41"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="40"/>
+      <c r="A172" s="41"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="A173" s="40"/>
+      <c r="A173" s="41"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="A174" s="40"/>
+      <c r="A174" s="41"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="A175" s="40"/>
+      <c r="A175" s="41"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="A176" s="40"/>
+      <c r="A176" s="41"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="A177" s="40"/>
+      <c r="A177" s="41"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="A178" s="40"/>
+      <c r="A178" s="41"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="A179" s="40"/>
+      <c r="A179" s="41"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="A180" s="40"/>
+      <c r="A180" s="41"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="A181" s="40"/>
+      <c r="A181" s="41"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="A182" s="40"/>
+      <c r="A182" s="41"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="A183" s="40"/>
+      <c r="A183" s="41"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="A184" s="40"/>
+      <c r="A184" s="41"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="A185" s="40"/>
+      <c r="A185" s="41"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="A186" s="40"/>
+      <c r="A186" s="41"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="A187" s="40"/>
+      <c r="A187" s="41"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="A188" s="40"/>
+      <c r="A188" s="41"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="A189" s="40"/>
+      <c r="A189" s="41"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="A190" s="40"/>
+      <c r="A190" s="41"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="A191" s="40"/>
+      <c r="A191" s="41"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="A192" s="40"/>
+      <c r="A192" s="41"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="A193" s="40"/>
+      <c r="A193" s="41"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="A194" s="40"/>
+      <c r="A194" s="41"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="A195" s="40"/>
+      <c r="A195" s="41"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="A196" s="40"/>
+      <c r="A196" s="41"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="A197" s="40"/>
+      <c r="A197" s="41"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="A198" s="40"/>
+      <c r="A198" s="41"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="A199" s="40"/>
+      <c r="A199" s="41"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="A200" s="40"/>
+      <c r="A200" s="41"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="A201" s="40"/>
+      <c r="A201" s="41"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="A202" s="40"/>
+      <c r="A202" s="41"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="A203" s="40"/>
+      <c r="A203" s="41"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="A204" s="40"/>
+      <c r="A204" s="41"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="A205" s="40"/>
+      <c r="A205" s="41"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="A206" s="40"/>
+      <c r="A206" s="41"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="A207" s="40"/>
+      <c r="A207" s="41"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="A208" s="40"/>
+      <c r="A208" s="41"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="A209" s="40"/>
+      <c r="A209" s="41"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="A210" s="40"/>
+      <c r="A210" s="41"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="A211" s="40"/>
+      <c r="A211" s="41"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="A212" s="40"/>
+      <c r="A212" s="41"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="A213" s="40"/>
+      <c r="A213" s="41"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="A214" s="40"/>
+      <c r="A214" s="41"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="A215" s="40"/>
+      <c r="A215" s="41"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="A216" s="40"/>
+      <c r="A216" s="41"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="A217" s="40"/>
+      <c r="A217" s="41"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="A218" s="40"/>
+      <c r="A218" s="41"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="A219" s="40"/>
+      <c r="A219" s="41"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="A220" s="40"/>
+      <c r="A220" s="41"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="A221" s="40"/>
+      <c r="A221" s="41"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="A222" s="40"/>
+      <c r="A222" s="41"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="A223" s="40"/>
+      <c r="A223" s="41"/>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="A224" s="40"/>
+      <c r="A224" s="41"/>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="A225" s="40"/>
+      <c r="A225" s="41"/>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="A226" s="40"/>
+      <c r="A226" s="41"/>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="A227" s="40"/>
+      <c r="A227" s="41"/>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="A228" s="40"/>
+      <c r="A228" s="41"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="A229" s="40"/>
+      <c r="A229" s="41"/>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="A230" s="40"/>
+      <c r="A230" s="41"/>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="A231" s="40"/>
+      <c r="A231" s="41"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="A232" s="40"/>
+      <c r="A232" s="41"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
-      <c r="A233" s="40"/>
+      <c r="A233" s="41"/>
     </row>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="A234" s="40"/>
+      <c r="A234" s="41"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="A235" s="40"/>
+      <c r="A235" s="41"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="A236" s="40"/>
+      <c r="A236" s="41"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="A237" s="40"/>
+      <c r="A237" s="41"/>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="A238" s="40"/>
+      <c r="A238" s="41"/>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="A239" s="40"/>
+      <c r="A239" s="41"/>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="A240" s="40"/>
+      <c r="A240" s="41"/>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="A241" s="40"/>
+      <c r="A241" s="41"/>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="A242" s="40"/>
+      <c r="A242" s="41"/>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="A243" s="40"/>
+      <c r="A243" s="41"/>
     </row>
     <row r="244" ht="15.75" customHeight="1">
-      <c r="A244" s="40"/>
+      <c r="A244" s="41"/>
     </row>
     <row r="245" ht="15.75" customHeight="1">
-      <c r="A245" s="40"/>
+      <c r="A245" s="41"/>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="A246" s="40"/>
+      <c r="A246" s="41"/>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="A247" s="40"/>
+      <c r="A247" s="41"/>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="A248" s="40"/>
+      <c r="A248" s="41"/>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="A249" s="40"/>
+      <c r="A249" s="41"/>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="A250" s="40"/>
+      <c r="A250" s="41"/>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="A251" s="40"/>
+      <c r="A251" s="41"/>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="A252" s="40"/>
+      <c r="A252" s="41"/>
     </row>
     <row r="253" ht="15.75" customHeight="1">
-      <c r="A253" s="40"/>
+      <c r="A253" s="41"/>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="A254" s="40"/>
+      <c r="A254" s="41"/>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="A255" s="40"/>
+      <c r="A255" s="41"/>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="A256" s="40"/>
+      <c r="A256" s="41"/>
     </row>
     <row r="257" ht="15.75" customHeight="1">
-      <c r="A257" s="40"/>
+      <c r="A257" s="41"/>
     </row>
     <row r="258" ht="15.75" customHeight="1">
-      <c r="A258" s="40"/>
+      <c r="A258" s="41"/>
     </row>
     <row r="259" ht="15.75" customHeight="1">
-      <c r="A259" s="40"/>
+      <c r="A259" s="41"/>
     </row>
     <row r="260" ht="15.75" customHeight="1">
-      <c r="A260" s="40"/>
+      <c r="A260" s="41"/>
     </row>
     <row r="261" ht="15.75" customHeight="1">
-      <c r="A261" s="40"/>
+      <c r="A261" s="41"/>
     </row>
     <row r="262" ht="15.75" customHeight="1">
-      <c r="A262" s="40"/>
+      <c r="A262" s="41"/>
     </row>
     <row r="263" ht="15.75" customHeight="1">
-      <c r="A263" s="40"/>
+      <c r="A263" s="41"/>
     </row>
     <row r="264" ht="15.75" customHeight="1">
-      <c r="A264" s="40"/>
+      <c r="A264" s="41"/>
     </row>
     <row r="265" ht="15.75" customHeight="1">
-      <c r="A265" s="40"/>
+      <c r="A265" s="41"/>
     </row>
     <row r="266" ht="15.75" customHeight="1">
-      <c r="A266" s="40"/>
+      <c r="A266" s="41"/>
     </row>
     <row r="267" ht="15.75" customHeight="1">
-      <c r="A267" s="40"/>
+      <c r="A267" s="41"/>
     </row>
     <row r="268" ht="15.75" customHeight="1">
-      <c r="A268" s="40"/>
+      <c r="A268" s="41"/>
     </row>
     <row r="269" ht="15.75" customHeight="1">
-      <c r="A269" s="40"/>
+      <c r="A269" s="41"/>
     </row>
     <row r="270" ht="15.75" customHeight="1">
-      <c r="A270" s="40"/>
+      <c r="A270" s="41"/>
     </row>
     <row r="271" ht="15.75" customHeight="1">
-      <c r="A271" s="40"/>
+      <c r="A271" s="41"/>
     </row>
     <row r="272" ht="15.75" customHeight="1">
-      <c r="A272" s="40"/>
+      <c r="A272" s="41"/>
     </row>
     <row r="273" ht="15.75" customHeight="1">
-      <c r="A273" s="40"/>
+      <c r="A273" s="41"/>
     </row>
     <row r="274" ht="15.75" customHeight="1">
-      <c r="A274" s="40"/>
+      <c r="A274" s="41"/>
     </row>
     <row r="275" ht="15.75" customHeight="1">
-      <c r="A275" s="40"/>
+      <c r="A275" s="41"/>
     </row>
     <row r="276" ht="15.75" customHeight="1">
-      <c r="A276" s="40"/>
+      <c r="A276" s="41"/>
     </row>
     <row r="277" ht="15.75" customHeight="1">
-      <c r="A277" s="40"/>
+      <c r="A277" s="41"/>
     </row>
     <row r="278" ht="15.75" customHeight="1">
-      <c r="A278" s="40"/>
+      <c r="A278" s="41"/>
     </row>
     <row r="279" ht="15.75" customHeight="1">
-      <c r="A279" s="40"/>
+      <c r="A279" s="41"/>
     </row>
     <row r="280" ht="15.75" customHeight="1">
-      <c r="A280" s="40"/>
+      <c r="A280" s="41"/>
     </row>
     <row r="281" ht="15.75" customHeight="1">
-      <c r="A281" s="40"/>
+      <c r="A281" s="41"/>
     </row>
     <row r="282" ht="15.75" customHeight="1">
-      <c r="A282" s="40"/>
+      <c r="A282" s="41"/>
     </row>
     <row r="283" ht="15.75" customHeight="1">
-      <c r="A283" s="40"/>
+      <c r="A283" s="41"/>
     </row>
     <row r="284" ht="15.75" customHeight="1">
-      <c r="A284" s="40"/>
+      <c r="A284" s="41"/>
     </row>
     <row r="285" ht="15.75" customHeight="1">
-      <c r="A285" s="40"/>
+      <c r="A285" s="41"/>
     </row>
     <row r="286" ht="15.75" customHeight="1">
-      <c r="A286" s="40"/>
+      <c r="A286" s="41"/>
     </row>
     <row r="287" ht="15.75" customHeight="1">
-      <c r="A287" s="40"/>
+      <c r="A287" s="41"/>
     </row>
     <row r="288" ht="15.75" customHeight="1">
-      <c r="A288" s="40"/>
+      <c r="A288" s="41"/>
     </row>
     <row r="289" ht="15.75" customHeight="1">
-      <c r="A289" s="40"/>
+      <c r="A289" s="41"/>
     </row>
     <row r="290" ht="15.75" customHeight="1">
-      <c r="A290" s="40"/>
+      <c r="A290" s="41"/>
     </row>
     <row r="291" ht="15.75" customHeight="1">
-      <c r="A291" s="40"/>
+      <c r="A291" s="41"/>
     </row>
     <row r="292" ht="15.75" customHeight="1">
-      <c r="A292" s="40"/>
+      <c r="A292" s="41"/>
     </row>
     <row r="293" ht="15.75" customHeight="1">
-      <c r="A293" s="40"/>
+      <c r="A293" s="41"/>
     </row>
     <row r="294" ht="15.75" customHeight="1">
-      <c r="A294" s="40"/>
+      <c r="A294" s="41"/>
     </row>
     <row r="295" ht="15.75" customHeight="1">
-      <c r="A295" s="40"/>
+      <c r="A295" s="41"/>
     </row>
     <row r="296" ht="15.75" customHeight="1">
-      <c r="A296" s="40"/>
+      <c r="A296" s="41"/>
     </row>
     <row r="297" ht="15.75" customHeight="1">
-      <c r="A297" s="40"/>
+      <c r="A297" s="41"/>
     </row>
     <row r="298" ht="15.75" customHeight="1">
-      <c r="A298" s="40"/>
+      <c r="A298" s="41"/>
     </row>
     <row r="299" ht="15.75" customHeight="1">
-      <c r="A299" s="40"/>
+      <c r="A299" s="41"/>
     </row>
     <row r="300" ht="15.75" customHeight="1">
-      <c r="A300" s="40"/>
+      <c r="A300" s="41"/>
     </row>
     <row r="301" ht="15.75" customHeight="1">
-      <c r="A301" s="40"/>
+      <c r="A301" s="41"/>
     </row>
     <row r="302" ht="15.75" customHeight="1">
-      <c r="A302" s="40"/>
+      <c r="A302" s="41"/>
     </row>
     <row r="303" ht="15.75" customHeight="1">
-      <c r="A303" s="40"/>
+      <c r="A303" s="41"/>
     </row>
     <row r="304" ht="15.75" customHeight="1">
-      <c r="A304" s="40"/>
+      <c r="A304" s="41"/>
     </row>
     <row r="305" ht="15.75" customHeight="1">
-      <c r="A305" s="40"/>
+      <c r="A305" s="41"/>
     </row>
     <row r="306" ht="15.75" customHeight="1">
-      <c r="A306" s="40"/>
+      <c r="A306" s="41"/>
     </row>
     <row r="307" ht="15.75" customHeight="1">
-      <c r="A307" s="40"/>
+      <c r="A307" s="41"/>
     </row>
     <row r="308" ht="15.75" customHeight="1">
-      <c r="A308" s="40"/>
+      <c r="A308" s="41"/>
     </row>
     <row r="309" ht="15.75" customHeight="1">
-      <c r="A309" s="40"/>
+      <c r="A309" s="41"/>
     </row>
     <row r="310" ht="15.75" customHeight="1">
-      <c r="A310" s="40"/>
+      <c r="A310" s="41"/>
     </row>
     <row r="311" ht="15.75" customHeight="1">
-      <c r="A311" s="40"/>
+      <c r="A311" s="41"/>
     </row>
     <row r="312" ht="15.75" customHeight="1">
-      <c r="A312" s="40"/>
+      <c r="A312" s="41"/>
     </row>
     <row r="313" ht="15.75" customHeight="1">
-      <c r="A313" s="40"/>
+      <c r="A313" s="41"/>
     </row>
     <row r="314" ht="15.75" customHeight="1">
-      <c r="A314" s="40"/>
+      <c r="A314" s="41"/>
     </row>
     <row r="315" ht="15.75" customHeight="1">
       <c r="A315" s="7"/>

</xml_diff>

<commit_message>
fix translate and add dropdown list
</commit_message>
<xml_diff>
--- a/translation.xlsx
+++ b/translation.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="280">
   <si>
     <t>English</t>
   </si>
@@ -931,6 +931,12 @@
   </si>
   <si>
     <t>Đăng xuất</t>
+  </si>
+  <si>
+    <t>SIGN IN</t>
+  </si>
+  <si>
+    <t>ĐĂNG NHẬP</t>
   </si>
 </sst>
 </file>
@@ -2692,7 +2698,12 @@
       </c>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="41"/>
+      <c r="A141" s="40" t="s">
+        <v>278</v>
+      </c>
+      <c r="B141" s="39" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="142" ht="15.75" customHeight="1">
       <c r="A142" s="41"/>

</xml_diff>

<commit_message>
fix excel formula and content
</commit_message>
<xml_diff>
--- a/translation.xlsx
+++ b/translation.xlsx
@@ -4,42 +4,20 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="nháp" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhr1DePOx5RSD6YsuSwLpgwB31ytg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7miTPNpMNQV1ZWlKghNOSpSf8Lo/ug=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="B67">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAMi1MQJs
-Dự Nguyễn Chiếm    (2021-06-21 14:26:01)
-chị vy ơi chỗ này bị sót ạ, chị dịch lại giúp em</t>
-      </text>
-    </comment>
-  </commentList>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mi49WZTwwXvKJfEd4VaJ3FpVfUNMQ=="/>
-    </ext>
-  </extLst>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="293">
   <si>
     <t>English</t>
   </si>
@@ -221,7 +199,7 @@
     <t>Ý KIẾN CỦA BẠN</t>
   </si>
   <si>
-    <t>Active Ageing Vietnam was established to deal with an issue that Vietnam and other ASEAN countries would face in the near future, ageing population and its consequences. . We believe that companionship by each individual to improve their initiative in financial management and health protection will create positive effects for the community, contributing to creating a more sustainable future</t>
+    <t>Active Ageing Vietnam was established to deal with an issue that Vietnam and other ASEAN countries would face in the near future, ageing population and its consequences. We believe that companionship by each individual to improve their initiative in financial management and health protection will create positive effects for the community, contributing to creating a more sustainable future</t>
   </si>
   <si>
     <t>Dự án Active Ageing được ra đời với nỗi trăn trở về một vấn đề mà Việt Nam và các nước trong khu vực đang và sẽ phải đối mặt trong tương lai gần, đó chính là già hoá dân số và những hệ luỵ có liên quan. Chúng tôi tin rằng việc đồng hành cùng mỗi cá nhân nâng cao sự chủ động trong quản lý tài chính và bảo vệ sức khoẻ sẽ tạo ra những ảnh hưởng tích cực cho cộng đồng, góp phần kiến tạo một tương lai bền vững hơn.</t>
@@ -314,13 +292,13 @@
     <t>Social issues</t>
   </si>
   <si>
-    <t>According to the United Nations Department on Economic and Social Issues, the rate of population aging in Southeast Asian countries is now speedy. According to a report by the National Committee on The Elderly of Vietnam in 2019, about 1 in 5 Vietnamese will be 60 years of age or older by 2035, making Vietnam one of only three ASEAN countries with an elderly rate of over 20%.</t>
+    <t>According to the United Nations Department on Economic and Social Issues, the rate of population aging in Southeast Asian countries is speedy. According to a report by the National Committee on The Elderly of Vietnam in 2019, about 1 in 5 Vietnamese will be 60 years of age or older by 2035, making Vietnam one of only three ASEAN countries with an elderly rate of over 20%.</t>
   </si>
   <si>
     <t>Theo Vụ Liên Hiệp Quốc về vấn đề Kinh tế và Xã hội, tốc độ già hoá dân số tại các quốc gia Đông Nam Á hiện nay rất nhanh. Theo báo cáo năm 2019 của Ủy ban Quốc gia về Người cao tuổi Việt Nam, khoảng 1/5 người Việt Nam sẽ từ 60 tuổi trở lên vào năm 2035, đưa Việt Nam trở thành một trong ba nước ASEAN duy nhất có tỷ lệ người cao tuổi trên 20%.</t>
   </si>
   <si>
-    <t>In that situation, the preparation for the ageing of the population is exceptionally urgent. If people do not grasp the golden period right now, in the next 15 years, Vietnam will fall into the middle-income trap, and people will be increasingly at risk of "getting old before getting rich".</t>
+    <t>In that situation, the preparation for the ageing of the population is exceptionally urgent. If people do not grasp the golden period right now, in the next 15 years, Vietnam will fall into the middle-income trap, and the country's socio-economic horizon will face the risk of "getting old before getting rich".</t>
   </si>
   <si>
     <t>Trước thực tế đó, sự chuẩn bị cho giai đoạn già hoá dân số là vô cùng cấp thiết. Nếu không nắm bắt được giai đoạn vàng lúc này, 15 năm tới, Việt Nam sẽ rơi vào bẫy thu nhập trung bình và người dân sẽ ngày càng có nguy cơ “già trước khi giàu”.</t>
@@ -332,7 +310,7 @@
     <t>“Getting old before getting rich” - khái niệm vĩ mô, tác động cá nhân.</t>
   </si>
   <si>
-    <t>The report "Vietnam as an Ageing Society" recently explained that up to 16% of Vietnamese aged over 60 fall into poverty. Meanwhile, only 23.5% of people over 60 are entitled to receive a monthly pension or social insurance benefit. The income of the elderly after retirement depends heavily on their family. The traditional family model of many generations living under the same roof is gradually shifting to the nuclear family model. At that time, the elderly had to live alone, away from their children. In addition, the health care system is limited in Vietnam, along with the increasing health care cost has negatively affected the living standard after the retirement of the elderly</t>
+    <t>The report "Vietnam as an Ageing Society" recently indicated that up to 16% of Vietnamese aged over 60 fall into poverty. Meanwhile, only 23.5% of people over 60 are entitled to receive a monthly pension or social insurance benefit. The income of the elderly after retirement depends heavily on their family. The traditional family model of many generations living under the same roof is gradually shifting to the nuclear family model. At that time, the elderly had to live alone, away from their children. In addition, the health care system is limited in Vietnam, along with the increasing health care cost and its negative effects on the post-retirement living standard of the elderly</t>
   </si>
   <si>
     <t>Báo cáo “Vietnam as an Ageing Society” mới đây đã chỉ ra rằng có đến 16% người Việt Nam trên 60 tuổi rơi vào nhóm nghèo. Trong khi đó, chỉ có 23,5% người trên 60 tuổi được hưởng lương hưu hoặc trợ cấp bảo hiểm xã hội hàng tháng. Thu nhập của người cao tuổi sau về hưu phụ thuộc lớn vào trợ cấp từ con cái. Mô hình gia đình truyền thống nhiều thế hệ cùng chung sống dưới một mái nhà đang chuyển dần sang mô hình gia đình hạt nhân. Khi đó, người cao tuổi phải sống xa con cái và có khả năng sống một mình. Ngoài ra, hệ thống chăm sóc sức khỏe còn hạn chế ở Việt Nam, cùng với chi phí khám chữa bệnh ngày càng tăng đã ảnh hưởng tiêu cực đến sự hưởng thụ sau khi về hưu của người cao tuổi.</t>
@@ -362,16 +340,16 @@
     <t>Nếu không có thái độ tích cực chuẩn bị cho độ tuổi trên 60, người cao tuổi sẽ phải đối mặt với những hậu quả nghiêm trọng như hạn chế tài chính và hạn chế tiếp cận các dịch vụ chăm sóc sức khỏe.</t>
   </si>
   <si>
-    <t>"These problems will be exacerbated when the number of elderly people will increase in the next 15 years"</t>
-  </si>
-  <si>
-    <t>"Những vấn đề trên sẽ trở nên càng trầm trọng hơn khi 15 năm tới đây, số người cao tuổi sẽ tăng"</t>
-  </si>
-  <si>
-    <t>Seeing these problems will be exacerbated when in the next 15 years, the number of older people will increase and account for more than a fifth of the population. Active Ageing Vietnam wishes to resonate with existing changes to help each person be better prepared for old age sooner. Along with the Government's policy changes, Active Ageing is an optimal solution in doing so.</t>
-  </si>
-  <si>
-    <t>Nhìn thấy những vấn đề trên sẽ trở nên càng trầm trọng hơn khi 15 năm tới đây, số người cao tuổi sẽ tăng và chiếm hơn ⅕ dân số, Active Ageing Vietnam mong muốn có thể cộng hưởng đến những thay đổi hiện có để giúp mỗi người có sự chuẩn bị cho tuổi già tốt hơn, sớm hơn. Cùng với những thay đổi chính sách của Chính phủ, Active Ageing là một giải pháp tối ưu trong việc.</t>
+    <t>"These problems will be exacerbated as the number of elderly people increases in the next 15 years"</t>
+  </si>
+  <si>
+    <t>"Những vấn đề trên sẽ trở nên càng trầm trọng hơn trong 15 năm tới đây, khi số người cao tuổi sẽ gia tăng đáng kể"</t>
+  </si>
+  <si>
+    <t>In the next 15 years, the number of older people will speedily increase and account for more than a fifth of the population. Active Ageing Vietnam wishes to resonate with existing changes to help each person better prepare for their old age before actually becoming old. Along with the Government's policy changes, Active Ageing is an optimal solution for ageing population in Vietnam.</t>
+  </si>
+  <si>
+    <t>Nhận thấy những vấn đề trên sẽ trở nên càng trầm trọng hơn khi 15 năm tới đây, số người cao tuổi sẽ tăng và chiếm hơn ⅕ dân số, Active Ageing Vietnam mong muốn có thể cộng hưởng với những thay đổi hiện có để giúp mỗi người có sự chuẩn bị cho tuổi già tốt hơn, sớm hơn. Cùng với những thay đổi chính sách của Chính phủ, Active Ageing là một giải pháp tối ưu cho tình trạng già hóa dân số tại Việt Nam.</t>
   </si>
   <si>
     <r>
@@ -380,7 +358,7 @@
         <color rgb="FF000000"/>
         <sz val="11.0"/>
       </rPr>
-      <t>"It is crucial to develop a positive attitude</t>
+      <t>"It is crucial to build an active attitude</t>
     </r>
     <r>
       <rPr>
@@ -397,7 +375,7 @@
         <color rgb="FF000000"/>
         <sz val="11.0"/>
       </rPr>
-      <t>towards the preparation for financial safety and the access to healthcare system."</t>
+      <t>towards the preparation for financial safety and the access to healthcare."</t>
     </r>
   </si>
   <si>
@@ -407,7 +385,7 @@
     <t>Prepare for Vietnam as it will become an aging nation by 2035.</t>
   </si>
   <si>
-    <t>chuẩn bị cho một Việt Nam sẽ là một quốc gia có già hóa dân số vào năm 2035.</t>
+    <t>Chuẩn bị cho Việt Nam - quốc gia được dự đoán sẽ bước vào thời kỳ dân số già vào năm 2035.</t>
   </si>
   <si>
     <t>In the early stages, our target audience is middle-income workers at least 15 years before retirement.</t>
@@ -458,25 +436,37 @@
     <t>Thu nhập hàng năm của hộ gia đình hiện tại (triệu VNĐ)</t>
   </si>
   <si>
-    <t>Số dư tài khoản tiết kiệm về hưu hiện tại của bạn.</t>
+    <t>Your current retirement savings account balance. Assuming you have accumulated 700 mil VND for your retirement savings, please enter '700'.</t>
+  </si>
+  <si>
+    <t>Số dư tài khoản tiết kiệm về hưu hiện tại của bạn. Giả sử bạn đã tích góp được 700 triệu VNĐ cho quỹ tiết kiệm hưu trí của mình, vui lòng nhập '700'.</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
   <si>
     <t>Current retirement savings balance (mil VND)</t>
   </si>
   <si>
-    <t>Số dư khoản tiết kiệm về hưu hiện tại (triệu VNĐ)</t>
-  </si>
-  <si>
-    <t>Percentage of annual income will be contributed to your retirement savings fund each year (%)</t>
+    <t>Số dư quỹ tiết kiệm hưu trí hiện tại (triệu VNĐ)</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Percentage of annual income to be contributed to your retirement savings fund each year (%)</t>
   </si>
   <si>
     <t>Phần trăm thu nhập hằng năm đóng góp vào quỹ tiết kiệm về hưu (%)</t>
   </si>
   <si>
-    <t>Annual retirement savings (As a percentage of income)</t>
-  </si>
-  <si>
-    <t>Khoản tiết kiệm về hưu hàng năm (Theo phần trăm thu nhập)</t>
+    <t>cái này xoá luôn ha chị</t>
+  </si>
+  <si>
+    <t>Annual retirement savings as a percentage of income (%)</t>
+  </si>
+  <si>
+    <t>Khoản tiết kiệm về hưu hàng năm tính theo phần trăm thu nhập (%)</t>
   </si>
   <si>
     <t>Expected annual income growth rate (%)</t>
@@ -509,16 +499,19 @@
     <t>Lợi suất ước tính trong quá trình về hưu (%)</t>
   </si>
   <si>
-    <t>Pension/Other Post-Retirement Income</t>
-  </si>
-  <si>
-    <t>Lương hưu và thu nhập sau về hưu khác</t>
-  </si>
-  <si>
-    <t>Expected inflation rate (%)</t>
-  </si>
-  <si>
-    <t>Mức lạm phát dự đoán (%)</t>
+    <t>Pension/Other Post-Retirement Income (mil VND)</t>
+  </si>
+  <si>
+    <t>Lương hưu và thu nhập sau về hưu khác (triệu VNĐ)</t>
+  </si>
+  <si>
+    <t>Expected inflation rate (Default 3.5%)</t>
+  </si>
+  <si>
+    <t>Mức lạm phát dự đoán (Mặc định 3.5%)</t>
+  </si>
+  <si>
+    <t>mặc định 3.5%</t>
   </si>
   <si>
     <t>Basic Information</t>
@@ -569,16 +562,16 @@
     <t>Độ tuổi bạn dự định nghỉ hưu, giả định rằng bạn không đóng góp thêm vào quỹ tiết kiệm hưu trí của mình trong năm này. Ví dụ, nếu bạn nghỉ hưu ở tuổi 60, vui lòng nhập '60'. Trong trường hợp này, khoản đóng góp cuối cùng của bạn xảy ra khi bạn 59 tuổi. Chúng tôi cũng giả định rằng bạn thực hiện toàn bộ khoản đóng góp của mình vào cuối mỗi năm.</t>
   </si>
   <si>
-    <t>Your total income in the current year. If your income this year is 180,000,000 VND, please type '180'.</t>
-  </si>
-  <si>
-    <t>Tổng thu nhập của bạn trong năm hiện tại. Nếu thu nhập trong năm nay của bạn là 180.000.000 VND, vui lòng nhập '180'.</t>
-  </si>
-  <si>
-    <t>Percentage of annual income will be contributed to your retirement savings fund each year. So if your annual income is 180,000,000 VND and your annual retirement savings is 8%, kindly insert '8'. In this case, this year contribution equals 180,000,000 x 8% = 14,400,000 VND (or 14.4 mil VND)</t>
-  </si>
-  <si>
-    <t>Phần trăm thu nhập hàng năm sẽ được đóng góp vào quỹ tiết kiệm hưu trí của bạn mỗi năm. Nếu thu nhập hàng năm của bạn là 180,000,000 đồng và tiết kiệm hưu trí hàng năm của bạn là 8%, vui lòng nhập '8'. Như vậy, mức đóng góp hàng năm bằng 180,000,000 x 8% = 14,400,000 VNĐ (14.4 triệu VNĐ).</t>
+    <t>Your total income in the current year. If your income this year is 180 mil VND, please type '180'.</t>
+  </si>
+  <si>
+    <t>Tổng thu nhập của bạn trong năm hiện tại. Nếu thu nhập trong năm nay của bạn là 180 triệu VND, vui lòng nhập '180'.</t>
+  </si>
+  <si>
+    <t>Percentage of annual income to be contributed to your retirement savings fund each year. So if your annual income is 180 mil VND and your annual retirement savings is 8%, kindly insert '8'. In this case, this year contribution equals 180 x 8% = 14.4 mil VND</t>
+  </si>
+  <si>
+    <t>Phần trăm thu nhập hàng năm sẽ được đóng góp vào quỹ tiết kiệm hưu trí của bạn mỗi năm. Nếu thu nhập hàng năm của bạn là 180 triệu VNĐ và tỷ lệ đóng góp hàng năm của bạn là 8%, vui lòng nhập '8'. Như vậy, mức đóng góp hàng năm bằng 180 x 8% = 14.4 triệu VNĐ.</t>
   </si>
   <si>
     <t>Expected rate of income increase each year until your expected retirement year. For example, you may type '2' if you expects your income will increase by 2% on an annual basis.</t>
@@ -587,43 +580,43 @@
     <t>Tỷ lệ thu nhập ước tính tăng hàng năm cho đến năm nghỉ hưu dự kiến của bạn. Nếu bạn ước tính mức lương hàng năm của bạn sẽ tăng 2%, vui lòng nhập '2'</t>
   </si>
   <si>
-    <t>Total number of years you expect to live on your retirement savings fund. Assuming you plan to retire at age 60 and wish to maintain a comfortable standard of living for another 30 years thereafter by means of your Retirement Savings Fund, please enter "30". In other words, your expected lifespan in this case is 60 + 30 = 90.</t>
-  </si>
-  <si>
-    <t>Tổng số năm bạn dự định sử dụng quỹ tiết kiệm hưu trí của mình để chi tiêu kể từ năm bạn nghỉ hưu. Giả sử bạn dự định về hưu ở tuổi 60 và mong muốn duy trì mức sống thoải mái trong vòng 30 năm nữa nhờ Quỹ Tiết kiệm về Hưu của mình, vui lòng nhập "30". Nói cách khác, tuổi thọ dự kiến của bạn trong trường hợp này là 60 + 30 = 90 (tuổi).</t>
-  </si>
-  <si>
-    <t>The percentage of your post-retirement household income you think you will need to cover your expenses in retirement. This amount is based on the household income earned during your last working year (the year immediately before your retirement).</t>
-  </si>
-  <si>
-    <t>Tỷ lệ phần trăm thu nhập hộ gia đình sau khi nghỉ hưu mà bạn nghĩ rằng bạn sẽ cần để trang trải các chi phí của mình khi nghỉ hưu. Số tiền này dựa trên thu nhập hộ gia đình trong năm làm việc cuối cùng của bạn (năm ngay trước khi bạn nghỉ hưu).</t>
-  </si>
-  <si>
-    <t>nếu chị sửa ô nào bên cột tiếng việt thì chị bôi đỏ giúp em nha chị, để em sửa lại code ạ</t>
-  </si>
-  <si>
-    <t>Annual expected rate of return on your retirement savings fund before retirement</t>
-  </si>
-  <si>
-    <t>Tỷ suất lợi nhuận kỳ vọng hàng năm trên quỹ tiết kiệm hưu trí của bạn trước khi nghỉ hưu.</t>
-  </si>
-  <si>
-    <t>Annual expected rate of return on your retirement savings fund after retirement</t>
-  </si>
-  <si>
-    <t>Tỷ suất lợi nhuận kỳ vọng hàng năm trên quỹ tiết kiệm hưu trí của bạn sau khi nghỉ hưu</t>
-  </si>
-  <si>
-    <t>Your expected income from pensions or other sources (post-retirement)</t>
-  </si>
-  <si>
-    <t>Thu nhập dự kiến từ lương hưu hoặc các nguồn khác</t>
-  </si>
-  <si>
-    <t>In recent years, Vietnam inflation rate has ranged from 3% to 4%</t>
-  </si>
-  <si>
-    <t>Trong những năm gần đây, tỷ lệ lạm phát Việt Nam đang ở mức dao động từ 3%-4%</t>
+    <t>Total number of years you expect to live on your retirement savings fund. Assuming you plan to retire at age 60 and wish to maintain a comfortable standard of living for another 30 years thereafter by means of your retirement savings fund, please enter '30'. In other words, your expected lifespan in this case is 60 + 30 = 90.</t>
+  </si>
+  <si>
+    <t>Tổng số năm bạn dự định sử dụng quỹ tiết kiệm hưu trí của mình để chi tiêu kể từ năm bạn nghỉ hưu. Giả sử bạn dự định về hưu ở tuổi 60 và mong muốn duy trì mức sống thoải mái trong vòng 30 năm nữa nhờ quỹ tiết kiệm hưu trí của mình, vui lòng nhập '30'. Nói cách khác, tuổi thọ dự kiến của bạn trong trường hợp này là 60 + 30 = 90 (tuổi).</t>
+  </si>
+  <si>
+    <t>The percentage of your post-retirement household income you think you will need to cover your expenses in retirement. This amount is based on the household income earned during your last working year (the year immediately before your retirement). Assuming you plan to retire at age 60, your income at age 59 is 210mil VND, and you believe this rate is 60%, please enter '60'. Then, the amount you need to cover your expenditures at 60 equals 210 x 60% = 126 million VND.</t>
+  </si>
+  <si>
+    <t>Tỷ lệ phần trăm thu nhập hộ gia đình sau khi nghỉ hưu mà bạn nghĩ rằng bạn sẽ cần để trang trải các chi phí của mình khi nghỉ hưu. Số tiền này dựa trên thu nhập hộ gia đình trong năm làm việc cuối cùng của bạn (năm ngay trước khi bạn nghỉ hưu). Giả sử bạn dự định về hưu ở tuổi 60, thu nhập năm bạn 59 tuổi là 210 triệu VNĐ, và bạn tin rằng tỷ lệ này là 60%, vui lòng nhập '60'. Khi đó, số tiền mà bạn cần để chi tiêu vào năm 60 tuổi bằng 210 x 60% = 126 triệu VNĐ.</t>
+  </si>
+  <si>
+    <t>Annual expected rate of return on your retirement savings fund before retirement. Please be noted that this ratio tends to decrease over time. If you expectes this rate to be 7%, please type '7'.</t>
+  </si>
+  <si>
+    <t>Tỷ suất lợi nhuận kỳ vọng hàng năm trên quỹ tiết kiệm hưu trí của bạn trước khi nghỉ hưu. Lưu ý rằng tỷ lệ này có xu hướng giảm theo thời gian. Nếu bạn kỳ vọng tỷ suất trên là 7%, vui lòng nhập '7'.</t>
+  </si>
+  <si>
+    <t>Annual expected rate of return on your retirement savings fund after retirement. Please be noted that this ratio tends to decrease over time. If you expectes this rate to be 4%, please type '4'.</t>
+  </si>
+  <si>
+    <t>Tỷ suất lợi nhuận kỳ vọng hàng năm trên quỹ tiết kiệm hưu trí của bạn sau khi nghỉ hưu. Lưu ý rằng tỷ lệ này có xu hướng giảm theo thời gian. Nếu bạn kỳ vọng tỷ suất trên là 4%, vui lòng nhập '4'.</t>
+  </si>
+  <si>
+    <t>Your expected income from pensions or other sources (post-retirement). If you predict your pension to be 2 mil VND per month or 24 mil VND per year, please enter '24'.</t>
+  </si>
+  <si>
+    <t>Thu nhập dự kiến từ lương hưu hoặc các nguồn khác. Nếu bạn dự đoán mức lương hưu của mình là 2 triệu VNĐ mỗi tháng hay 24 triệu VNĐ mỗi năm, vui lòng nhập '24'.</t>
+  </si>
+  <si>
+    <t>The annual level of expenditure will be assumed to increase with the rate of inflation. In recent years, Vietnam inflation rate has ranged from 3% to 4%. Therefore, we assume this rate to be 3.5%.</t>
+  </si>
+  <si>
+    <t>Mức chi tiêu hàng năm sẽ được giả định tăng theo tỷ lệ lạm phát. Trong những năm gần đây, tỷ lệ lạm phát Việt Nam đang ở mức dao động từ 3%-4%. Vì vậy, chúng tôi giả định tỷ lệ này là 3.5%.</t>
+  </si>
+  <si>
+    <t>Vẫn hiển thị thành 1 ô như các ô khác duy nhất ô này ng dùng ko chỉnh được, mặc định 3.5%</t>
   </si>
   <si>
     <t xml:space="preserve">It’s </t>
@@ -650,10 +643,10 @@
     <t>% thu nhập năm cuối cùng trước khi về hưu của bạn sẽ được ước tính là chi tiêu hằng năm trong giai đoạn hưu trí của bạn tương ứng</t>
   </si>
   <si>
-    <t>VND. This value will increase subject to the inflation rate thereafter.</t>
-  </si>
-  <si>
-    <t>VND. Giá trị này sẽ tăng theo tỷ lệ lạm phát sau đó.</t>
+    <t>mil VND. This value will increase subject to the inflation rate thereafter.</t>
+  </si>
+  <si>
+    <t>triệu VNĐ. Giá trị này sẽ tăng theo tỷ lệ lạm phát sau đó.</t>
   </si>
   <si>
     <t>Your retirement savings plan is on track. Use the Manage Savings function to easily track and manage your progress!</t>
@@ -946,13 +939,19 @@
   </si>
   <si>
     <t>Khác</t>
+  </si>
+  <si>
+    <t>The annual level of expenditure will be assumed to increase with the rate of inflation. In recent years, Vietnam inflation rate has ranged from 3% to 4%. For instance, you may enter "3.5" If you think this rate is 3.5%.</t>
+  </si>
+  <si>
+    <t>Mức chi tiêu hàng năm sẽ được giả định tăng theo tỷ lệ lạm phát. Trong những năm gần đây, tỷ lệ lạm phát Việt Nam đang ở mức dao động từ 3%-4%. Nếu bạn cho rằng tỷ lệ này là 3.5%, vui lòng nhập "3.5".</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -978,14 +977,25 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font/>
+    <font>
+      <b/>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
     </font>
     <font>
-      <color theme="1"/>
+      <strike/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+    </font>
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -1047,8 +1057,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF00FF"/>
-        <bgColor rgb="FFFF00FF"/>
+        <fgColor rgb="FFE06666"/>
+        <bgColor rgb="FFE06666"/>
       </patternFill>
     </fill>
   </fills>
@@ -1064,7 +1074,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1089,98 +1099,104 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="0" fillId="7" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1192,6 +1208,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1404,7 +1424,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="61.13"/>
     <col customWidth="1" min="2" max="2" width="52.38"/>
-    <col customWidth="1" min="3" max="3" width="12.63"/>
+    <col customWidth="1" min="3" max="3" width="17.0"/>
     <col customWidth="1" min="4" max="4" width="21.25"/>
     <col customWidth="1" min="5" max="23" width="7.63"/>
   </cols>
@@ -1552,7 +1572,7 @@
       <c r="C15" s="9"/>
     </row>
     <row r="16">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1570,7 +1590,7 @@
       <c r="C17" s="9"/>
     </row>
     <row r="18">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1579,7 +1599,7 @@
       <c r="C18" s="9"/>
     </row>
     <row r="19">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1671,7 +1691,7 @@
       <c r="C28" s="9"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1752,7 +1772,7 @@
       <c r="C37" s="9"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -1761,7 +1781,7 @@
       <c r="C38" s="9"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="11" t="s">
         <v>76</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -1770,7 +1790,7 @@
       <c r="C39" s="9"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="11" t="s">
         <v>78</v>
       </c>
       <c r="B40" s="5" t="s">
@@ -1788,7 +1808,7 @@
       <c r="C41" s="9"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="11" t="s">
         <v>82</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1831,29 +1851,29 @@
         <v>9</v>
       </c>
       <c r="C46" s="6"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="13"/>
-      <c r="O46" s="13"/>
-      <c r="P46" s="13"/>
-      <c r="Q46" s="13"/>
-      <c r="R46" s="13"/>
-      <c r="S46" s="13"/>
-      <c r="T46" s="13"/>
-      <c r="U46" s="13"/>
-      <c r="V46" s="13"/>
-      <c r="W46" s="13"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+      <c r="O46" s="12"/>
+      <c r="P46" s="12"/>
+      <c r="Q46" s="12"/>
+      <c r="R46" s="12"/>
+      <c r="S46" s="12"/>
+      <c r="T46" s="12"/>
+      <c r="U46" s="12"/>
+      <c r="V46" s="12"/>
+      <c r="W46" s="12"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="11" t="s">
         <v>91</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -1862,7 +1882,7 @@
       <c r="C47" s="9"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="11" t="s">
         <v>93</v>
       </c>
       <c r="B48" s="5" t="s">
@@ -1880,7 +1900,7 @@
       <c r="C49" s="9"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="11" t="s">
         <v>97</v>
       </c>
       <c r="B50" s="7" t="s">
@@ -1907,7 +1927,7 @@
       <c r="C52" s="9"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="13" t="s">
         <v>103</v>
       </c>
       <c r="B53" s="5" t="s">
@@ -1916,7 +1936,7 @@
       <c r="C53" s="9"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="13" t="s">
         <v>105</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -1928,7 +1948,7 @@
       <c r="A55" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="11" t="s">
         <v>108</v>
       </c>
       <c r="C55" s="9"/>
@@ -1937,13 +1957,13 @@
       <c r="A56" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="11" t="s">
         <v>110</v>
       </c>
       <c r="C56" s="9"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="14" t="s">
         <v>111</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -1952,16 +1972,16 @@
       <c r="C57" s="9"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="16" t="s">
+      <c r="A58" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="11" t="s">
         <v>114</v>
       </c>
       <c r="C58" s="9"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="14" t="s">
+      <c r="A59" s="13" t="s">
         <v>115</v>
       </c>
       <c r="B59" s="5" t="s">
@@ -1970,7 +1990,7 @@
       <c r="C59" s="9"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="14" t="s">
+      <c r="A60" s="13" t="s">
         <v>117</v>
       </c>
       <c r="B60" s="5" t="s">
@@ -1979,7 +1999,7 @@
       <c r="C60" s="9"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="14" t="s">
+      <c r="A61" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -1988,7 +2008,7 @@
       <c r="C61" s="9"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="14" t="s">
+      <c r="A62" s="13" t="s">
         <v>121</v>
       </c>
       <c r="B62" s="5" t="s">
@@ -1997,7 +2017,7 @@
       <c r="C62" s="9"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="14" t="s">
+      <c r="A63" s="13" t="s">
         <v>123</v>
       </c>
       <c r="B63" s="5" t="s">
@@ -2006,486 +2026,525 @@
       <c r="C63" s="9"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="14" t="s">
+      <c r="A64" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="16" t="s">
         <v>126</v>
       </c>
       <c r="C64" s="9"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="14" t="s">
+      <c r="A65" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="16" t="s">
         <v>128</v>
       </c>
       <c r="C65" s="9"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="18" t="s">
+      <c r="A66" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="B66" s="19" t="s">
+      <c r="B66" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C66" s="9"/>
+      <c r="C66" s="18"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="20"/>
-      <c r="B67" s="19" t="s">
+      <c r="A67" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="C67" s="9"/>
+      <c r="B67" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="B68" s="19" t="s">
+      <c r="A68" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="69" ht="15.75" customHeight="1">
+      <c r="A69" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B69" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" ht="15.75" customHeight="1">
+      <c r="A70" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="C70" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="C68" s="9"/>
-    </row>
-    <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B69" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="C69" s="9"/>
-    </row>
-    <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B70" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="C70" s="9"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C71" s="9"/>
+      <c r="A71" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B71" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>141</v>
+        <v>144</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>145</v>
       </c>
       <c r="C72" s="9"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>143</v>
+        <v>146</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>147</v>
       </c>
       <c r="C73" s="9"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B74" s="17" t="s">
-        <v>145</v>
+        <v>148</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>149</v>
       </c>
       <c r="C74" s="9"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>147</v>
+        <v>150</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>151</v>
       </c>
       <c r="C75" s="9"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="5" t="s">
-        <v>148</v>
+      <c r="A76" s="11" t="s">
+        <v>152</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="C76" s="9"/>
+        <v>153</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C77" s="9"/>
+      <c r="A77" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C78" s="9"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="B79" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="C79" s="25"/>
-      <c r="D79" s="26"/>
+      <c r="A79" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C79" s="29"/>
+      <c r="D79" s="30"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="14" t="s">
-        <v>156</v>
+      <c r="A80" s="13" t="s">
+        <v>161</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C80" s="9"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="B81" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="C81" s="29"/>
+      <c r="A81" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B81" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C81" s="18" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="B82" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="C82" s="9"/>
+      <c r="A82" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="B83" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="C83" s="9"/>
+      <c r="A83" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="B83" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="B84" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="C84" s="9"/>
+      <c r="A84" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="C84" s="18" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="B85" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="C85" s="9"/>
+      <c r="A85" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="B85" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="B86" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="C86" s="30" t="s">
-        <v>170</v>
+      <c r="A86" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="B86" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C86" s="18" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C87" s="9"/>
+      <c r="A87" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="B87" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="C87" s="18" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C88" s="9"/>
+      <c r="A88" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="B88" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="C89" s="9"/>
+      <c r="A89" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="B89" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C90" s="9"/>
+      <c r="A90" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="B90" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="C90" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="D90" s="32" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="16" t="s">
-        <v>179</v>
+      <c r="A91" s="15" t="s">
+        <v>184</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C91" s="9"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="14" t="s">
-        <v>181</v>
+      <c r="A92" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C92" s="9"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="14" t="s">
-        <v>183</v>
+      <c r="A93" s="13" t="s">
+        <v>188</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C93" s="9"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="14" t="s">
-        <v>185</v>
+      <c r="A94" s="13" t="s">
+        <v>190</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C94" s="9"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C95" s="9"/>
+      <c r="A95" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="B95" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="C95" s="18" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="96" ht="67.5" customHeight="1">
-      <c r="A96" s="31" t="s">
-        <v>189</v>
+      <c r="A96" s="33" t="s">
+        <v>194</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C96" s="9"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="14" t="s">
-        <v>191</v>
+      <c r="A97" s="13" t="s">
+        <v>196</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C97" s="9"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="14" t="s">
-        <v>193</v>
+      <c r="A98" s="13" t="s">
+        <v>198</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C98" s="9"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="14" t="s">
-        <v>195</v>
+      <c r="A99" s="13" t="s">
+        <v>200</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="C99" s="9"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="B100" s="24" t="s">
-        <v>198</v>
+      <c r="A100" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>203</v>
       </c>
       <c r="C100" s="9"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="B101" s="24" t="s">
-        <v>200</v>
+      <c r="A101" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>205</v>
       </c>
       <c r="C101" s="9"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="B102" s="24" t="s">
-        <v>202</v>
+      <c r="A102" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>207</v>
       </c>
       <c r="C102" s="9"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="B103" s="24" t="s">
-        <v>204</v>
+      <c r="A103" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>209</v>
       </c>
       <c r="C103" s="9"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="B104" s="24" t="s">
-        <v>206</v>
+      <c r="A104" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>211</v>
       </c>
       <c r="C104" s="9"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="14" t="s">
-        <v>207</v>
+      <c r="A105" s="13" t="s">
+        <v>212</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="C105" s="9"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="14" t="s">
-        <v>209</v>
+      <c r="A106" s="13" t="s">
+        <v>214</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C106" s="9"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="14" t="s">
-        <v>211</v>
+      <c r="A107" s="13" t="s">
+        <v>216</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C107" s="9"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="B108" s="32" t="s">
-        <v>214</v>
+      <c r="A108" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="B108" s="34" t="s">
+        <v>219</v>
       </c>
       <c r="C108" s="9"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="14" t="s">
-        <v>215</v>
+      <c r="A109" s="13" t="s">
+        <v>220</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C109" s="9"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="14" t="s">
-        <v>217</v>
+      <c r="A110" s="13" t="s">
+        <v>222</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="C110" s="9"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="14" t="s">
-        <v>219</v>
+      <c r="A111" s="13" t="s">
+        <v>224</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C111" s="9"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="14" t="s">
-        <v>221</v>
+      <c r="A112" s="13" t="s">
+        <v>226</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="C112" s="9"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="14" t="s">
-        <v>223</v>
+      <c r="A113" s="13" t="s">
+        <v>228</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C113" s="9"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="14" t="s">
-        <v>225</v>
+      <c r="A114" s="13" t="s">
+        <v>230</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="C114" s="9"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="14" t="s">
-        <v>227</v>
+      <c r="A115" s="13" t="s">
+        <v>232</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="C115" s="9"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="33" t="s">
-        <v>229</v>
+      <c r="A116" s="35" t="s">
+        <v>234</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C116" s="9"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="11" t="s">
-        <v>231</v>
+      <c r="A117" s="25" t="s">
+        <v>236</v>
       </c>
       <c r="B117" s="7" t="s">
         <v>15</v>
@@ -2493,744 +2552,744 @@
       <c r="C117" s="9"/>
     </row>
     <row r="118" ht="90.0" customHeight="1">
-      <c r="A118" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="B118" s="14" t="s">
-        <v>233</v>
+      <c r="A118" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="B118" s="13" t="s">
+        <v>238</v>
       </c>
       <c r="C118" s="9"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="B119" s="14" t="s">
-        <v>235</v>
+      <c r="A119" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="B119" s="13" t="s">
+        <v>240</v>
       </c>
       <c r="C119" s="9"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="B120" s="14" t="s">
-        <v>237</v>
+      <c r="A120" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="B120" s="13" t="s">
+        <v>242</v>
       </c>
       <c r="C120" s="9"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="B121" s="14" t="s">
-        <v>239</v>
+      <c r="A121" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="B121" s="13" t="s">
+        <v>244</v>
       </c>
       <c r="C121" s="9"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="B122" s="14" t="s">
-        <v>241</v>
+      <c r="A122" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="B122" s="13" t="s">
+        <v>246</v>
       </c>
       <c r="C122" s="9"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="B123" s="14" t="s">
-        <v>243</v>
+      <c r="A123" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="B123" s="13" t="s">
+        <v>248</v>
       </c>
       <c r="C123" s="9"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="B124" s="14" t="s">
-        <v>245</v>
+      <c r="A124" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="B124" s="13" t="s">
+        <v>250</v>
       </c>
       <c r="C124" s="9"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="B125" s="14" t="s">
-        <v>247</v>
+      <c r="A125" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="B125" s="13" t="s">
+        <v>252</v>
       </c>
       <c r="C125" s="9"/>
     </row>
     <row r="126" ht="82.5" customHeight="1">
-      <c r="A126" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="B126" s="14" t="s">
-        <v>249</v>
+      <c r="A126" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="B126" s="13" t="s">
+        <v>254</v>
       </c>
       <c r="C126" s="9"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="B127" s="14" t="s">
-        <v>251</v>
+      <c r="A127" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="B127" s="13" t="s">
+        <v>256</v>
       </c>
       <c r="C127" s="9"/>
     </row>
     <row r="128" ht="17.25" customHeight="1">
-      <c r="A128" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="B128" s="14" t="s">
-        <v>253</v>
+      <c r="A128" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="B128" s="13" t="s">
+        <v>258</v>
       </c>
       <c r="C128" s="9"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="34" t="s">
-        <v>254</v>
-      </c>
-      <c r="B129" s="35" t="s">
-        <v>255</v>
+      <c r="A129" s="36" t="s">
+        <v>259</v>
+      </c>
+      <c r="B129" s="37" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="B130" s="35" t="s">
-        <v>257</v>
+      <c r="A130" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="B130" s="37" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="34" t="s">
-        <v>258</v>
-      </c>
-      <c r="B131" s="35" t="s">
-        <v>259</v>
+      <c r="A131" s="36" t="s">
+        <v>263</v>
+      </c>
+      <c r="B131" s="37" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="132" ht="16.5" customHeight="1">
-      <c r="A132" s="34" t="s">
-        <v>260</v>
-      </c>
-      <c r="B132" s="35" t="s">
-        <v>261</v>
+      <c r="A132" s="36" t="s">
+        <v>265</v>
+      </c>
+      <c r="B132" s="37" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="34" t="s">
-        <v>262</v>
-      </c>
-      <c r="B133" s="35" t="s">
-        <v>263</v>
+      <c r="A133" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="B133" s="37" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="34" t="s">
-        <v>264</v>
-      </c>
-      <c r="B134" s="37" t="s">
-        <v>265</v>
+      <c r="A134" s="36" t="s">
+        <v>269</v>
+      </c>
+      <c r="B134" s="32" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="38" t="s">
-        <v>266</v>
-      </c>
-      <c r="B135" s="37" t="s">
-        <v>267</v>
+      <c r="A135" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="B135" s="32" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="38" t="s">
-        <v>268</v>
-      </c>
-      <c r="B136" s="37" t="s">
-        <v>269</v>
+      <c r="A136" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="B136" s="32" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="137" ht="39.75" customHeight="1">
-      <c r="A137" s="38" t="s">
-        <v>270</v>
-      </c>
-      <c r="B137" s="30" t="s">
-        <v>271</v>
+      <c r="A137" s="39" t="s">
+        <v>275</v>
+      </c>
+      <c r="B137" s="40" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="38" t="s">
-        <v>272</v>
-      </c>
-      <c r="B138" s="37" t="s">
-        <v>273</v>
+      <c r="A138" s="39" t="s">
+        <v>277</v>
+      </c>
+      <c r="B138" s="32" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="38" t="s">
-        <v>274</v>
-      </c>
-      <c r="B139" s="37" t="s">
-        <v>275</v>
+      <c r="A139" s="39" t="s">
+        <v>279</v>
+      </c>
+      <c r="B139" s="32" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="38" t="s">
-        <v>276</v>
-      </c>
-      <c r="B140" s="37" t="s">
-        <v>277</v>
+      <c r="A140" s="39" t="s">
+        <v>281</v>
+      </c>
+      <c r="B140" s="32" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="38" t="s">
-        <v>278</v>
-      </c>
-      <c r="B141" s="37" t="s">
-        <v>279</v>
+      <c r="A141" s="39" t="s">
+        <v>283</v>
+      </c>
+      <c r="B141" s="32" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="B142" s="37" t="s">
-        <v>281</v>
+      <c r="A142" s="39" t="s">
+        <v>285</v>
+      </c>
+      <c r="B142" s="32" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="38" t="s">
-        <v>282</v>
-      </c>
-      <c r="B143" s="37" t="s">
-        <v>283</v>
+      <c r="A143" s="39" t="s">
+        <v>287</v>
+      </c>
+      <c r="B143" s="32" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="A144" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="B144" s="37" t="s">
-        <v>285</v>
+      <c r="A144" s="39" t="s">
+        <v>289</v>
+      </c>
+      <c r="B144" s="32" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="39"/>
+      <c r="A145" s="41"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="39"/>
+      <c r="A146" s="41"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="39"/>
+      <c r="A147" s="41"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="A148" s="39"/>
+      <c r="A148" s="41"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="A149" s="39"/>
+      <c r="A149" s="41"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="A150" s="39"/>
+      <c r="A150" s="41"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="A151" s="39"/>
+      <c r="A151" s="41"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="A152" s="39"/>
+      <c r="A152" s="41"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="A153" s="39"/>
+      <c r="A153" s="41"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="A154" s="39"/>
+      <c r="A154" s="41"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="39"/>
+      <c r="A155" s="41"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="A156" s="39"/>
+      <c r="A156" s="41"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="A157" s="39"/>
+      <c r="A157" s="41"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="A158" s="39"/>
+      <c r="A158" s="41"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="A159" s="39"/>
+      <c r="A159" s="41"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="39"/>
+      <c r="A160" s="41"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="A161" s="39"/>
+      <c r="A161" s="41"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="A162" s="39"/>
+      <c r="A162" s="41"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="A163" s="39"/>
+      <c r="A163" s="41"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="A164" s="39"/>
+      <c r="A164" s="41"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="39"/>
+      <c r="A165" s="41"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="A166" s="39"/>
+      <c r="A166" s="41"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="A167" s="39"/>
+      <c r="A167" s="41"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="A168" s="39"/>
+      <c r="A168" s="41"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="A169" s="39"/>
+      <c r="A169" s="41"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="A170" s="39"/>
+      <c r="A170" s="41"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="A171" s="39"/>
+      <c r="A171" s="41"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="39"/>
+      <c r="A172" s="41"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="A173" s="39"/>
+      <c r="A173" s="41"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="A174" s="39"/>
+      <c r="A174" s="41"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="A175" s="39"/>
+      <c r="A175" s="41"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="A176" s="39"/>
+      <c r="A176" s="41"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="A177" s="39"/>
+      <c r="A177" s="41"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="A178" s="39"/>
+      <c r="A178" s="41"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="A179" s="39"/>
+      <c r="A179" s="41"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="A180" s="39"/>
+      <c r="A180" s="41"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="A181" s="39"/>
+      <c r="A181" s="41"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="A182" s="39"/>
+      <c r="A182" s="41"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="A183" s="39"/>
+      <c r="A183" s="41"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="A184" s="39"/>
+      <c r="A184" s="41"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="A185" s="39"/>
+      <c r="A185" s="41"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="A186" s="39"/>
+      <c r="A186" s="41"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="A187" s="39"/>
+      <c r="A187" s="41"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="A188" s="39"/>
+      <c r="A188" s="41"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="A189" s="39"/>
+      <c r="A189" s="41"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="A190" s="39"/>
+      <c r="A190" s="41"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="A191" s="39"/>
+      <c r="A191" s="41"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="A192" s="39"/>
+      <c r="A192" s="41"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="A193" s="39"/>
+      <c r="A193" s="41"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="A194" s="39"/>
+      <c r="A194" s="41"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="A195" s="39"/>
+      <c r="A195" s="41"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="A196" s="39"/>
+      <c r="A196" s="41"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="A197" s="39"/>
+      <c r="A197" s="41"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="A198" s="39"/>
+      <c r="A198" s="41"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="A199" s="39"/>
+      <c r="A199" s="41"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="A200" s="39"/>
+      <c r="A200" s="41"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="A201" s="39"/>
+      <c r="A201" s="41"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="A202" s="39"/>
+      <c r="A202" s="41"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="A203" s="39"/>
+      <c r="A203" s="41"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="A204" s="39"/>
+      <c r="A204" s="41"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="A205" s="39"/>
+      <c r="A205" s="41"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="A206" s="39"/>
+      <c r="A206" s="41"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="A207" s="39"/>
+      <c r="A207" s="41"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="A208" s="39"/>
+      <c r="A208" s="41"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="A209" s="39"/>
+      <c r="A209" s="41"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="A210" s="39"/>
+      <c r="A210" s="41"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="A211" s="39"/>
+      <c r="A211" s="41"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="A212" s="39"/>
+      <c r="A212" s="41"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="A213" s="39"/>
+      <c r="A213" s="41"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="A214" s="39"/>
+      <c r="A214" s="41"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="A215" s="39"/>
+      <c r="A215" s="41"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="A216" s="39"/>
+      <c r="A216" s="41"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="A217" s="39"/>
+      <c r="A217" s="41"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="A218" s="39"/>
+      <c r="A218" s="41"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="A219" s="39"/>
+      <c r="A219" s="41"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="A220" s="39"/>
+      <c r="A220" s="41"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="A221" s="39"/>
+      <c r="A221" s="41"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="A222" s="39"/>
+      <c r="A222" s="41"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="A223" s="39"/>
+      <c r="A223" s="41"/>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="A224" s="39"/>
+      <c r="A224" s="41"/>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="A225" s="39"/>
+      <c r="A225" s="41"/>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="A226" s="39"/>
+      <c r="A226" s="41"/>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="A227" s="39"/>
+      <c r="A227" s="41"/>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="A228" s="39"/>
+      <c r="A228" s="41"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="A229" s="39"/>
+      <c r="A229" s="41"/>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="A230" s="39"/>
+      <c r="A230" s="41"/>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="A231" s="39"/>
+      <c r="A231" s="41"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="A232" s="39"/>
+      <c r="A232" s="41"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
-      <c r="A233" s="39"/>
+      <c r="A233" s="41"/>
     </row>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="A234" s="39"/>
+      <c r="A234" s="41"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="A235" s="39"/>
+      <c r="A235" s="41"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="A236" s="39"/>
+      <c r="A236" s="41"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="A237" s="39"/>
+      <c r="A237" s="41"/>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="A238" s="39"/>
+      <c r="A238" s="41"/>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="A239" s="39"/>
+      <c r="A239" s="41"/>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="A240" s="39"/>
+      <c r="A240" s="41"/>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="A241" s="39"/>
+      <c r="A241" s="41"/>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="A242" s="39"/>
+      <c r="A242" s="41"/>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="A243" s="39"/>
+      <c r="A243" s="41"/>
     </row>
     <row r="244" ht="15.75" customHeight="1">
-      <c r="A244" s="39"/>
+      <c r="A244" s="41"/>
     </row>
     <row r="245" ht="15.75" customHeight="1">
-      <c r="A245" s="39"/>
+      <c r="A245" s="41"/>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="A246" s="39"/>
+      <c r="A246" s="41"/>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="A247" s="39"/>
+      <c r="A247" s="41"/>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="A248" s="39"/>
+      <c r="A248" s="41"/>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="A249" s="39"/>
+      <c r="A249" s="41"/>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="A250" s="39"/>
+      <c r="A250" s="41"/>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="A251" s="39"/>
+      <c r="A251" s="41"/>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="A252" s="39"/>
+      <c r="A252" s="41"/>
     </row>
     <row r="253" ht="15.75" customHeight="1">
-      <c r="A253" s="39"/>
+      <c r="A253" s="41"/>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="A254" s="39"/>
+      <c r="A254" s="41"/>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="A255" s="39"/>
+      <c r="A255" s="41"/>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="A256" s="39"/>
+      <c r="A256" s="41"/>
     </row>
     <row r="257" ht="15.75" customHeight="1">
-      <c r="A257" s="39"/>
+      <c r="A257" s="41"/>
     </row>
     <row r="258" ht="15.75" customHeight="1">
-      <c r="A258" s="39"/>
+      <c r="A258" s="41"/>
     </row>
     <row r="259" ht="15.75" customHeight="1">
-      <c r="A259" s="39"/>
+      <c r="A259" s="41"/>
     </row>
     <row r="260" ht="15.75" customHeight="1">
-      <c r="A260" s="39"/>
+      <c r="A260" s="41"/>
     </row>
     <row r="261" ht="15.75" customHeight="1">
-      <c r="A261" s="39"/>
+      <c r="A261" s="41"/>
     </row>
     <row r="262" ht="15.75" customHeight="1">
-      <c r="A262" s="39"/>
+      <c r="A262" s="41"/>
     </row>
     <row r="263" ht="15.75" customHeight="1">
-      <c r="A263" s="39"/>
+      <c r="A263" s="41"/>
     </row>
     <row r="264" ht="15.75" customHeight="1">
-      <c r="A264" s="39"/>
+      <c r="A264" s="41"/>
     </row>
     <row r="265" ht="15.75" customHeight="1">
-      <c r="A265" s="39"/>
+      <c r="A265" s="41"/>
     </row>
     <row r="266" ht="15.75" customHeight="1">
-      <c r="A266" s="39"/>
+      <c r="A266" s="41"/>
     </row>
     <row r="267" ht="15.75" customHeight="1">
-      <c r="A267" s="39"/>
+      <c r="A267" s="41"/>
     </row>
     <row r="268" ht="15.75" customHeight="1">
-      <c r="A268" s="39"/>
+      <c r="A268" s="41"/>
     </row>
     <row r="269" ht="15.75" customHeight="1">
-      <c r="A269" s="39"/>
+      <c r="A269" s="41"/>
     </row>
     <row r="270" ht="15.75" customHeight="1">
-      <c r="A270" s="39"/>
+      <c r="A270" s="41"/>
     </row>
     <row r="271" ht="15.75" customHeight="1">
-      <c r="A271" s="39"/>
+      <c r="A271" s="41"/>
     </row>
     <row r="272" ht="15.75" customHeight="1">
-      <c r="A272" s="39"/>
+      <c r="A272" s="41"/>
     </row>
     <row r="273" ht="15.75" customHeight="1">
-      <c r="A273" s="39"/>
+      <c r="A273" s="41"/>
     </row>
     <row r="274" ht="15.75" customHeight="1">
-      <c r="A274" s="39"/>
+      <c r="A274" s="41"/>
     </row>
     <row r="275" ht="15.75" customHeight="1">
-      <c r="A275" s="39"/>
+      <c r="A275" s="41"/>
     </row>
     <row r="276" ht="15.75" customHeight="1">
-      <c r="A276" s="39"/>
+      <c r="A276" s="41"/>
     </row>
     <row r="277" ht="15.75" customHeight="1">
-      <c r="A277" s="39"/>
+      <c r="A277" s="41"/>
     </row>
     <row r="278" ht="15.75" customHeight="1">
-      <c r="A278" s="39"/>
+      <c r="A278" s="41"/>
     </row>
     <row r="279" ht="15.75" customHeight="1">
-      <c r="A279" s="39"/>
+      <c r="A279" s="41"/>
     </row>
     <row r="280" ht="15.75" customHeight="1">
-      <c r="A280" s="39"/>
+      <c r="A280" s="41"/>
     </row>
     <row r="281" ht="15.75" customHeight="1">
-      <c r="A281" s="39"/>
+      <c r="A281" s="41"/>
     </row>
     <row r="282" ht="15.75" customHeight="1">
-      <c r="A282" s="39"/>
+      <c r="A282" s="41"/>
     </row>
     <row r="283" ht="15.75" customHeight="1">
-      <c r="A283" s="39"/>
+      <c r="A283" s="41"/>
     </row>
     <row r="284" ht="15.75" customHeight="1">
-      <c r="A284" s="39"/>
+      <c r="A284" s="41"/>
     </row>
     <row r="285" ht="15.75" customHeight="1">
-      <c r="A285" s="39"/>
+      <c r="A285" s="41"/>
     </row>
     <row r="286" ht="15.75" customHeight="1">
-      <c r="A286" s="39"/>
+      <c r="A286" s="41"/>
     </row>
     <row r="287" ht="15.75" customHeight="1">
-      <c r="A287" s="39"/>
+      <c r="A287" s="41"/>
     </row>
     <row r="288" ht="15.75" customHeight="1">
-      <c r="A288" s="39"/>
+      <c r="A288" s="41"/>
     </row>
     <row r="289" ht="15.75" customHeight="1">
-      <c r="A289" s="39"/>
+      <c r="A289" s="41"/>
     </row>
     <row r="290" ht="15.75" customHeight="1">
-      <c r="A290" s="39"/>
+      <c r="A290" s="41"/>
     </row>
     <row r="291" ht="15.75" customHeight="1">
-      <c r="A291" s="39"/>
+      <c r="A291" s="41"/>
     </row>
     <row r="292" ht="15.75" customHeight="1">
-      <c r="A292" s="39"/>
+      <c r="A292" s="41"/>
     </row>
     <row r="293" ht="15.75" customHeight="1">
-      <c r="A293" s="39"/>
+      <c r="A293" s="41"/>
     </row>
     <row r="294" ht="15.75" customHeight="1">
-      <c r="A294" s="39"/>
+      <c r="A294" s="41"/>
     </row>
     <row r="295" ht="15.75" customHeight="1">
-      <c r="A295" s="39"/>
+      <c r="A295" s="41"/>
     </row>
     <row r="296" ht="15.75" customHeight="1">
-      <c r="A296" s="39"/>
+      <c r="A296" s="41"/>
     </row>
     <row r="297" ht="15.75" customHeight="1">
-      <c r="A297" s="39"/>
+      <c r="A297" s="41"/>
     </row>
     <row r="298" ht="15.75" customHeight="1">
-      <c r="A298" s="39"/>
+      <c r="A298" s="41"/>
     </row>
     <row r="299" ht="15.75" customHeight="1">
-      <c r="A299" s="39"/>
+      <c r="A299" s="41"/>
     </row>
     <row r="300" ht="15.75" customHeight="1">
-      <c r="A300" s="39"/>
+      <c r="A300" s="41"/>
     </row>
     <row r="301" ht="15.75" customHeight="1">
-      <c r="A301" s="39"/>
+      <c r="A301" s="41"/>
     </row>
     <row r="302" ht="15.75" customHeight="1">
-      <c r="A302" s="39"/>
+      <c r="A302" s="41"/>
     </row>
     <row r="303" ht="15.75" customHeight="1">
-      <c r="A303" s="39"/>
+      <c r="A303" s="41"/>
     </row>
     <row r="304" ht="15.75" customHeight="1">
-      <c r="A304" s="39"/>
+      <c r="A304" s="41"/>
     </row>
     <row r="305" ht="15.75" customHeight="1">
-      <c r="A305" s="39"/>
+      <c r="A305" s="41"/>
     </row>
     <row r="306" ht="15.75" customHeight="1">
-      <c r="A306" s="39"/>
+      <c r="A306" s="41"/>
     </row>
     <row r="307" ht="15.75" customHeight="1">
-      <c r="A307" s="39"/>
+      <c r="A307" s="41"/>
     </row>
     <row r="308" ht="15.75" customHeight="1">
-      <c r="A308" s="39"/>
+      <c r="A308" s="41"/>
     </row>
     <row r="309" ht="15.75" customHeight="1">
-      <c r="A309" s="39"/>
+      <c r="A309" s="41"/>
     </row>
     <row r="310" ht="15.75" customHeight="1">
-      <c r="A310" s="39"/>
+      <c r="A310" s="41"/>
     </row>
     <row r="311" ht="15.75" customHeight="1">
-      <c r="A311" s="39"/>
+      <c r="A311" s="41"/>
     </row>
     <row r="312" ht="15.75" customHeight="1">
-      <c r="A312" s="39"/>
+      <c r="A312" s="41"/>
     </row>
     <row r="313" ht="15.75" customHeight="1">
-      <c r="A313" s="39"/>
+      <c r="A313" s="41"/>
     </row>
     <row r="314" ht="15.75" customHeight="1">
-      <c r="A314" s="39"/>
+      <c r="A314" s="41"/>
     </row>
     <row r="315" ht="15.75" customHeight="1">
-      <c r="A315" s="39"/>
+      <c r="A315" s="41"/>
     </row>
     <row r="316" ht="15.75" customHeight="1">
       <c r="A316" s="9"/>
@@ -5309,7 +5368,33 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="41.38"/>
+    <col customWidth="1" min="2" max="2" width="48.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add  posts to information nav
</commit_message>
<xml_diff>
--- a/translation.xlsx
+++ b/translation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ActiveAgeing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dunguyenchiem/Project/ActiveAgeing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DFF323-1D90-41D4-B147-705653F886FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2542C6-3FB6-F74A-9F49-789818CB3AF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="419">
   <si>
     <t>English</t>
   </si>
@@ -366,6 +366,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>"It is crucial to build an active attitude</t>
     </r>
@@ -375,6 +376,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -383,6 +385,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>towards the preparation for financial safety and the access to healthcare."</t>
     </r>
@@ -546,6 +549,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">The age at which you </t>
     </r>
@@ -555,6 +559,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>plan</t>
     </r>
@@ -563,6 +568,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> to retire, assuming that you do not make any contributions to your retirement savings fund this year. So if you retire at age 60, kindly type '60'. In this case, your last contribution occurs when you are 59. This calculator also assumes that you make your entire contribution at the end of each year.</t>
     </r>
@@ -954,13 +960,393 @@
   </si>
   <si>
     <t>Sign in</t>
+  </si>
+  <si>
+    <t>Top 3 divine secrets to have a prosperous, healthy and happy old age</t>
+  </si>
+  <si>
+    <t>Top 3 bí quyết để có một tuổi “xế chiều” thịnh vượng khỏe mạnh an vui</t>
+  </si>
+  <si>
+    <t>Lão hóa theo thời gian là quá trình mà ai trong chúng ta dù sớm hay muộn đều sẽ phải trải qua. Thay vì lo sợ hay suy nghĩ tiêu cực, bạn có thể tìm cách tận hưởng tuổi già một cách trọn vẹn nhất với 3 bí quyết trong bài viết dưới đây.</t>
+  </si>
+  <si>
+    <t>Aging is a period of lifetime that any of us would have to go through even sooner or later. Instead of getting fearful or negative thoughts, you can find ways of enjoying old age with the top 3 secrets below.</t>
+  </si>
+  <si>
+    <t>Understanding the Okinawan diet</t>
+  </si>
+  <si>
+    <t>Học tập chế độ ăn của người Okinawa</t>
+  </si>
+  <si>
+    <t>You might have not known that residents in Okinawa Japan used to have a longer life expectancy than people elsewhere on Earth, and the reason stems from their traditional diet.</t>
+  </si>
+  <si>
+    <t>Chế độ ăn truyền thống của người Okinawa giàu các loại rau có màu xanh và vàng, và cung cấp lượng năng lượng thấp. Thêm vào đó, truyền thống dùng bữa khiến họ chỉ tiêu thụ khoảng 80% số thức ăn đã được chuẩn bị. Những người trẻ tuổi của Okinawa ngày nay đã dần rời xa phong cách truyền thống, và điều này khiến họ không còn sống thọ như các bậc tiền bối trước đây.</t>
+  </si>
+  <si>
+    <t>It emphasizes nutrient-dense, high-fiber vegetables and lean protein sources while discouraging saturated fat, sugar, and processed foods. In addition, the tradition of dining makes them consume only about 80% of the prepared food. Nowadays, the young people of Okinawa have gradually moved away from the traditional style, and consequently, they can’t live as long as their predecessors.</t>
+  </si>
+  <si>
+    <t>Stay physically active</t>
+  </si>
+  <si>
+    <t>Sống năng động</t>
+  </si>
+  <si>
+    <t>Các bằng chứng hiện nay đã khẳng định những người tập luyện thể dục thể thao sẽ sống lâu hơn người không tập, bởi luyện tập giúp giảm nguy cơ mắc bệnh lý tim mạch, đột quỵ, đái tháo đường và một số loại ung thư cũng như trầm cảm. Tập luyện thể dục thể thao cũng giúp giữ cho tinh thần minh mẫn cho dù cơ thể đã già đi.</t>
+  </si>
+  <si>
+    <t>It is said that people who exercise will live longer than those who don't because exercise reduces the risk of diseases such as stroke, diabetes, depression and even cancer as well. Exercise also helps keep the mind sharp even though the body is old.</t>
+  </si>
+  <si>
+    <t>Have a detailed financial plan</t>
+  </si>
+  <si>
+    <t>Financial planning not only helps you proactively prepare for your old age but also helps you find other financial sources to improve your income in retirement. Making a detailed financial plan is extremely necessary, however, it is much more important to check whether it is reasonable. You can check your financial plan for FREE at the Active Ageing Vietnam website.</t>
+  </si>
+  <si>
+    <t>Lập kế hoạch tài chính để nghỉ hưu an nhàn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theo chuyên gia Patricia Wenzel - Cố vấn tài chính cấp cao tại Merrill Lynch: “Nghỉ hưu thành công là có kế hoạch tài chính chi tiết và đảm bảo có đủ chi phí chăm sóc sức khỏe”. Việc lập kế hoạch tài chính không chỉ giúp bạn chủ động chuẩn bị cho tuổi “xế chiều” của mình mà còn giúp bạn tìm kiếm thêm các nguồn tài chính khác để cải thiện thu nhập khi về hưu. Lập một kế hoạch tài chính cụ thể chi tiết là vô cùng cần thiết, tuy nhiên, việc kiểm tra kế hoạch đó đã hợp lý hay chưa càng quan trọng hơn rất nhiều. Bạn hoàn toàn có thể kiểm tra kế hoạch tài chính của mình MIỄN PHÍ tại website Active Ageing Vietnam. </t>
+  </si>
+  <si>
+    <t>Có thể bạn chưa biết dân cư ở Okinawa (Nhật Bản) đã từng là những người có tuổi thọ trung bình cao hơn so với những người ở nơi khác trên Trái Đất, và lí do bắt nguồn từ chính chế độ ăn truyền thống của họ.</t>
+  </si>
+  <si>
+    <t>Tầm quan trọng của quản lý tài chính, chăm sóc sức khỏe trong thờI đại “vuca”</t>
+  </si>
+  <si>
+    <t>Trước hết, thuật ngữ "VUCA" được sử dụng để mô tả một thế giới "đa cực", hình thành khi đáp ứng bốn điều kiện: Biến động (Volatility), Không chắc chắn (Uncertainty), Phức tạp (Complexity) và Mơ hồ (Ambiguity). Đầu thập niên 90, khái niệm này đã được Trường Chiến tranh Lục quân Hoa Kỳ giới thiệu nhằm mô tả thế giới "đa cực" xuất hiện sau Chiến tranh Lạnh. Lần cuối cùng thế giới rơi vào tình trạng này là khi cuộc khủng hoảng tài chính toàn cầu năm 2008-2009 diễn ra. Hiện nay, thực tế đã cho thấy rằng đại dịch Covid-19 và những hệ quả của nó đã một lần nữa khiến thế giới rơi vào tình trạng VUCA.</t>
+  </si>
+  <si>
+    <t>Active Ageing Vietnam sẽ luôn đồng hành cùng bạn, đặc biệt là khi bạn chưa biết nên bắt đầu từ đâu. Chúng tôi luôn tin rằng, khi chúng ta đủ sẵn sàng và chủ động thì việc vượt qua khó khăn sẽ dễ dàng hơn. VUCA sẽ không thể “đánh gục” chúng ta mà sẽ trở thành cơ hội để ta chuyển mình và phát triển hơn.</t>
+  </si>
+  <si>
+    <t>The importance of financial management, healthcare in the era of "vuca"</t>
+  </si>
+  <si>
+    <t>Firstly, the acronym "VUCA" is used to describe a "multi-polar" world, established when four conditions are met: Volatility, Uncertainty, Complexity, and Ambiguity. VUCA represents a set of challenges that individuals, teams, managers, and organizations in affected industries all have to face. In the early 1990s, one of the earliest organizations that use the acronym VUCA was the United States Army War College. The last time the world fell into this situation was when the global financial crisis of 2008-2009 took place. Nowadays, the Covid-19 pandemic and its consequences have once again put the world in VUCA.</t>
+  </si>
+  <si>
+    <t>When the global economic situation deteriorates, its consequences will directly affect personal finance, such as reduced income, unemployment, bankruptcy, and so on. Although Vietnam is suffering less damage from this process than some countries, we should not ignore its potential dangers. We need to have strict plans for peaceful co-living and proactive psychological preparation for a long-lasting VUCA state.</t>
+  </si>
+  <si>
+    <t>From now, you should make an effective plan for financial, spending, and savings management, improve your healthcare levels to prepare for future uncertainty. Before the risk occurs, actively equip yourself with financial provisions, long-term and stable plans.</t>
+  </si>
+  <si>
+    <t>Active Ageing Vietnam will always accompany you, especially when you do not know where to start. We always believe that when we are ready and proactive, it will be easier to overcome difficulties. VUCA will not be able to "knock out" us but will become an opportunity for us to transform and thrive.</t>
+  </si>
+  <si>
+    <t>Khi tình hình kinh tế toàn cầu suy thoái, những hậu quả của nó sẽ tác động trực tiếp đến tài chính cá nhân: thu nhập giảm, thất nghiệp, đối mặt nguy cơ phá sản,… So với một số quốc gia khác, Việt Nam dù đang chịu ít tổn thất hơn từ quá trình này, chúng ta cũng không nên lơ là trước những mối nguy hiểm tiềm tàng đó. Chúng ta cần có những kế hoạch chặt chẽ để chung sống hòa bình, và chuẩn bị tâm lý cho trạng thái VUCA kéo dài một cách chủ động.</t>
+  </si>
+  <si>
+    <t>Ngay từ bây giờ, bạn nên lập một kế hoạch quản lý tài chính, chi tiêu và tiết kiệm hiệu quả, nâng cao mức độ chăm sóc sức khỏe cho bản thân để chuẩn bị cho những biến động trong tương lai. Trước khi rủi ro xảy ra, hãy chủ động trang bị cho bản thân những nguồn dự phòng tài chính, những kế hoạch lâu dài và ổn định.</t>
+  </si>
+  <si>
+    <t>Tôi đã nghỉ hưu ở tuổi 40 bằng cách nào?</t>
+  </si>
+  <si>
+    <t>“Nghỉ hưu vào tuổi 40” là điều mà nhiều người cho là suy nghĩ viễn vông. Tuy nhiên, điều đó hoàn toàn có thể thực hiện được nếu bạn có chiến lược tài chính đúng đắn, kế hoạch cụ thể và tuân thủ kỷ luật. Sẽ có một ngày, bạn thức dậy chỉ để theo đuổi ước mơ của chính mình, như chu du khắp thế giới, thực hiện sở thích riêng, theo học điều mình muốn mà chẳng phải đắn đo gì. Hãy xem những người U40 đã nghỉ hưu sớm chia sẻ kinh nghiệm của họ nhé!</t>
+  </si>
+  <si>
+    <t>“Tôi dự trù rất chi tiết về các khoản chi tiêu lúc về hưu”.</t>
+  </si>
+  <si>
+    <t>“Tôi có chiến lược chi tiêu và kiên trì tuân thủ”.</t>
+  </si>
+  <si>
+    <t>“Tôi luôn có kế hoạch dự phòng”.</t>
+  </si>
+  <si>
+    <t>How did i retire at 40?</t>
+  </si>
+  <si>
+    <t>As a matter of fact, "Retirement at age 40" seems to be unfeasible. However, it is entirely achievable if you have a precise financial strategy that is particularly planned and strictly followed. One day, you wake up just to pursue your own dreams, like traveling the world, doing your hobbies, learning what you want without anxiety. Let's see how the early retired U40s share their experiences!</t>
+  </si>
+  <si>
+    <t>"I have a detailed plan for my retirement expenditure".</t>
+  </si>
+  <si>
+    <t>Imagine what your retirement days will look like. Will you live a quiet life to take care of the garden that you have forgotten, or will you travel everywhere, experience many new things? The more accurately you visualize, the clearer you will know the amount of money you need while you no longer work and plan your spending in accordance with the "less than 4%" rule on the profitability of all portfolios.</t>
+  </si>
+  <si>
+    <t>"I have a spending strategy and persevere in compliance."</t>
+  </si>
+  <si>
+    <t>"I always have a backup plan".</t>
+  </si>
+  <si>
+    <t>When there are financial fluctuations, you can face losing a large amount of money. Be willing to choose a lower living standard, or worse, increase your earnings, from part-time work, collaborators, rent out your second home so you can maintain your financial plan.</t>
+  </si>
+  <si>
+    <t>Retirement at the age of 40s is not difficult to do if you start thinking about accumulation and investment from your 20s - 30s. By the time you are 40, you have mastered this skill, and your retirement age may not be 60 as usual. Active Aging Vietnam wishes you the best of luck and courage so you can enjoy your life at the age of 40!</t>
+  </si>
+  <si>
+    <t>Hãy hình dung rõ những ngày tháng nghỉ hưu của bạn sẽ như thế nào. Bạn sẽ sống cuộc đời tĩnh lặng để chăm sóc khu vườn mà mình từng bỏ quên, hay sẽ ngao du khắp nơi, trải nghiệm nhiều điều mới lạ? Hình dung càng chính xác, bạn sẽ biết được càng rõ ràng số tiền mình cần trong thời gian không còn làm việc và lên kế hoạch chi tiêu theo đúng quy tắc “dưới 4%” trên mức lợi nhuận của tất cả các danh mục đầu tư.</t>
+  </si>
+  <si>
+    <t>Đó chính là dùng ít hơn số tiền tôi nghĩ mình nên dùng và tiết kiệm nhiều hơn số tiền tôi nghĩ sẽ cần đến. Có thể bạn cảm thấy chẳng có gì là ‘chiến lược’, nhưng thực tế chẳng dễ dàng gì để bảo toàn tiền lương hoặc thưởng khi xung quanh có quá nhiều ‘cám dỗ’. Do đó, hãy nghiêm khắc tuân thủ theo nguyên tắc: Bắt đầu tiết kiệm càng sớm càng tốt, chỉ chi xài cho những gì thật sự cần thiết để cảm thấy vừa đủ thoải mái, đồng thời tìm mọi cách để cắt bớt chi tiêu không cần thiết.</t>
+  </si>
+  <si>
+    <t>Khi có những biến động về tài chính, bạn có thể đối mặt với việc mất một khoản tiền lớn. Hãy sẵn sàng tâm thế chọn mức sống thấp hơn, hoặc tệ hơn là tìm lại nguồn thu nhập, từ công việc bán thời gian, cộng tác viên, cho thuê căn nhà thứ 2 để bạn có thể duy trì được kế hoạch tài chính của mình.</t>
+  </si>
+  <si>
+    <t>Việc nghỉ hưu ở tuổi U40 không phải là điều khó thực hiện nếu bạn bắt đầu nghĩ đến tích lũy và đầu tư từ những năm 20 - 30 tuổi. Đến thời điểm 40 tuổi, bạn đã rèn luyện được tốt kỹ năng này và thời điểm nghỉ hưu có thể không phải là 60 như thông thường. Active Aging Vietnam chúc bạn luôn lạc quan và can đảm để có thể tận hưởng cuộc đời của chính mình ở tuổi 40!</t>
+  </si>
+  <si>
+    <t>It is essential to keep your expenditure down, and by extension, your savings rate is keeping your lifestyle in check. It is about spending less than you think it should and saving more than you think it needs. You may feel like there's nothing 'strategic', but it's actually not easy to preserve wages or bonuses when there are too many 'temptations’ around. Therefore, strictly follow the principle: &lt;br&gt; - Start saving as soon as possible.&lt;br&gt;
+- Spending only on what is really necessary to feel just comfortable enough, &lt;br&gt;
+- Find ways to cut down on unnecessary spending.</t>
+  </si>
+  <si>
+    <t>Bước 1: Truy cập website Active Ageing Vietnam (http://activeageingvietnam.com/ ) và chọn tab “Lập kế hoạch về hưu”.</t>
+  </si>
+  <si>
+    <t>Bước 2: Điền các thông tin vào bảng hỏi, lưu ý đơn vị của các câu hỏi. Bạn có thể rê chuột vào nút "i" để đọc phần giải thích câu hỏi.</t>
+  </si>
+  <si>
+    <t>Bước 3: Xem kết quả phân tích.</t>
+  </si>
+  <si>
+    <t>Bước 4: Xem đề xuất nếu kế hoạch chưa hợp lí. Đăng ký trở thành hội viên của Active Ageing Vietnam để nhận thêm thông tin hơn về các tính năng khác.</t>
+  </si>
+  <si>
+    <t>Trước hết, để giúp bạn dễ thao tác, chúng tôi đã đặt ra bài toán:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Ông Nguyễn Văn X hiện đang 45 tuổi, thu nhập trung bình 15 triệu VNĐ/ tháng (180 triệu VNĐ/năm). Ông dự kiến thu nhập của mình sẽ tăng 2% hàng năm cho đến khi ông nghỉ hưu ở tuổi 60. Để chuẩn bị cho tương lai, ông đã tích góp được 700 triệu VNĐ riêng cho “Quỹ Tiết kiệm Về hưu” của mình (Quỹ tiết kiệm về hưu là một Quỹ tiết kiệm riêng, tách biệt khỏi các khoản tiết kiệm khác như: Tiết kiệm mua xe, Tiết kiệm cho con,...). </t>
+  </si>
+  <si>
+    <t>Hàng năm, ông dự kiến trích 8% trên tổng thu nhập để đóng góp thêm vào Quỹ Tiết kiệm Về hưu. Khoản đóng góp cuối cùng xảy ra vào năm ông 59 tuổi. Kể từ sau năm này, ông không có thêm thu nhập nào do ông không có lương hưu. Khoản tiền từ Quỹ Tiết kiệm Về hưu sẽ được sử dụng để đầu tư bằng nhiều hình thức khác nhau (gửi tiết kiệm, đầu tư vàng, ngoại tệ, các tài sản tài chính khác,...) và ông dự kiến sẽ thu được lợi tức (lãi suất) hàng năm là 6.5% (trước khi về hưu) và 4.5% (sau khi về hưu). Ông hy vọng mình sẽ thọ đến 90 tuổi và vẫn chủ động về tài chính.”</t>
+  </si>
+  <si>
+    <t>Từ những dữ liệu trên, Active Ageing Vietnam đã giúp ông X tính toán kế hoạch về hưu của ông và đề xuất được kết quả như 4 hình minh hoạ.</t>
+  </si>
+  <si>
+    <t>Active Ageing Vienam xin trân trọng cảm ơn các bạn đã quan tâm, ủng hộ và trải nghiệm sản phẩm đầu tiên của chúng tôi!</t>
+  </si>
+  <si>
+    <t>Step 1: Go to Active Ageing Vietnam's website (http://activeageingvietnam.com/) and select the "Retirement Planning" tab.</t>
+  </si>
+  <si>
+    <t>Step 2: Fill in the questionnaire. Please pay attention to the measurement of the answers. You can hover your mouse over the button "i" to read the question description.</t>
+  </si>
+  <si>
+    <t>Step 3: View analysis results</t>
+  </si>
+  <si>
+    <t>Step 4: See the proposal if your plan is not reasonable. Sign up to become an Active Ageing Vietnam member to obtain further information about other features.</t>
+  </si>
+  <si>
+    <t>To make it easy for you to understand, we assume that:</t>
+  </si>
+  <si>
+    <t>“Currently, Mr. Nguyen Van X is 45 years old, and his average income is 15 million VND per month (180 million VND per year). He expects his income growth rate is 2% annually until he retires at the age of 60. To prepare for the future, he has accumulated VND 700 million for his "Retirement Savings Fund" (Retirement savings fund is a separate savings fund, separate from other savings such as saving to buy a car, saving for his children,...).</t>
+  </si>
+  <si>
+    <t>Every year, he expects to deduct 8% of his total income to make additional contributions to the Retirement Savings Fund. The last donation occurred when he was 59 years old. Since this year, he has had no additional income because he does not have a pension. Besides, funds from the Retirement Savings Fund will be used to invest in a variety of forms (savings, gold investments, foreign currencies, and other financial assets), and he expects to earn an annual interest of 6.5% (before retirement) and 4.5% (after retirement). He hopes to live until the age of 90 and remain financially secure.”</t>
+  </si>
+  <si>
+    <t>Active Ageing Vietnam will help Mr. Nguyen Van X make his retirement plan in just four simple steps illustrated in four pictures.</t>
+  </si>
+  <si>
+    <t>Active Ageing Vietnam would like to express our special thanks for your interest, support, and experience with our first product!</t>
+  </si>
+  <si>
+    <t>Tiết kiệm là một hành trình của thói quen</t>
+  </si>
+  <si>
+    <t>“Phải tiết kiệm từ khi nào hay tiết kiệm trong bao lâu để có thể tự xây hay mua được một căn nhà?”. Đây chắc hẳn là mối quan tâm chung của rất nhiều người bởi lẽ mua nhà, mua xe vẫn được coi là mục tiêu quan trọng cần hướng tới. Vậy tiết kiệm bao nhiêu là đủ?</t>
+  </si>
+  <si>
+    <t>Mới đây, trên mạng xã hội đã xuất hiện một bảng thống kê có liên quan đến vấn đề kể trên. Bảng thống kê đã nêu ra một kế hoạch cụ thể mỗi năm bạn cần tiết kiệm bao nhiêu tiền để có thể mua nhà trước năm 35 tuổi. Chẳng hạn như năm 19-21 tuổi, bạn sẽ cần tiết kiệm 500 nghìn/tháng tương đương với 6 triệu/năm. Năm 22 tuổi, con số bạn cần để dành mỗi tháng là 1 triệu. Lúc này, cộng dồn với khoản từ 3 năm trước, bạn có được tổng tiền tiết kiệm là 30 triệu. Cứ thế, đến năm 35 tuổi và 35 triệu tiết kiệm/tháng, bạn sẽ tích đủ 2,022 tỷ. Số tiền này hẳn là đã khá đầy đủ để tậu một căn nhà cho riêng mình.</t>
+  </si>
+  <si>
+    <t>Có thể nói tiết kiệm là cách duy nhất giúp bạn mua được nhà sớm mà không cần sự trợ giúp của bất kỳ ai. Mấu chốt quan trọng của việc mua nhà nằm ở khả năng quản lý tài chính xem bạn kiếm được bao nhiêu và tiết kiệm được bao nhiêu. Không phải tự nhiên mà tỷ phú Warren Buffett luôn tâm đắc rằng: “Đừng tiết kiệm những gì còn lại sau khi bạn tiêu tiền, hãy tiêu phần còn lại sau khi bạn tiết kiệm được.” Chính vì vậy, tiết kiệm luôn là một hành trình của thói quen!</t>
+  </si>
+  <si>
+    <t>Nguồn: VNExpress</t>
+  </si>
+  <si>
+    <t>Saving is a journey of habits</t>
+  </si>
+  <si>
+    <t>"When should I start saving journeys, and how long does it take to build or buy my own house? This question could have raised a common interest as buying a house or getting a car is still considered an important goal. Accordingly, how much is enough for saving?</t>
+  </si>
+  <si>
+    <t>Recently, a statistical table related to the above problem has been shared widely on social media channels and drew much attention. It has presented a specific plan on how much we need to save money each year to buy a house before the age of 35. For example, at the age of 19 to 21, you will need to save 500 thousand VND per month, equivalent to 6 million per year. At 22 years old, the number you need to save each month is 1 million. Then, adding up the amount of 3 previous years, we have a total savings of 30 million. Similarly, by the age of 35, with savings equivalent to 35 million per month, we will have accumulated enough 2,022 billion. This amount should have been quite enough to buy a house.</t>
+  </si>
+  <si>
+    <t>It could be said that no matter what stage of life you are in, one thing will always remain the same: You are never too young — or too old — to save money. Saving is the only way to help you buy a house early without anyone's help. The key to buying a house lies in managing a financial plan to see how much we earn and how much we save. Billionaire Warren Buffett always admires: "Do not save what is left after spending; instead spend what is left after saving". Hence, saving is always a journey of habits!</t>
+  </si>
+  <si>
+    <t>Source: VNExpress</t>
+  </si>
+  <si>
+    <t>Giải mã phương pháp 50/20/30 trong quản lý tài chính cá nhân hiệu quả</t>
+  </si>
+  <si>
+    <t>Theo các bạn “giàu có” nghĩa là gì?</t>
+  </si>
+  <si>
+    <t>Có một định nghĩa rất hay được đề cập trong cuốn sách "Cha giàu, cha nghèo" của tác giả Robert Kiyosaki rằng “giàu có” có nghĩa là nếu như bây giờ các bạn không làm gì nữa cả, thì tất cả những tài sản mà các bạn đang có sẽ giúp cho các bạn sống được trong bao nhiêu lâu? Nếu như các bạn sống được càng lâu thì điều đó có nghĩa là các bạn càng “giàu có”.</t>
+  </si>
+  <si>
+    <t>Để sống một cuộc sống thoải mái và tự do hơn và không phải lo nghĩ về tài chính quá nhiều mỗi tháng, thì điều mà các bạn cần làm đầu tiên đó chính là "Kỷ luật và nguyên tắc". Chính vì vậy, Active Ageing Vietnam muốn chia sẻ phương pháp 50/20/30, một phương pháp quản lý tài chính cá nhân vô cùng hiệu quả mà ai cũng nên biết. Vậy, quy tắc 50/20/30 hoạt động như thế nào? Quy tắc này sẽ chia nhỏ thu nhập của bạn thành 3 danh mục chính bao gồm khoản chi cho nhu cầu thiết yếu, khoản chi cho những thứ sở thích và tiết kiệm, đầu tư với tỷ lệ phần trăm lần lượt là 50-20-30.</t>
+  </si>
+  <si>
+    <t>50% thu nhập của bạn - Các yếu tố cần thiết</t>
+  </si>
+  <si>
+    <t>Để bắt đầu, hãy dành ra không quá một nửa thu nhập của bạn cho những nhu cầu thiết yếu trong cuộc sống. 50% có thể là một tỷ lệ cao nhưng một khi xem xét những danh mục thuộc các chi phí cần thiết bạn mới thấy con số đó có ý nghĩa.</t>
+  </si>
+  <si>
+    <t>Nói một cách rõ ràng, chi phí thiết yếu là những khoản mà bạn chắc chắn phải bỏ ra bất kể bạn ở đâu, làm gì hay có kế hoạch gì trong tương lai. Thông thường, những chi phí này thường giống nhau ở hầu hết mọi người, bao gồm tiền ăn, tiền ở, chi phí đi lại và các hóa đơn tiện ích như điện, nước.</t>
+  </si>
+  <si>
+    <t>Hãy cố gắng để tổng chi phí thiết yếu không vượt quá 50% lương. Nhưng nếu con số đó lớn hơn 50%, hãy thử giảm tiền các hóa đơn xuống như sử dụng phương tiện công cộng thay vì phương tiện cá nhân,…Mà nếu không thể làm được điều đó nữa thì bắt buộc bạn phải giảm 5% ở mỗi danh mục tiếp theo. (Các chuyên gia khuyên bạn cắt giảm ở phần chi tiêu cá nhân, chứ không nên giảm ở mục tiêu tài chính).</t>
+  </si>
+  <si>
+    <t>20% thu nhập của bạn – Mục tiêu tài chính</t>
+  </si>
+  <si>
+    <t>Bước tiếp theo là dành 20% lương để dành cho mục tiêu tài chính bao gồm tiết kiệm, trả nợ và quỹ dự phòng. Danh mục này chỉ nên được bổ sung khi danh mục chi phí thiết yếu đã được xét đến và trước khi bạn kịp nghĩ đến bất cứ điều gì thuộc danh mục chi tiêu cá nhân.</t>
+  </si>
+  <si>
+    <t>Nếu bạn đạt được mục tiêu 50% hoặc ít hơn thu nhập dành cho chi phí thiết yếu và 20% hoặc lớn hơn dành cho mục tiêu tài chính, bạn sẽ có thể trả nợ nhanh hơn hoặc nếu không bạn sẽ ít phải lo lắng hơn khi bước vào tuổi nghỉ hưu. "Nghỉ hưu" có thể là một khái niệm chưa thực sự cần thiết ở tuổi 20, 30 nhưng hãy nhớ bạn càng bắt đầu tiết kiệm sớm bao nhiêu thì tuổi già của bạn càng thoải mái bấy nhiêu khi không phải nghĩ đến chuyện tích cóp hằng ngày.</t>
+  </si>
+  <si>
+    <t>30% thu nhập của bạn – Chi tiêu cá nhân</t>
+  </si>
+  <si>
+    <t>Danh mục cuối cùng và cũng là yếu tố có thể tạo ra sự khác biệt lớn nhất trong ngân sách của bạn – những chi phí không thiết yếu. Một số chuyên gia tài chính xem xét đây là danh mục hoàn toàn linh hoạt nhưng trong cuộc sống hiện đại, nhiều người cho rằng một số thứ thuộc những thứ "xa xỉ" là một phần không thể thiếu với họ. Lý do danh mục này chiếm phần trăm lớn hơn mục tiêu tài chính là bởi có quá nhiều thứ thuộc vào đây.</t>
+  </si>
+  <si>
+    <t>Những chi phí phục vụ cuộc sống cá nhân bao gồm tiền điện thoại, thực phẩm giải trí, du lịch, mua sắm,…Cũng giống như danh mục chi phí thiết yếu, 30% là tỷ lệ tối đa bạn nên dành cho cuộc sống cá nhân. Chi phí thuộc danh mục này càng ít tương lại tài chính càng được đảm bảo khi bạn về hưu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhắc đến quản lý tài chính, nhiều người thường cho rằng: "Tôi không có tiền, thu nhập thì thấp, không biết quản lý, mà quản lý thì có tác dụng gì đâu". Tuy nhiên, tiền bạc là thứ cần tích lũy từng chút từng chút một. Đừng nói bạn không có tiền nên không cần quản lý, ngược lại, cần phải học xong cách quản lý, chi tiêu cho hợp, bạn mới có thể có tiền. </t>
+  </si>
+  <si>
+    <t>Tuy nhiên cũng cần lưu ý rằng, quy tắc 50/20/30 này không thể áp dụng một cách hoàn hảo cho mọi người trong mọi trường hợp mà chúng chỉ là hướng dẫn để bạn có thể áp dụng một cách linh hoạt cho quỹ ngân sách của mình. Bạn có thể linh hoạt thay đổi tỷ lệ phần trăm dựa vào những ưu tài chính của bản thân. Hãy nhớ là tiền đã vào túi mình rồi thì đừng để nó trôi đi chỗ khác và vụt mất nhé. Active Ageing Vietnam chúc các bạn sẽ quản lý tài chính cá nhân thật thành công!</t>
+  </si>
+  <si>
+    <t>Già hóa dân số và những gánh nặng người già đang và sẽ gặp phải</t>
+  </si>
+  <si>
+    <t>Hiện nay, Việt Nam đang là một trong những nước có tốc độ già hóa dân số rất nhanh. Vào năm 2035, hơn 20% dân số nước ta có độ tuổi trên 60. Trước tình hình đó, những người sắp đến độ tuổi nghỉ hưu cần chủ động chuẩn bị để đối mặt với những vấn đề mà người cao tuổi thường gặp. Khi tuổi tác tăng cao, người già lại phải đối mặt với việc sức khỏe giảm dần, những biến đổi sinh lý do tuổi tác, và khả năng lao động bị ảnh hưởng. Cụ thể, người già có nguy cơ mắc phải các căn bệnh hiểm nghèo, hoặc bệnh không lây nhiễm như ung thư, đột quỵ, xương khớp hay suy giảm trí nhớ. Không chỉ riêng sức khoẻ, họ còn phải đối mặt với những vấn đề về tài chính. Ví dụ, chi phí chăm sóc sức khoẻ (viện phí, thuốc thang,…) ngày càng tăng cao, mà người già lại không còn chủ động trong thu nhập vì khả năng lao động không còn như trước. Từ đó, người già sẽ phải cần đến sự quan tâm, giúp đỡ từ người khác.</t>
+  </si>
+  <si>
+    <t>Hẳn rằng, mọi người đều muốn ngay cả khi về già vẫn có thể làm chủ cuộc sống của riêng mình, và không muốn lệ thuộc vào bất cứ ai. Thành ngữ cũng khuyên rằng “phòng bệnh hơn chữa bệnh”, hay đừng để “mất bò mới lo làm chuồng”, cho thấy việc lập kế hoạch về hưu là rất cần thiết. Để giảm thiểu những tác động mà tuổi già mang lại, con người nên có sự chuẩn bị kỹ càng từ trước, nhất là ở độ tuổi lao động. Với một kế hoạch về hưu khoa học, cùng với kỹ năng quản lý tài chính và sự chủ động chăm sóc sức khỏe từ trước, con người sẽ giảm bớt được rất nhiều gánh nặng vào tuổi già.</t>
+  </si>
+  <si>
+    <t>Ageing population and the burden that the elderly has been facing</t>
+  </si>
+  <si>
+    <t>Nowadays, Vietnam is one of the fastest ageing population countries. By 2035, more than 20% of the country's population will be over 60 years of age. Hence, people being around retirement age should proactively prepare for confronting challenges that the elderly may face. As age increases, older people may suffer health issues, physiological changes, and reduced or gradual loss of workability. Specifically, older people tend to contact uninfectious or severe diseases, such as cancer, stroke, osteoarthritis, or Alzheimer's. Not only health, but they also have to deal with financial problems. For example, healthcare costs have been rising significantly, whereas the declined workability makes the elderly no longer proactive in income. Thus, the elderly would need care and attention from others.</t>
+  </si>
+  <si>
+    <t>Indeed, everyone prefers to have their own life even when they are old, which means they do not want to depend on others. There are idioms "prevention is better than cure" or "It is too late to lock the stable when the horse is stolen, " indicating the importance of making a retirement plan. To minimize the impacts relating to high age, people should be well-prepared from working age. If people have a well-prepared scientific retirement plan, financial management skills, and healthcare proactiveness from working ag, they can reduce their burden in retirement age.</t>
+  </si>
+  <si>
+    <t>Trên thế giới nói chung, và tại Việt Nam nói riêng, quá trình già hóa dân số diễn ra rất nhanh và tác động đến cuộc sống con người trên nhiều phương diện từ kinh tế, an sinh xã hội, quốc phòng. Già hóa dân số thể hiện qua sự thay đổi cơ cấu dân số của một quốc gia: số lượng trẻ em sinh ra giảm đi, tuổi thọ trung bình tăng lên, hệ quả là tỉ trọng người cao tuổi trong cơ cấu dân số tăng. Theo số liệu từ World Bank, tuổi thọ trung bình tại Việt Nam đã tăng lên 76,3 từ 70,5 trong giai đoạn 1990 – 2019, cao nhất trong các quốc gia có cùng mức thu nhập, tạo ra thách thức vô cùng lớn: “getting old before getting rich" (tạm dịch: chưa giàu đã già). Trên thực tế, già hóa dân số không chỉ là một vấn đề vĩ mô mà còn ảnh hưởng lên mỗi cá nhân. Một trong những giải pháp từ phía chính phủ là nâng độ tuổi về hưu. Cụ thể, mức tuổi này tăng lên 62 từ 60 ở nam, và từ 55 lên 60 ở nữ vào năm 2035.</t>
+  </si>
+  <si>
+    <t>Tuy nhiên, một giải pháp thôi là chưa đủ. Do đó, việc phát triển các giải pháp giúp toàn xã hội chuẩn bị cho giai đoạn già hóa dân số trong 15 năm tới đây là vô cùng cấp thiết. Active Ageing Vietnam là một trong số những giải pháp đầu tiên hướng tới giải quyết hiệu quả và đầy đủ các tác động của già hoá dân số.</t>
+  </si>
+  <si>
+    <t>As the world has been grappling with the rapid ageing population, Vietnam is no exception. Indeed, Vietnam is one of the fastest ageing countries. It has impacted our lives in several aspects, including the economy, society, welfare, and defense. Ageing population is revealed as a change in a country's population structure due to a decrease in the number of children born together with an increase in life expectancy, which results in an increased proportion of the elderly in the population structure. According to the World Bank, life expectancy in Vietnam increased to 76.3 from 70.5 between 1990 and 2019, the highest among countries with similar income levels. It leads to a significant challenge called "getting old before getting rich". Indeed, ageing population is not only a macro perspective, it also exerts considerable impacts on individuals. The government has introduced a policy that raises the retirement age in Vietnam to cope with this challenge, in which the retirement age increases to 62 for men and to 60 for women by 2035.</t>
+  </si>
+  <si>
+    <t>However, one resolution only is insufficient. Therefore, developing the set of collaborative actions for the society to prepare for the upcoming ageing population period in the next 15 years is essential. Active Ageing Vietnam is among the first solutions in Vietnam for the holistic settlement of issues arising from ageing population.</t>
+  </si>
+  <si>
+    <t>"Ageing population" - challenge for Vietnam</t>
+  </si>
+  <si>
+    <t>"Già hóa dân số" - Thách thức mà Việt Nam phải đối mặt</t>
+  </si>
+  <si>
+    <t>Giải pháp xã hội của Active Ageing Vietnam</t>
+  </si>
+  <si>
+    <t>The social solution prototype of Active Ageing Vietnam</t>
+  </si>
+  <si>
+    <t>Hiện nay, thế giới đang phải vật lộn với quá trình già hóa dân số diễn ra rất nhanh, và Việt Nam cũng không phải là ngoại lệ. Thực tế, Việt Nam là một trong những quốc gia có tốc độ già hóa dân số nhanh nhất. Nếu không kịp thời chuẩn bị cho giai đoạn dân số già sắp tới, người cao tuổi sẽ phải đối mặt với hậu quả nghiêm trọng như thiếu hụt tài chính, khó tiếp cận các dịch vụ chăm sóc sức khỏe và suy giảm phúc lợi. Gói giải pháp cung cấp bởi Active Ageing Vietnam bao gồm một ứng dụng trên nền tảng di động, một trang web và chuỗi các hội thảo.</t>
+  </si>
+  <si>
+    <t>Xin vui lòng dành ít phút để xem video minh họa giải pháp xã hội của chúng tôi. Video này thể hiện mức độ mà Active Ageing Vietnam hiểu rõ nguyên nhân gốc rễ của vấn đề xã hội nêu trên; giải thích quá trình mà chúng tôi tiếp cận chúng để đưa ra các giải pháp cho người lao động nhằm giúp họ nâng cao mức sống của mình khi về hưu; và chỉ ra những tác động xã hội mà Active Ageing Vietnam có thể mang đến cho cộng đồng.</t>
+  </si>
+  <si>
+    <t>Bên cạnh đó, chúng tôi đã mời ông Lê Hồng Lĩnh (CEO của Hiệp hội CFO Việt Nam) và ông Ngô Đình Đức (Nhà sáng lập kiêm Tổng Giám đốc Công ty Cổ phần Tư vấn POCD) góp mặt trong video này nhằm chia sẻ quan điểm về giải pháp của Active Ageing Vietnam. Các tác động xã hội mà chúng tôi hướng đến dựa trên mục tiêu phát triển bền vững thứ #1, #3 và #11 của Liên Hợp Quốc.</t>
+  </si>
+  <si>
+    <t>Chúng tôi rất mong nhận được ý kiến, phản hồi của bạn để phát triển giải pháp hoàn thiện hơn. Chúng tôi xin trân trọng cảm ơn sự quan tâm, theo dõi va ủng hộ của bạn/ anh/ chị trong thời gian qua và sắp tới.</t>
+  </si>
+  <si>
+    <t>As the world has been grappling with the rapid ageing population, Vietnam is not an exception. Indeed, Vietnam is one of the fastest ageing countries. Without preparation for the next ageing population phase, the elderly will face serious consequences such as financial restraint, limited healthcare services access, and depreciation in their well-being. The solution package provided by Active Ageing Vietnam includes a mobile app, a website, and a series of workshops.</t>
+  </si>
+  <si>
+    <t>Please spend some minutes watching the video illustrating our social solution prototype. This video reveals how Active Ageing Vietnam thoroughly recognize the root cause of the social issue mentioned above; explains the process by which we approach the root cause to offer the solutions for working people to enhance their living standards when they retire; and indicates potential social impacts that Active Ageing Vietnam will bring to society.</t>
+  </si>
+  <si>
+    <t>In this video, we also invite Mr. Le Hong Linh (CEO of Vietnam CFO Association) and Mr. Ngo Dinh Duc (Founder &amp; CEO of Practical Organization Consulting Development Corporation) to share their opinions about Active Ageing Vietnam’s solution. Our intended social impacts are aligned with UN SDGs #1, #3, and #11.</t>
+  </si>
+  <si>
+    <t>We would love to receive your opinion to develop our solution. Last but not least, we would like to express our special thanks for your continuous support and love for us.</t>
+  </si>
+  <si>
+    <t>Giới thiệu gói giải pháp của Active Ageing Vietnam</t>
+  </si>
+  <si>
+    <t>Introduction about solution package of Active Ageing Vietnam</t>
+  </si>
+  <si>
+    <t>Bạn có mong muốn khoảng thời gian nghỉ hưu của mình sẽ vui vẻ, an yên?</t>
+  </si>
+  <si>
+    <t>Bạn có mong muốn mình sẽ có một kế hoạch cụ thể để chuẩn bị cho tuổi “xế chiều”?</t>
+  </si>
+  <si>
+    <t>Chúng tôi tin rằng tất cả các dự định này đều có thể khả thi cùng với Active Ageing Vietnam. Được ra đời với nỗi trăn trở về già hóa dân số, gói giải pháp của chúng tôi bao gồm ứng dụng di động, trang web được phát triển theo hướng kỹ thuật số và các chuỗi hội thảo nhằm cung cấp các thông tin từ các chuyên gia có kinh nghiệm.</t>
+  </si>
+  <si>
+    <t>Vậy, những giải pháp này sẽ được vận hành ra sao? Bằng cách nào dự án có thể đem lại lợi ích nhiều nhất tới cộng động? Hãy cùng chúng tôi khám phá tại video dưới đây!</t>
+  </si>
+  <si>
+    <t>Active Ageing Vietnam xin gửi lời cảm ơn chân thành nhất đến ông Raymond Chu (Chu Quang Thái) - đại diện thường trực phía Nam Cục Phát triển thị trường và doanh nghiệp Khoa học và Công nghệ, Bộ Khoa học và Công nghệ đã tham gia đóng góp ý kiến về tiềm năng của dự án. Những nhận xét và lời động viên của ông là sự khích lệ vô cùng lớn đối với Active Ageing Vietnam!</t>
+  </si>
+  <si>
+    <t>Ngoài ra, dự án rất mong nhận được ý kiến, phản hồi của bạn để phát triển giải pháp hoàn thiện hơn. Chúng tôi xin trân trọng cảm ơn sự quan tâm, theo dõi và ủng hộ của bạn trong thời gian qua và sắp tới.</t>
+  </si>
+  <si>
+    <t>Do you yearn for a comfortable and peaceful retirement?</t>
+  </si>
+  <si>
+    <t>Do you yearn for having a specific plan on retirement preparation?</t>
+  </si>
+  <si>
+    <t>We believe that all of your wishes will be possible with Active Ageing Vietnam. Being launched with concern about ageing population, our solution package comprises a mobile app, a website developed with a digital approach, and a series of workshops.</t>
+  </si>
+  <si>
+    <t>So, how are these solutions operated? How do they bring great value to the community? The answer is well presented in the video below!</t>
+  </si>
+  <si>
+    <t>Active Ageing Vietnam would like to express our sincere thanks to Mr. Raymond Chu - Head Southern office of National Startup Support Center - NSSC HCM Office/ NATEC/ MOST, who has devotedly given constructive comments to encourage our project’s development.</t>
+  </si>
+  <si>
+    <t>Besides, we would love to receive your opinions to enhance our solution further and look forward to receiving your continuous support.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -970,57 +1356,68 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <strike/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1032,6 +1429,41 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFE4E6EB"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Headings)"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1103,7 +1535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1221,9 +1653,28 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1441,21 +1892,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A153" sqref="A153"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="61.125" customWidth="1"/>
-    <col min="2" max="2" width="52.375" customWidth="1"/>
+    <col min="1" max="1" width="61.1640625" customWidth="1"/>
+    <col min="2" max="2" width="52.33203125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="21.25" customWidth="1"/>
-    <col min="5" max="23" width="7.625" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="5" max="23" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75">
+    <row r="1" spans="1:16" ht="17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1465,23 +1916,23 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+    </row>
+    <row r="2" spans="1:16" ht="16">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1490,7 +1941,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" ht="16">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1499,7 +1950,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" ht="16">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -1508,7 +1959,7 @@
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" ht="16">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1517,7 +1968,7 @@
       </c>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" ht="16">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1526,7 +1977,7 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" ht="16">
       <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
@@ -1535,7 +1986,7 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" ht="16">
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
@@ -1544,17 +1995,17 @@
       </c>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:16" ht="16">
+      <c r="A9" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="43" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:16" ht="16">
+      <c r="A10" s="42" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -1562,7 +2013,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" ht="16">
       <c r="A11" s="9" t="s">
         <v>22</v>
       </c>
@@ -1571,7 +2022,7 @@
       </c>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" ht="16">
       <c r="A12" s="9" t="s">
         <v>24</v>
       </c>
@@ -1580,7 +2031,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:16" ht="30">
+    <row r="13" spans="1:16" ht="32">
       <c r="A13" s="7" t="s">
         <v>26</v>
       </c>
@@ -1591,7 +2042,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" ht="16">
       <c r="A14" s="7" t="s">
         <v>29</v>
       </c>
@@ -1600,7 +2051,7 @@
       </c>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:16" ht="30">
+    <row r="15" spans="1:16" ht="32">
       <c r="A15" s="10" t="s">
         <v>31</v>
       </c>
@@ -1609,7 +2060,7 @@
       </c>
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:16" ht="30">
+    <row r="16" spans="1:16" ht="32">
       <c r="A16" s="10" t="s">
         <v>33</v>
       </c>
@@ -1618,7 +2069,7 @@
       </c>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" ht="16">
       <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
@@ -1627,7 +2078,7 @@
       </c>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:3" ht="60">
+    <row r="18" spans="1:3" ht="64">
       <c r="A18" s="10" t="s">
         <v>37</v>
       </c>
@@ -1636,7 +2087,7 @@
       </c>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:3" ht="105">
+    <row r="19" spans="1:3" ht="112">
       <c r="A19" s="10" t="s">
         <v>39</v>
       </c>
@@ -1645,7 +2096,7 @@
       </c>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" ht="16">
       <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
@@ -1656,7 +2107,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" ht="16">
       <c r="A21" s="4" t="s">
         <v>44</v>
       </c>
@@ -1665,7 +2116,7 @@
       </c>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" ht="16">
       <c r="A22" s="4" t="s">
         <v>46</v>
       </c>
@@ -1674,7 +2125,7 @@
       </c>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" ht="16">
       <c r="A23" s="4" t="s">
         <v>48</v>
       </c>
@@ -1683,7 +2134,7 @@
       </c>
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" ht="16">
       <c r="A24" s="4" t="s">
         <v>50</v>
       </c>
@@ -1692,7 +2143,7 @@
       </c>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+    <row r="25" spans="1:3" ht="16">
       <c r="A25" s="4" t="s">
         <v>52</v>
       </c>
@@ -1701,7 +2152,7 @@
       </c>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+    <row r="26" spans="1:3" ht="16">
       <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
@@ -1710,7 +2161,7 @@
       </c>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1">
+    <row r="27" spans="1:3" ht="16">
       <c r="A27" s="4" t="s">
         <v>56</v>
       </c>
@@ -1719,7 +2170,7 @@
       </c>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+    <row r="28" spans="1:3" ht="16">
       <c r="A28" s="4" t="s">
         <v>58</v>
       </c>
@@ -1728,7 +2179,7 @@
       </c>
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+    <row r="29" spans="1:3" ht="112">
       <c r="A29" s="10" t="s">
         <v>60</v>
       </c>
@@ -1737,7 +2188,7 @@
       </c>
       <c r="C29" s="8"/>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1">
+    <row r="30" spans="1:3" ht="16">
       <c r="A30" s="4" t="s">
         <v>16</v>
       </c>
@@ -1746,7 +2197,7 @@
       </c>
       <c r="C30" s="8"/>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1">
+    <row r="31" spans="1:3" ht="16">
       <c r="A31" s="4" t="s">
         <v>62</v>
       </c>
@@ -1755,7 +2206,7 @@
       </c>
       <c r="C31" s="8"/>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1">
+    <row r="32" spans="1:3" ht="16">
       <c r="A32" s="4" t="s">
         <v>64</v>
       </c>
@@ -1764,7 +2215,7 @@
       </c>
       <c r="C32" s="8"/>
     </row>
-    <row r="33" spans="1:23" ht="15.75" customHeight="1">
+    <row r="33" spans="1:23" ht="16">
       <c r="A33" s="4" t="s">
         <v>66</v>
       </c>
@@ -1773,7 +2224,7 @@
       </c>
       <c r="C33" s="8"/>
     </row>
-    <row r="34" spans="1:23" ht="15.75" customHeight="1">
+    <row r="34" spans="1:23" ht="16">
       <c r="A34" s="4" t="s">
         <v>68</v>
       </c>
@@ -1782,7 +2233,7 @@
       </c>
       <c r="C34" s="8"/>
     </row>
-    <row r="35" spans="1:23" ht="15.75" customHeight="1">
+    <row r="35" spans="1:23" ht="16">
       <c r="A35" s="4" t="s">
         <v>70</v>
       </c>
@@ -1791,7 +2242,7 @@
       </c>
       <c r="C35" s="8"/>
     </row>
-    <row r="36" spans="1:23" ht="15.75" customHeight="1">
+    <row r="36" spans="1:23" ht="16">
       <c r="A36" s="4" t="s">
         <v>72</v>
       </c>
@@ -1800,7 +2251,7 @@
       </c>
       <c r="C36" s="8"/>
     </row>
-    <row r="37" spans="1:23" ht="15.75" customHeight="1">
+    <row r="37" spans="1:23" ht="16">
       <c r="A37" s="4" t="s">
         <v>74</v>
       </c>
@@ -1809,7 +2260,7 @@
       </c>
       <c r="C37" s="8"/>
     </row>
-    <row r="38" spans="1:23" ht="15.75" customHeight="1">
+    <row r="38" spans="1:23" ht="64">
       <c r="A38" s="10" t="s">
         <v>37</v>
       </c>
@@ -1818,7 +2269,7 @@
       </c>
       <c r="C38" s="8"/>
     </row>
-    <row r="39" spans="1:23" ht="15.75" customHeight="1">
+    <row r="39" spans="1:23" ht="160">
       <c r="A39" s="10" t="s">
         <v>76</v>
       </c>
@@ -1827,7 +2278,7 @@
       </c>
       <c r="C39" s="8"/>
     </row>
-    <row r="40" spans="1:23" ht="15.75" customHeight="1">
+    <row r="40" spans="1:23" ht="128">
       <c r="A40" s="10" t="s">
         <v>78</v>
       </c>
@@ -1836,7 +2287,7 @@
       </c>
       <c r="C40" s="8"/>
     </row>
-    <row r="41" spans="1:23" ht="15.75" customHeight="1">
+    <row r="41" spans="1:23" ht="16">
       <c r="A41" s="4" t="s">
         <v>80</v>
       </c>
@@ -1845,7 +2296,7 @@
       </c>
       <c r="C41" s="8"/>
     </row>
-    <row r="42" spans="1:23" ht="15.75" customHeight="1">
+    <row r="42" spans="1:23" ht="32">
       <c r="A42" s="10" t="s">
         <v>82</v>
       </c>
@@ -1854,7 +2305,7 @@
       </c>
       <c r="C42" s="8"/>
     </row>
-    <row r="43" spans="1:23" ht="15.75" customHeight="1">
+    <row r="43" spans="1:23" ht="48">
       <c r="A43" s="4" t="s">
         <v>84</v>
       </c>
@@ -1863,7 +2314,7 @@
       </c>
       <c r="C43" s="8"/>
     </row>
-    <row r="44" spans="1:23" ht="15.75" customHeight="1">
+    <row r="44" spans="1:23" ht="32">
       <c r="A44" s="4" t="s">
         <v>86</v>
       </c>
@@ -1872,7 +2323,7 @@
       </c>
       <c r="C44" s="8"/>
     </row>
-    <row r="45" spans="1:23" ht="15.75" customHeight="1">
+    <row r="45" spans="1:23" ht="16">
       <c r="A45" s="4" t="s">
         <v>88</v>
       </c>
@@ -1881,7 +2332,7 @@
       </c>
       <c r="C45" s="8"/>
     </row>
-    <row r="46" spans="1:23" ht="15.75" customHeight="1">
+    <row r="46" spans="1:23" ht="16">
       <c r="A46" s="4" t="s">
         <v>90</v>
       </c>
@@ -1910,7 +2361,7 @@
       <c r="V46" s="11"/>
       <c r="W46" s="11"/>
     </row>
-    <row r="47" spans="1:23" ht="15.75" customHeight="1">
+    <row r="47" spans="1:23" ht="96">
       <c r="A47" s="10" t="s">
         <v>91</v>
       </c>
@@ -1919,7 +2370,7 @@
       </c>
       <c r="C47" s="8"/>
     </row>
-    <row r="48" spans="1:23" ht="15.75" customHeight="1">
+    <row r="48" spans="1:23" ht="64">
       <c r="A48" s="10" t="s">
         <v>93</v>
       </c>
@@ -1928,7 +2379,7 @@
       </c>
       <c r="C48" s="8"/>
     </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1">
+    <row r="49" spans="1:3" ht="32">
       <c r="A49" s="4" t="s">
         <v>95</v>
       </c>
@@ -1937,7 +2388,7 @@
       </c>
       <c r="C49" s="8"/>
     </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1">
+    <row r="50" spans="1:3" ht="176">
       <c r="A50" s="10" t="s">
         <v>97</v>
       </c>
@@ -1946,7 +2397,7 @@
       </c>
       <c r="C50" s="8"/>
     </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1">
+    <row r="51" spans="1:3" ht="16">
       <c r="A51" s="4" t="s">
         <v>99</v>
       </c>
@@ -1955,7 +2406,7 @@
       </c>
       <c r="C51" s="8"/>
     </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1">
+    <row r="52" spans="1:3" ht="16">
       <c r="A52" s="4" t="s">
         <v>101</v>
       </c>
@@ -1964,7 +2415,7 @@
       </c>
       <c r="C52" s="8"/>
     </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1">
+    <row r="53" spans="1:3" ht="16">
       <c r="A53" s="12" t="s">
         <v>103</v>
       </c>
@@ -1973,7 +2424,7 @@
       </c>
       <c r="C53" s="8"/>
     </row>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1">
+    <row r="54" spans="1:3" ht="48">
       <c r="A54" s="12" t="s">
         <v>105</v>
       </c>
@@ -1982,7 +2433,7 @@
       </c>
       <c r="C54" s="8"/>
     </row>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1">
+    <row r="55" spans="1:3" ht="32">
       <c r="A55" s="13" t="s">
         <v>107</v>
       </c>
@@ -1991,7 +2442,7 @@
       </c>
       <c r="C55" s="8"/>
     </row>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1">
+    <row r="56" spans="1:3" ht="112">
       <c r="A56" s="13" t="s">
         <v>109</v>
       </c>
@@ -2000,7 +2451,7 @@
       </c>
       <c r="C56" s="8"/>
     </row>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1">
+    <row r="57" spans="1:3" ht="32">
       <c r="A57" s="13" t="s">
         <v>111</v>
       </c>
@@ -2009,7 +2460,7 @@
       </c>
       <c r="C57" s="8"/>
     </row>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1">
+    <row r="58" spans="1:3" ht="32">
       <c r="A58" s="14" t="s">
         <v>113</v>
       </c>
@@ -2018,7 +2469,7 @@
       </c>
       <c r="C58" s="8"/>
     </row>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1">
+    <row r="59" spans="1:3" ht="48">
       <c r="A59" s="12" t="s">
         <v>115</v>
       </c>
@@ -2027,7 +2478,7 @@
       </c>
       <c r="C59" s="8"/>
     </row>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1">
+    <row r="60" spans="1:3" ht="16">
       <c r="A60" s="12" t="s">
         <v>117</v>
       </c>
@@ -2036,7 +2487,7 @@
       </c>
       <c r="C60" s="8"/>
     </row>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1">
+    <row r="61" spans="1:3" ht="16">
       <c r="A61" s="12" t="s">
         <v>119</v>
       </c>
@@ -2045,7 +2496,7 @@
       </c>
       <c r="C61" s="8"/>
     </row>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1">
+    <row r="62" spans="1:3" ht="64">
       <c r="A62" s="12" t="s">
         <v>121</v>
       </c>
@@ -2054,7 +2505,7 @@
       </c>
       <c r="C62" s="8"/>
     </row>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1">
+    <row r="63" spans="1:3" ht="16">
       <c r="A63" s="12" t="s">
         <v>123</v>
       </c>
@@ -2063,7 +2514,7 @@
       </c>
       <c r="C63" s="8"/>
     </row>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1">
+    <row r="64" spans="1:3" ht="16">
       <c r="A64" s="12" t="s">
         <v>125</v>
       </c>
@@ -2072,7 +2523,7 @@
       </c>
       <c r="C64" s="8"/>
     </row>
-    <row r="65" spans="1:4" ht="15.75" customHeight="1">
+    <row r="65" spans="1:4" ht="16">
       <c r="A65" s="12" t="s">
         <v>127</v>
       </c>
@@ -2081,7 +2532,7 @@
       </c>
       <c r="C65" s="8"/>
     </row>
-    <row r="66" spans="1:4" ht="15.75" customHeight="1">
+    <row r="66" spans="1:4" ht="16">
       <c r="A66" s="13" t="s">
         <v>129</v>
       </c>
@@ -2090,7 +2541,7 @@
       </c>
       <c r="C66" s="17"/>
     </row>
-    <row r="67" spans="1:4" ht="15.75" customHeight="1">
+    <row r="67" spans="1:4" ht="45">
       <c r="A67" s="18" t="s">
         <v>131</v>
       </c>
@@ -2101,7 +2552,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.75" customHeight="1">
+    <row r="68" spans="1:4" ht="16">
       <c r="A68" s="13" t="s">
         <v>134</v>
       </c>
@@ -2112,7 +2563,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.75" customHeight="1">
+    <row r="69" spans="1:4" ht="32">
       <c r="A69" s="20" t="s">
         <v>137</v>
       </c>
@@ -2123,7 +2574,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15.75" customHeight="1">
+    <row r="70" spans="1:4" ht="30">
       <c r="A70" s="22" t="s">
         <v>140</v>
       </c>
@@ -2134,7 +2585,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.75" customHeight="1">
+    <row r="71" spans="1:4" ht="16">
       <c r="A71" s="24" t="s">
         <v>142</v>
       </c>
@@ -2145,7 +2596,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1">
+    <row r="72" spans="1:4" ht="16">
       <c r="A72" s="10" t="s">
         <v>144</v>
       </c>
@@ -2154,7 +2605,7 @@
       </c>
       <c r="C72" s="8"/>
     </row>
-    <row r="73" spans="1:4" ht="15.75" customHeight="1">
+    <row r="73" spans="1:4" ht="16">
       <c r="A73" s="4" t="s">
         <v>146</v>
       </c>
@@ -2163,7 +2614,7 @@
       </c>
       <c r="C73" s="8"/>
     </row>
-    <row r="74" spans="1:4" ht="15.75" customHeight="1">
+    <row r="74" spans="1:4" ht="16">
       <c r="A74" s="4" t="s">
         <v>148</v>
       </c>
@@ -2172,7 +2623,7 @@
       </c>
       <c r="C74" s="8"/>
     </row>
-    <row r="75" spans="1:4" ht="15.75" customHeight="1">
+    <row r="75" spans="1:4" ht="16">
       <c r="A75" s="4" t="s">
         <v>150</v>
       </c>
@@ -2181,7 +2632,7 @@
       </c>
       <c r="C75" s="8"/>
     </row>
-    <row r="76" spans="1:4" ht="15.75" customHeight="1">
+    <row r="76" spans="1:4" ht="16">
       <c r="A76" s="10" t="s">
         <v>152</v>
       </c>
@@ -2192,7 +2643,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.75" customHeight="1">
+    <row r="77" spans="1:4">
       <c r="A77" s="26" t="s">
         <v>154</v>
       </c>
@@ -2203,7 +2654,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15.75" customHeight="1">
+    <row r="78" spans="1:4" ht="16">
       <c r="A78" s="4" t="s">
         <v>157</v>
       </c>
@@ -2212,7 +2663,7 @@
       </c>
       <c r="C78" s="8"/>
     </row>
-    <row r="79" spans="1:4" ht="15.75" customHeight="1">
+    <row r="79" spans="1:4" ht="16">
       <c r="A79" s="24" t="s">
         <v>159</v>
       </c>
@@ -2222,7 +2673,7 @@
       <c r="C79" s="28"/>
       <c r="D79" s="29"/>
     </row>
-    <row r="80" spans="1:4" ht="15.75" customHeight="1">
+    <row r="80" spans="1:4" ht="16">
       <c r="A80" s="12" t="s">
         <v>161</v>
       </c>
@@ -2231,7 +2682,7 @@
       </c>
       <c r="C80" s="8"/>
     </row>
-    <row r="81" spans="1:4" ht="15.75" customHeight="1">
+    <row r="81" spans="1:4" ht="90">
       <c r="A81" s="13" t="s">
         <v>163</v>
       </c>
@@ -2242,7 +2693,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.75" customHeight="1">
+    <row r="82" spans="1:4" ht="32">
       <c r="A82" s="13" t="s">
         <v>165</v>
       </c>
@@ -2253,7 +2704,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.75" customHeight="1">
+    <row r="83" spans="1:4" ht="80">
       <c r="A83" s="30" t="s">
         <v>167</v>
       </c>
@@ -2264,7 +2715,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.75" customHeight="1">
+    <row r="84" spans="1:4" ht="48">
       <c r="A84" s="13" t="s">
         <v>169</v>
       </c>
@@ -2275,7 +2726,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.75" customHeight="1">
+    <row r="85" spans="1:4" ht="90">
       <c r="A85" s="30" t="s">
         <v>171</v>
       </c>
@@ -2286,7 +2737,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15.75" customHeight="1">
+    <row r="86" spans="1:4" ht="120">
       <c r="A86" s="30" t="s">
         <v>173</v>
       </c>
@@ -2297,7 +2748,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.75" customHeight="1">
+    <row r="87" spans="1:4" ht="60">
       <c r="A87" s="30" t="s">
         <v>175</v>
       </c>
@@ -2308,7 +2759,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.75" customHeight="1">
+    <row r="88" spans="1:4" ht="60">
       <c r="A88" s="30" t="s">
         <v>177</v>
       </c>
@@ -2319,7 +2770,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.75" customHeight="1">
+    <row r="89" spans="1:4" ht="45">
       <c r="A89" s="30" t="s">
         <v>179</v>
       </c>
@@ -2330,7 +2781,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.75" customHeight="1">
+    <row r="90" spans="1:4" ht="91">
       <c r="A90" s="30" t="s">
         <v>181</v>
       </c>
@@ -2344,7 +2795,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.75" customHeight="1">
+    <row r="91" spans="1:4" ht="16">
       <c r="A91" s="14" t="s">
         <v>184</v>
       </c>
@@ -2353,7 +2804,7 @@
       </c>
       <c r="C91" s="8"/>
     </row>
-    <row r="92" spans="1:4" ht="15.75" customHeight="1">
+    <row r="92" spans="1:4" ht="16">
       <c r="A92" s="12" t="s">
         <v>186</v>
       </c>
@@ -2362,7 +2813,7 @@
       </c>
       <c r="C92" s="8"/>
     </row>
-    <row r="93" spans="1:4" ht="15.75" customHeight="1">
+    <row r="93" spans="1:4" ht="16">
       <c r="A93" s="12" t="s">
         <v>188</v>
       </c>
@@ -2371,7 +2822,7 @@
       </c>
       <c r="C93" s="8"/>
     </row>
-    <row r="94" spans="1:4" ht="15.75" customHeight="1">
+    <row r="94" spans="1:4" ht="32">
       <c r="A94" s="12" t="s">
         <v>190</v>
       </c>
@@ -2380,7 +2831,7 @@
       </c>
       <c r="C94" s="8"/>
     </row>
-    <row r="95" spans="1:4" ht="15.75" customHeight="1">
+    <row r="95" spans="1:4">
       <c r="A95" s="30" t="s">
         <v>192</v>
       </c>
@@ -2391,7 +2842,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="67.5" customHeight="1">
+    <row r="96" spans="1:4" ht="48">
       <c r="A96" s="32" t="s">
         <v>194</v>
       </c>
@@ -2400,7 +2851,7 @@
       </c>
       <c r="C96" s="8"/>
     </row>
-    <row r="97" spans="1:3" ht="15.75" customHeight="1">
+    <row r="97" spans="1:3" ht="48">
       <c r="A97" s="12" t="s">
         <v>196</v>
       </c>
@@ -2409,7 +2860,7 @@
       </c>
       <c r="C97" s="8"/>
     </row>
-    <row r="98" spans="1:3" ht="15.75" customHeight="1">
+    <row r="98" spans="1:3" ht="16">
       <c r="A98" s="12" t="s">
         <v>198</v>
       </c>
@@ -2418,7 +2869,7 @@
       </c>
       <c r="C98" s="8"/>
     </row>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1">
+    <row r="99" spans="1:3" ht="32">
       <c r="A99" s="12" t="s">
         <v>200</v>
       </c>
@@ -2427,7 +2878,7 @@
       </c>
       <c r="C99" s="8"/>
     </row>
-    <row r="100" spans="1:3" ht="15.75" customHeight="1">
+    <row r="100" spans="1:3" ht="16">
       <c r="A100" s="12" t="s">
         <v>202</v>
       </c>
@@ -2436,7 +2887,7 @@
       </c>
       <c r="C100" s="8"/>
     </row>
-    <row r="101" spans="1:3" ht="15.75" customHeight="1">
+    <row r="101" spans="1:3" ht="16">
       <c r="A101" s="12" t="s">
         <v>204</v>
       </c>
@@ -2445,7 +2896,7 @@
       </c>
       <c r="C101" s="8"/>
     </row>
-    <row r="102" spans="1:3" ht="15.75" customHeight="1">
+    <row r="102" spans="1:3" ht="32">
       <c r="A102" s="12" t="s">
         <v>206</v>
       </c>
@@ -2454,7 +2905,7 @@
       </c>
       <c r="C102" s="8"/>
     </row>
-    <row r="103" spans="1:3" ht="15.75" customHeight="1">
+    <row r="103" spans="1:3" ht="16">
       <c r="A103" s="12" t="s">
         <v>208</v>
       </c>
@@ -2463,7 +2914,7 @@
       </c>
       <c r="C103" s="8"/>
     </row>
-    <row r="104" spans="1:3" ht="15.75" customHeight="1">
+    <row r="104" spans="1:3" ht="16">
       <c r="A104" s="12" t="s">
         <v>210</v>
       </c>
@@ -2472,7 +2923,7 @@
       </c>
       <c r="C104" s="8"/>
     </row>
-    <row r="105" spans="1:3" ht="15.75" customHeight="1">
+    <row r="105" spans="1:3" ht="16">
       <c r="A105" s="12" t="s">
         <v>212</v>
       </c>
@@ -2481,7 +2932,7 @@
       </c>
       <c r="C105" s="8"/>
     </row>
-    <row r="106" spans="1:3" ht="15.75" customHeight="1">
+    <row r="106" spans="1:3" ht="16">
       <c r="A106" s="12" t="s">
         <v>214</v>
       </c>
@@ -2490,7 +2941,7 @@
       </c>
       <c r="C106" s="8"/>
     </row>
-    <row r="107" spans="1:3" ht="15.75" customHeight="1">
+    <row r="107" spans="1:3" ht="16">
       <c r="A107" s="12" t="s">
         <v>216</v>
       </c>
@@ -2499,7 +2950,7 @@
       </c>
       <c r="C107" s="8"/>
     </row>
-    <row r="108" spans="1:3" ht="15.75" customHeight="1">
+    <row r="108" spans="1:3" ht="16">
       <c r="A108" s="12" t="s">
         <v>218</v>
       </c>
@@ -2508,7 +2959,7 @@
       </c>
       <c r="C108" s="8"/>
     </row>
-    <row r="109" spans="1:3" ht="15.75" customHeight="1">
+    <row r="109" spans="1:3" ht="16">
       <c r="A109" s="12" t="s">
         <v>220</v>
       </c>
@@ -2517,7 +2968,7 @@
       </c>
       <c r="C109" s="8"/>
     </row>
-    <row r="110" spans="1:3" ht="15.75" customHeight="1">
+    <row r="110" spans="1:3" ht="16">
       <c r="A110" s="12" t="s">
         <v>222</v>
       </c>
@@ -2526,7 +2977,7 @@
       </c>
       <c r="C110" s="8"/>
     </row>
-    <row r="111" spans="1:3" ht="15.75" customHeight="1">
+    <row r="111" spans="1:3" ht="16">
       <c r="A111" s="12" t="s">
         <v>224</v>
       </c>
@@ -2535,7 +2986,7 @@
       </c>
       <c r="C111" s="8"/>
     </row>
-    <row r="112" spans="1:3" ht="15.75" customHeight="1">
+    <row r="112" spans="1:3" ht="16">
       <c r="A112" s="12" t="s">
         <v>226</v>
       </c>
@@ -2544,7 +2995,7 @@
       </c>
       <c r="C112" s="8"/>
     </row>
-    <row r="113" spans="1:3" ht="15.75" customHeight="1">
+    <row r="113" spans="1:3" ht="16">
       <c r="A113" s="12" t="s">
         <v>228</v>
       </c>
@@ -2553,7 +3004,7 @@
       </c>
       <c r="C113" s="8"/>
     </row>
-    <row r="114" spans="1:3" ht="15.75" customHeight="1">
+    <row r="114" spans="1:3" ht="16">
       <c r="A114" s="12" t="s">
         <v>230</v>
       </c>
@@ -2562,7 +3013,7 @@
       </c>
       <c r="C114" s="8"/>
     </row>
-    <row r="115" spans="1:3" ht="15.75" customHeight="1">
+    <row r="115" spans="1:3" ht="16">
       <c r="A115" s="12" t="s">
         <v>232</v>
       </c>
@@ -2571,7 +3022,7 @@
       </c>
       <c r="C115" s="8"/>
     </row>
-    <row r="116" spans="1:3" ht="15.75" customHeight="1">
+    <row r="116" spans="1:3" ht="16">
       <c r="A116" s="34" t="s">
         <v>234</v>
       </c>
@@ -2580,7 +3031,7 @@
       </c>
       <c r="C116" s="8"/>
     </row>
-    <row r="117" spans="1:3" ht="15.75" customHeight="1">
+    <row r="117" spans="1:3" ht="16">
       <c r="A117" s="24" t="s">
         <v>236</v>
       </c>
@@ -2589,7 +3040,7 @@
       </c>
       <c r="C117" s="8"/>
     </row>
-    <row r="118" spans="1:3" ht="90" customHeight="1">
+    <row r="118" spans="1:3" ht="96">
       <c r="A118" s="14" t="s">
         <v>237</v>
       </c>
@@ -2598,7 +3049,7 @@
       </c>
       <c r="C118" s="8"/>
     </row>
-    <row r="119" spans="1:3" ht="15.75" customHeight="1">
+    <row r="119" spans="1:3" ht="16">
       <c r="A119" s="24" t="s">
         <v>239</v>
       </c>
@@ -2607,7 +3058,7 @@
       </c>
       <c r="C119" s="8"/>
     </row>
-    <row r="120" spans="1:3" ht="15.75" customHeight="1">
+    <row r="120" spans="1:3" ht="16">
       <c r="A120" s="24" t="s">
         <v>241</v>
       </c>
@@ -2616,7 +3067,7 @@
       </c>
       <c r="C120" s="8"/>
     </row>
-    <row r="121" spans="1:3" ht="15.75" customHeight="1">
+    <row r="121" spans="1:3" ht="16">
       <c r="A121" s="24" t="s">
         <v>243</v>
       </c>
@@ -2625,7 +3076,7 @@
       </c>
       <c r="C121" s="8"/>
     </row>
-    <row r="122" spans="1:3" ht="15.75" customHeight="1">
+    <row r="122" spans="1:3" ht="16">
       <c r="A122" s="24" t="s">
         <v>245</v>
       </c>
@@ -2634,7 +3085,7 @@
       </c>
       <c r="C122" s="8"/>
     </row>
-    <row r="123" spans="1:3" ht="15.75" customHeight="1">
+    <row r="123" spans="1:3" ht="16">
       <c r="A123" s="24" t="s">
         <v>247</v>
       </c>
@@ -2643,7 +3094,7 @@
       </c>
       <c r="C123" s="8"/>
     </row>
-    <row r="124" spans="1:3" ht="15.75" customHeight="1">
+    <row r="124" spans="1:3" ht="16">
       <c r="A124" s="14" t="s">
         <v>249</v>
       </c>
@@ -2652,7 +3103,7 @@
       </c>
       <c r="C124" s="8"/>
     </row>
-    <row r="125" spans="1:3" ht="15.75" customHeight="1">
+    <row r="125" spans="1:3" ht="16">
       <c r="A125" s="24" t="s">
         <v>251</v>
       </c>
@@ -2661,7 +3112,7 @@
       </c>
       <c r="C125" s="8"/>
     </row>
-    <row r="126" spans="1:3" ht="82.5" customHeight="1">
+    <row r="126" spans="1:3" ht="80">
       <c r="A126" s="24" t="s">
         <v>253</v>
       </c>
@@ -2670,7 +3121,7 @@
       </c>
       <c r="C126" s="8"/>
     </row>
-    <row r="127" spans="1:3" ht="15.75" customHeight="1">
+    <row r="127" spans="1:3" ht="32">
       <c r="A127" s="24" t="s">
         <v>255</v>
       </c>
@@ -2679,7 +3130,7 @@
       </c>
       <c r="C127" s="8"/>
     </row>
-    <row r="128" spans="1:3" ht="17.25" customHeight="1">
+    <row r="128" spans="1:3" ht="16">
       <c r="A128" s="24" t="s">
         <v>257</v>
       </c>
@@ -2688,7 +3139,7 @@
       </c>
       <c r="C128" s="8"/>
     </row>
-    <row r="129" spans="1:2" ht="15.75" customHeight="1">
+    <row r="129" spans="1:2" ht="34">
       <c r="A129" s="35" t="s">
         <v>259</v>
       </c>
@@ -2696,7 +3147,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="15.75" customHeight="1">
+    <row r="130" spans="1:2" ht="16">
       <c r="A130" s="37" t="s">
         <v>261</v>
       </c>
@@ -2704,7 +3155,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="15.75" customHeight="1">
+    <row r="131" spans="1:2" ht="32">
       <c r="A131" s="35" t="s">
         <v>263</v>
       </c>
@@ -2712,7 +3163,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="16.5" customHeight="1">
+    <row r="132" spans="1:2" ht="17">
       <c r="A132" s="35" t="s">
         <v>265</v>
       </c>
@@ -2720,7 +3171,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="15.75" customHeight="1">
+    <row r="133" spans="1:2" ht="34">
       <c r="A133" s="35" t="s">
         <v>267</v>
       </c>
@@ -2728,7 +3179,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="15.75" customHeight="1">
+    <row r="134" spans="1:2" ht="34">
       <c r="A134" s="35" t="s">
         <v>269</v>
       </c>
@@ -2736,7 +3187,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="15.75" customHeight="1">
+    <row r="135" spans="1:2" ht="17">
       <c r="A135" s="38" t="s">
         <v>271</v>
       </c>
@@ -2744,7 +3195,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="15.75" customHeight="1">
+    <row r="136" spans="1:2" ht="17">
       <c r="A136" s="38" t="s">
         <v>273</v>
       </c>
@@ -2752,7 +3203,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="39.75" customHeight="1">
+    <row r="137" spans="1:2" ht="51">
       <c r="A137" s="38" t="s">
         <v>275</v>
       </c>
@@ -2760,7 +3211,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="15.75" customHeight="1">
+    <row r="138" spans="1:2" ht="34">
       <c r="A138" s="38" t="s">
         <v>277</v>
       </c>
@@ -2768,7 +3219,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="15.75" customHeight="1">
+    <row r="139" spans="1:2" ht="17">
       <c r="A139" s="38" t="s">
         <v>279</v>
       </c>
@@ -2776,7 +3227,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="15.75" customHeight="1">
+    <row r="140" spans="1:2" ht="17">
       <c r="A140" s="38" t="s">
         <v>281</v>
       </c>
@@ -2784,7 +3235,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="15.75" customHeight="1">
+    <row r="141" spans="1:2" ht="17">
       <c r="A141" s="38" t="s">
         <v>283</v>
       </c>
@@ -2792,15 +3243,15 @@
         <v>284</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="15.75" customHeight="1">
+    <row r="142" spans="1:2" ht="17">
       <c r="A142" s="38" t="s">
         <v>292</v>
       </c>
-      <c r="B142" s="43" t="s">
+      <c r="B142" s="41" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="15.75" customHeight="1">
+    <row r="143" spans="1:2" ht="17">
       <c r="A143" s="38" t="s">
         <v>285</v>
       </c>
@@ -2808,7 +3259,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="15.75" customHeight="1">
+    <row r="144" spans="1:2" ht="17">
       <c r="A144" s="38" t="s">
         <v>287</v>
       </c>
@@ -2816,196 +3267,519 @@
         <v>288</v>
       </c>
     </row>
-    <row r="145" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A145" s="40"/>
-    </row>
-    <row r="146" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A146" s="40"/>
-    </row>
-    <row r="147" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A147" s="40"/>
-    </row>
-    <row r="148" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A148" s="40"/>
-    </row>
-    <row r="149" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A149" s="40"/>
-    </row>
-    <row r="150" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A150" s="40"/>
-    </row>
-    <row r="151" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A151" s="40"/>
-    </row>
-    <row r="152" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A152" s="40"/>
-    </row>
-    <row r="153" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A153" s="40"/>
-    </row>
-    <row r="154" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A154" s="40"/>
-    </row>
-    <row r="155" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A155" s="40"/>
-    </row>
-    <row r="156" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A156" s="40"/>
-    </row>
-    <row r="157" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A157" s="40"/>
-    </row>
-    <row r="158" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A158" s="40"/>
-    </row>
-    <row r="159" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A159" s="40"/>
-    </row>
-    <row r="160" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A160" s="40"/>
-    </row>
-    <row r="161" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A161" s="40"/>
-    </row>
-    <row r="162" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A162" s="40"/>
-    </row>
-    <row r="163" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A163" s="40"/>
-    </row>
-    <row r="164" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A164" s="40"/>
-    </row>
-    <row r="165" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A165" s="40"/>
-    </row>
-    <row r="166" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A166" s="40"/>
-    </row>
-    <row r="167" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A167" s="40"/>
-    </row>
-    <row r="168" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A168" s="40"/>
-    </row>
-    <row r="169" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A169" s="40"/>
-    </row>
-    <row r="170" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A170" s="40"/>
-    </row>
-    <row r="171" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A171" s="40"/>
-    </row>
-    <row r="172" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A172" s="40"/>
-    </row>
-    <row r="173" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A173" s="40"/>
-    </row>
-    <row r="174" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A174" s="40"/>
-    </row>
-    <row r="175" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A175" s="40"/>
-    </row>
-    <row r="176" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A176" s="40"/>
-    </row>
-    <row r="177" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A177" s="40"/>
-    </row>
-    <row r="178" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A178" s="40"/>
-    </row>
-    <row r="179" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A179" s="40"/>
-    </row>
-    <row r="180" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A180" s="40"/>
-    </row>
-    <row r="181" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A181" s="40"/>
-    </row>
-    <row r="182" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A182" s="40"/>
-    </row>
-    <row r="183" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A183" s="40"/>
-    </row>
-    <row r="184" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A184" s="40"/>
-    </row>
-    <row r="185" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A185" s="40"/>
-    </row>
-    <row r="186" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A186" s="40"/>
-    </row>
-    <row r="187" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A187" s="40"/>
-    </row>
-    <row r="188" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A188" s="40"/>
-    </row>
-    <row r="189" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A189" s="40"/>
-    </row>
-    <row r="190" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A190" s="40"/>
-    </row>
-    <row r="191" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A191" s="40"/>
-    </row>
-    <row r="192" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A192" s="40"/>
-    </row>
-    <row r="193" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A193" s="40"/>
-    </row>
-    <row r="194" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A194" s="40"/>
-    </row>
-    <row r="195" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A195" s="40"/>
-    </row>
-    <row r="196" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A196" s="40"/>
-    </row>
-    <row r="197" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A197" s="40"/>
-    </row>
-    <row r="198" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A198" s="40"/>
-    </row>
-    <row r="199" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A199" s="40"/>
-    </row>
-    <row r="200" spans="1:1" ht="15.75" customHeight="1">
+    <row r="145" spans="1:2" ht="17">
+      <c r="A145" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="B145" s="41" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="64">
+      <c r="A146" s="40" t="s">
+        <v>296</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="17">
+      <c r="A147" s="40" t="s">
+        <v>297</v>
+      </c>
+      <c r="B147" s="41" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="51">
+      <c r="A148" s="40" t="s">
+        <v>299</v>
+      </c>
+      <c r="B148" s="41" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="119">
+      <c r="A149" s="41" t="s">
+        <v>301</v>
+      </c>
+      <c r="B149" s="40" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="17">
+      <c r="A150" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="B150" s="41" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="68">
+      <c r="A151" s="40" t="s">
+        <v>305</v>
+      </c>
+      <c r="B151" s="41" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="17">
+      <c r="A152" s="41" t="s">
+        <v>306</v>
+      </c>
+      <c r="B152" s="40" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" s="41" t="s">
+        <v>307</v>
+      </c>
+      <c r="B153" s="41" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="17">
+      <c r="A154" s="47" t="s">
+        <v>314</v>
+      </c>
+      <c r="B154" s="45" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="16">
+      <c r="A155" s="53" t="s">
+        <v>315</v>
+      </c>
+      <c r="B155" s="48" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="16">
+      <c r="A156" s="53" t="s">
+        <v>316</v>
+      </c>
+      <c r="B156" s="44" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="16">
+      <c r="A157" s="53" t="s">
+        <v>317</v>
+      </c>
+      <c r="B157" s="44" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="16">
+      <c r="A158" s="53" t="s">
+        <v>318</v>
+      </c>
+      <c r="B158" s="44" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="16">
+      <c r="A159" s="53" t="s">
+        <v>326</v>
+      </c>
+      <c r="B159" s="44" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="16">
+      <c r="A160" s="53" t="s">
+        <v>327</v>
+      </c>
+      <c r="B160" s="44" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" ht="16">
+      <c r="A161" s="53" t="s">
+        <v>328</v>
+      </c>
+      <c r="B161" s="44" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="166">
+      <c r="A162" s="53" t="s">
+        <v>329</v>
+      </c>
+      <c r="B162" s="44" t="s">
+        <v>334</v>
+      </c>
+      <c r="H162" s="46" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="91">
+      <c r="A163" s="53" t="s">
+        <v>330</v>
+      </c>
+      <c r="B163" s="44" t="s">
+        <v>324</v>
+      </c>
+      <c r="H163" s="46" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" ht="409.6">
+      <c r="A164" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="B164" s="44" t="s">
+        <v>335</v>
+      </c>
+      <c r="H164" s="46" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" ht="16">
+      <c r="A165" s="53" t="s">
+        <v>331</v>
+      </c>
+      <c r="B165" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="H165" s="50" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" ht="121">
+      <c r="A166" s="53" t="s">
+        <v>332</v>
+      </c>
+      <c r="B166" s="44" t="s">
+        <v>336</v>
+      </c>
+      <c r="H166" s="46" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" ht="409.6">
+      <c r="A167" s="53" t="s">
+        <v>333</v>
+      </c>
+      <c r="B167" s="44" t="s">
+        <v>337</v>
+      </c>
+      <c r="H167" s="46" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" ht="409.6">
+      <c r="A168" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="B168" s="44" t="s">
+        <v>339</v>
+      </c>
+      <c r="H168" s="46" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="409.6">
+      <c r="A169" s="53" t="s">
+        <v>349</v>
+      </c>
+      <c r="B169" s="44" t="s">
+        <v>340</v>
+      </c>
+      <c r="H169" s="46" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" ht="106">
+      <c r="A170" s="53" t="s">
+        <v>350</v>
+      </c>
+      <c r="B170" s="44" t="s">
+        <v>341</v>
+      </c>
+      <c r="H170" s="46" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" ht="409.6">
+      <c r="A171" s="53" t="s">
+        <v>351</v>
+      </c>
+      <c r="B171" s="44" t="s">
+        <v>342</v>
+      </c>
+      <c r="H171" s="46" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" ht="409.6">
+      <c r="A172" s="53" t="s">
+        <v>352</v>
+      </c>
+      <c r="B172" s="44" t="s">
+        <v>343</v>
+      </c>
+      <c r="H172" s="46" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" ht="106">
+      <c r="A173" s="53" t="s">
+        <v>353</v>
+      </c>
+      <c r="B173" s="44" t="s">
+        <v>344</v>
+      </c>
+      <c r="H173" s="46" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" ht="18">
+      <c r="A174" s="53" t="s">
+        <v>354</v>
+      </c>
+      <c r="B174" s="44" t="s">
+        <v>345</v>
+      </c>
+      <c r="H174" s="49" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" ht="409.6">
+      <c r="A175" s="53" t="s">
+        <v>355</v>
+      </c>
+      <c r="B175" s="44" t="s">
+        <v>346</v>
+      </c>
+      <c r="H175" s="46" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" ht="409.6">
+      <c r="A176" s="53" t="s">
+        <v>356</v>
+      </c>
+      <c r="B176" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="H176" s="46" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" ht="409.6">
+      <c r="A177" s="54" t="s">
+        <v>362</v>
+      </c>
+      <c r="B177" s="44" t="s">
+        <v>357</v>
+      </c>
+      <c r="H177" s="46" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" ht="76">
+      <c r="A178" s="54" t="s">
+        <v>363</v>
+      </c>
+      <c r="B178" s="46" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" ht="151">
+      <c r="A179" s="54" t="s">
+        <v>364</v>
+      </c>
+      <c r="B179" s="46" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" ht="121">
+      <c r="A180" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="B180" s="46" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" ht="16">
+      <c r="A181" s="54" t="s">
+        <v>366</v>
+      </c>
+      <c r="B181" s="46" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" ht="31">
+      <c r="A182" s="54" t="s">
+        <v>386</v>
+      </c>
+      <c r="B182" s="46" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" ht="241">
+      <c r="A183" s="54" t="s">
+        <v>387</v>
+      </c>
+      <c r="B183" s="46" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" ht="151">
+      <c r="A184" s="54" t="s">
+        <v>388</v>
+      </c>
+      <c r="B184" s="46" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" ht="16">
+      <c r="A185" s="54" t="s">
+        <v>393</v>
+      </c>
+      <c r="B185" s="46" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" ht="226">
+      <c r="A186" s="54" t="s">
+        <v>391</v>
+      </c>
+      <c r="B186" s="46" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" ht="91">
+      <c r="A187" s="54" t="s">
+        <v>392</v>
+      </c>
+      <c r="B187" s="46" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A188" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="B188" s="46" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A189" s="40" t="s">
+        <v>401</v>
+      </c>
+      <c r="B189" s="46" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A190" s="40" t="s">
+        <v>402</v>
+      </c>
+      <c r="B190" s="46" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A191" s="40" t="s">
+        <v>403</v>
+      </c>
+      <c r="B191" s="46" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A192" s="40" t="s">
+        <v>404</v>
+      </c>
+      <c r="B192" s="46" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A193" s="40" t="s">
+        <v>406</v>
+      </c>
+      <c r="B193" s="46" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A194" s="40" t="s">
+        <v>413</v>
+      </c>
+      <c r="B194" s="46" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A195" s="40" t="s">
+        <v>414</v>
+      </c>
+      <c r="B195" s="46" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A196" s="40" t="s">
+        <v>415</v>
+      </c>
+      <c r="B196" s="46" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A197" s="40" t="s">
+        <v>416</v>
+      </c>
+      <c r="B197" s="46" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A198" s="40" t="s">
+        <v>417</v>
+      </c>
+      <c r="B198" s="46" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A199" s="40" t="s">
+        <v>418</v>
+      </c>
+      <c r="B199" s="46" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="15.75" customHeight="1">
       <c r="A200" s="40"/>
     </row>
-    <row r="201" spans="1:1" ht="15.75" customHeight="1">
+    <row r="201" spans="1:2" ht="15.75" customHeight="1">
       <c r="A201" s="40"/>
     </row>
-    <row r="202" spans="1:1" ht="15.75" customHeight="1">
+    <row r="202" spans="1:2" ht="15.75" customHeight="1">
       <c r="A202" s="40"/>
     </row>
-    <row r="203" spans="1:1" ht="15.75" customHeight="1">
+    <row r="203" spans="1:2" ht="15.75" customHeight="1">
       <c r="A203" s="40"/>
     </row>
-    <row r="204" spans="1:1" ht="15.75" customHeight="1">
+    <row r="204" spans="1:2" ht="15.75" customHeight="1">
       <c r="A204" s="40"/>
     </row>
-    <row r="205" spans="1:1" ht="15.75" customHeight="1">
+    <row r="205" spans="1:2" ht="15.75" customHeight="1">
       <c r="A205" s="40"/>
     </row>
-    <row r="206" spans="1:1" ht="15.75" customHeight="1">
+    <row r="206" spans="1:2" ht="15.75" customHeight="1">
       <c r="A206" s="40"/>
     </row>
-    <row r="207" spans="1:1" ht="15.75" customHeight="1">
+    <row r="207" spans="1:2" ht="15.75" customHeight="1">
       <c r="A207" s="40"/>
     </row>
-    <row r="208" spans="1:1" ht="15.75" customHeight="1">
+    <row r="208" spans="1:2" ht="15.75" customHeight="1">
       <c r="A208" s="40"/>
     </row>
     <row r="209" spans="1:1" ht="15.75" customHeight="1">
@@ -5417,9 +6191,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="41.375" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" customWidth="1"/>
     <col min="2" max="2" width="48" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
fix content website, add webinar
</commit_message>
<xml_diff>
--- a/translation.xlsx
+++ b/translation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dunguyenchiem/Project/ActiveAgeing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2542C6-3FB6-F74A-9F49-789818CB3AF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DAF79A-ADCC-3E4F-B8B0-5359EC6D7A47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="421">
   <si>
     <t>English</t>
   </si>
@@ -1340,6 +1340,12 @@
   </si>
   <si>
     <t>Besides, we would love to receive your opinions to enhance our solution further and look forward to receiving your continuous support.</t>
+  </si>
+  <si>
+    <t>Tin tức</t>
+  </si>
+  <si>
+    <t>News</t>
   </si>
 </sst>
 </file>
@@ -1671,10 +1677,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1894,7 +1900,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C200" sqref="C200"/>
+      <selection pane="bottomLeft" activeCell="A201" sqref="A201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -1916,21 +1922,21 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:16" ht="16">
       <c r="A2" s="4" t="s">
@@ -3348,7 +3354,7 @@
       </c>
     </row>
     <row r="155" spans="1:2" ht="16">
-      <c r="A155" s="53" t="s">
+      <c r="A155" s="51" t="s">
         <v>315</v>
       </c>
       <c r="B155" s="48" t="s">
@@ -3356,7 +3362,7 @@
       </c>
     </row>
     <row r="156" spans="1:2" ht="16">
-      <c r="A156" s="53" t="s">
+      <c r="A156" s="51" t="s">
         <v>316</v>
       </c>
       <c r="B156" s="44" t="s">
@@ -3364,7 +3370,7 @@
       </c>
     </row>
     <row r="157" spans="1:2" ht="16">
-      <c r="A157" s="53" t="s">
+      <c r="A157" s="51" t="s">
         <v>317</v>
       </c>
       <c r="B157" s="44" t="s">
@@ -3372,7 +3378,7 @@
       </c>
     </row>
     <row r="158" spans="1:2" ht="16">
-      <c r="A158" s="53" t="s">
+      <c r="A158" s="51" t="s">
         <v>318</v>
       </c>
       <c r="B158" s="44" t="s">
@@ -3380,7 +3386,7 @@
       </c>
     </row>
     <row r="159" spans="1:2" ht="16">
-      <c r="A159" s="53" t="s">
+      <c r="A159" s="51" t="s">
         <v>326</v>
       </c>
       <c r="B159" s="44" t="s">
@@ -3388,7 +3394,7 @@
       </c>
     </row>
     <row r="160" spans="1:2" ht="16">
-      <c r="A160" s="53" t="s">
+      <c r="A160" s="51" t="s">
         <v>327</v>
       </c>
       <c r="B160" s="44" t="s">
@@ -3396,7 +3402,7 @@
       </c>
     </row>
     <row r="161" spans="1:8" ht="16">
-      <c r="A161" s="53" t="s">
+      <c r="A161" s="51" t="s">
         <v>328</v>
       </c>
       <c r="B161" s="44" t="s">
@@ -3404,7 +3410,7 @@
       </c>
     </row>
     <row r="162" spans="1:8" ht="166">
-      <c r="A162" s="53" t="s">
+      <c r="A162" s="51" t="s">
         <v>329</v>
       </c>
       <c r="B162" s="44" t="s">
@@ -3415,7 +3421,7 @@
       </c>
     </row>
     <row r="163" spans="1:8" ht="91">
-      <c r="A163" s="53" t="s">
+      <c r="A163" s="51" t="s">
         <v>330</v>
       </c>
       <c r="B163" s="44" t="s">
@@ -3426,7 +3432,7 @@
       </c>
     </row>
     <row r="164" spans="1:8" ht="409.6">
-      <c r="A164" s="53" t="s">
+      <c r="A164" s="51" t="s">
         <v>338</v>
       </c>
       <c r="B164" s="44" t="s">
@@ -3437,7 +3443,7 @@
       </c>
     </row>
     <row r="165" spans="1:8" ht="16">
-      <c r="A165" s="53" t="s">
+      <c r="A165" s="51" t="s">
         <v>331</v>
       </c>
       <c r="B165" s="44" t="s">
@@ -3448,7 +3454,7 @@
       </c>
     </row>
     <row r="166" spans="1:8" ht="121">
-      <c r="A166" s="53" t="s">
+      <c r="A166" s="51" t="s">
         <v>332</v>
       </c>
       <c r="B166" s="44" t="s">
@@ -3459,7 +3465,7 @@
       </c>
     </row>
     <row r="167" spans="1:8" ht="409.6">
-      <c r="A167" s="53" t="s">
+      <c r="A167" s="51" t="s">
         <v>333</v>
       </c>
       <c r="B167" s="44" t="s">
@@ -3470,7 +3476,7 @@
       </c>
     </row>
     <row r="168" spans="1:8" ht="409.6">
-      <c r="A168" s="53" t="s">
+      <c r="A168" s="51" t="s">
         <v>348</v>
       </c>
       <c r="B168" s="44" t="s">
@@ -3481,7 +3487,7 @@
       </c>
     </row>
     <row r="169" spans="1:8" ht="409.6">
-      <c r="A169" s="53" t="s">
+      <c r="A169" s="51" t="s">
         <v>349</v>
       </c>
       <c r="B169" s="44" t="s">
@@ -3492,7 +3498,7 @@
       </c>
     </row>
     <row r="170" spans="1:8" ht="106">
-      <c r="A170" s="53" t="s">
+      <c r="A170" s="51" t="s">
         <v>350</v>
       </c>
       <c r="B170" s="44" t="s">
@@ -3503,7 +3509,7 @@
       </c>
     </row>
     <row r="171" spans="1:8" ht="409.6">
-      <c r="A171" s="53" t="s">
+      <c r="A171" s="51" t="s">
         <v>351</v>
       </c>
       <c r="B171" s="44" t="s">
@@ -3514,7 +3520,7 @@
       </c>
     </row>
     <row r="172" spans="1:8" ht="409.6">
-      <c r="A172" s="53" t="s">
+      <c r="A172" s="51" t="s">
         <v>352</v>
       </c>
       <c r="B172" s="44" t="s">
@@ -3525,7 +3531,7 @@
       </c>
     </row>
     <row r="173" spans="1:8" ht="106">
-      <c r="A173" s="53" t="s">
+      <c r="A173" s="51" t="s">
         <v>353</v>
       </c>
       <c r="B173" s="44" t="s">
@@ -3536,7 +3542,7 @@
       </c>
     </row>
     <row r="174" spans="1:8" ht="18">
-      <c r="A174" s="53" t="s">
+      <c r="A174" s="51" t="s">
         <v>354</v>
       </c>
       <c r="B174" s="44" t="s">
@@ -3547,7 +3553,7 @@
       </c>
     </row>
     <row r="175" spans="1:8" ht="409.6">
-      <c r="A175" s="53" t="s">
+      <c r="A175" s="51" t="s">
         <v>355</v>
       </c>
       <c r="B175" s="44" t="s">
@@ -3558,7 +3564,7 @@
       </c>
     </row>
     <row r="176" spans="1:8" ht="409.6">
-      <c r="A176" s="53" t="s">
+      <c r="A176" s="51" t="s">
         <v>356</v>
       </c>
       <c r="B176" s="44" t="s">
@@ -3569,7 +3575,7 @@
       </c>
     </row>
     <row r="177" spans="1:8" ht="409.6">
-      <c r="A177" s="54" t="s">
+      <c r="A177" s="52" t="s">
         <v>362</v>
       </c>
       <c r="B177" s="44" t="s">
@@ -3580,7 +3586,7 @@
       </c>
     </row>
     <row r="178" spans="1:8" ht="76">
-      <c r="A178" s="54" t="s">
+      <c r="A178" s="52" t="s">
         <v>363</v>
       </c>
       <c r="B178" s="46" t="s">
@@ -3588,7 +3594,7 @@
       </c>
     </row>
     <row r="179" spans="1:8" ht="151">
-      <c r="A179" s="54" t="s">
+      <c r="A179" s="52" t="s">
         <v>364</v>
       </c>
       <c r="B179" s="46" t="s">
@@ -3596,7 +3602,7 @@
       </c>
     </row>
     <row r="180" spans="1:8" ht="121">
-      <c r="A180" s="54" t="s">
+      <c r="A180" s="52" t="s">
         <v>365</v>
       </c>
       <c r="B180" s="46" t="s">
@@ -3604,7 +3610,7 @@
       </c>
     </row>
     <row r="181" spans="1:8" ht="16">
-      <c r="A181" s="54" t="s">
+      <c r="A181" s="52" t="s">
         <v>366</v>
       </c>
       <c r="B181" s="46" t="s">
@@ -3612,7 +3618,7 @@
       </c>
     </row>
     <row r="182" spans="1:8" ht="31">
-      <c r="A182" s="54" t="s">
+      <c r="A182" s="52" t="s">
         <v>386</v>
       </c>
       <c r="B182" s="46" t="s">
@@ -3620,7 +3626,7 @@
       </c>
     </row>
     <row r="183" spans="1:8" ht="241">
-      <c r="A183" s="54" t="s">
+      <c r="A183" s="52" t="s">
         <v>387</v>
       </c>
       <c r="B183" s="46" t="s">
@@ -3628,7 +3634,7 @@
       </c>
     </row>
     <row r="184" spans="1:8" ht="151">
-      <c r="A184" s="54" t="s">
+      <c r="A184" s="52" t="s">
         <v>388</v>
       </c>
       <c r="B184" s="46" t="s">
@@ -3636,7 +3642,7 @@
       </c>
     </row>
     <row r="185" spans="1:8" ht="16">
-      <c r="A185" s="54" t="s">
+      <c r="A185" s="52" t="s">
         <v>393</v>
       </c>
       <c r="B185" s="46" t="s">
@@ -3644,7 +3650,7 @@
       </c>
     </row>
     <row r="186" spans="1:8" ht="226">
-      <c r="A186" s="54" t="s">
+      <c r="A186" s="52" t="s">
         <v>391</v>
       </c>
       <c r="B186" s="46" t="s">
@@ -3652,7 +3658,7 @@
       </c>
     </row>
     <row r="187" spans="1:8" ht="91">
-      <c r="A187" s="54" t="s">
+      <c r="A187" s="52" t="s">
         <v>392</v>
       </c>
       <c r="B187" s="46" t="s">
@@ -3756,7 +3762,12 @@
       </c>
     </row>
     <row r="200" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A200" s="40"/>
+      <c r="A200" s="40" t="s">
+        <v>420</v>
+      </c>
+      <c r="B200" s="46" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="201" spans="1:2" ht="15.75" customHeight="1">
       <c r="A201" s="40"/>

</xml_diff>